<commit_message>
Finished process pH and alkalinity data from processing day on 11/17/2020. Data all looked good and fell under the threshold of a coefficient of variation of 1%.
I renamed the processed file to match the data of actual lab processing even though the R files have today's date....
</commit_message>
<xml_diff>
--- a/check sample work/TA QAQC/20201110 results summary both probes.xlsx
+++ b/check sample work/TA QAQC/20201110 results summary both probes.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\915712257\Documents\R\rye-tech-sfsu\2020-season-summary\check sample work\TA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\915712257\Documents\R\rye-tech-sfsu\2021-season-summary\check sample work\TA QAQC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="example to follow" sheetId="1" r:id="rId1"/>
-    <sheet name="data 11dec2019 to 20feb2020" sheetId="2" r:id="rId2"/>
+    <sheet name="data 11dec2019 to 17nov2020" sheetId="2" r:id="rId2"/>
     <sheet name="QAQC crm &amp; baystd assessment" sheetId="3" r:id="rId3"/>
     <sheet name="QAQC crms assessment" sheetId="4" r:id="rId4"/>
     <sheet name="QAQC baystds assessment" sheetId="5" r:id="rId5"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="230">
   <si>
     <t>sample</t>
   </si>
@@ -687,6 +687,45 @@
   </si>
   <si>
     <t>probe C started on 11/10/2020</t>
+  </si>
+  <si>
+    <t>P-0023-1</t>
+  </si>
+  <si>
+    <t>P-0023-2</t>
+  </si>
+  <si>
+    <t>P-0023-3</t>
+  </si>
+  <si>
+    <t>B-0041-1</t>
+  </si>
+  <si>
+    <t>B-0041-2</t>
+  </si>
+  <si>
+    <t>B-0041-3</t>
+  </si>
+  <si>
+    <t>P-0034-1</t>
+  </si>
+  <si>
+    <t>P-0034-2</t>
+  </si>
+  <si>
+    <t>P-0034-3</t>
+  </si>
+  <si>
+    <t>BAYSTD1-11172020-1</t>
+  </si>
+  <si>
+    <t>BAYSTD1-11172020-2</t>
+  </si>
+  <si>
+    <t>BAYSTD1-11172020-3</t>
+  </si>
+  <si>
+    <t>baystd1</t>
   </si>
 </sst>
 </file>
@@ -779,7 +818,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -849,6 +888,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2009,11 +2051,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M175"/>
+  <dimension ref="A1:M189"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D170" sqref="D170"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A193" sqref="A193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2025,7 +2067,7 @@
     <col min="5" max="5" width="10" style="19" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.140625" style="19"/>
     <col min="8" max="8" width="13" style="19" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="19"/>
+    <col min="9" max="9" width="9.140625" style="41"/>
     <col min="10" max="10" width="11.42578125" style="19" customWidth="1"/>
     <col min="11" max="12" width="9.140625" style="19"/>
     <col min="13" max="13" width="51.140625" customWidth="1"/>
@@ -2056,7 +2098,7 @@
       <c r="H1" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="41" t="s">
         <v>24</v>
       </c>
       <c r="J1" s="19" t="s">
@@ -2086,7 +2128,7 @@
       <c r="F2" s="21"/>
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
+      <c r="I2" s="42"/>
       <c r="J2" s="21"/>
       <c r="K2" s="21"/>
       <c r="L2" s="21"/>
@@ -2106,7 +2148,7 @@
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
+      <c r="I3" s="42"/>
       <c r="J3" s="21"/>
       <c r="K3" s="21"/>
       <c r="L3" s="21"/>
@@ -2171,7 +2213,7 @@
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
+      <c r="I5" s="42"/>
       <c r="J5" s="21"/>
       <c r="K5" s="21"/>
       <c r="L5" s="21"/>
@@ -2191,7 +2233,7 @@
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
+      <c r="I6" s="42"/>
       <c r="J6" s="21"/>
       <c r="K6" s="21"/>
       <c r="L6" s="21"/>
@@ -2256,7 +2298,7 @@
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
+      <c r="I8" s="42"/>
       <c r="J8" s="21"/>
       <c r="K8" s="21"/>
       <c r="L8" s="21"/>
@@ -2276,7 +2318,7 @@
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
+      <c r="I9" s="42"/>
       <c r="J9" s="21"/>
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
@@ -2341,7 +2383,7 @@
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
+      <c r="I11" s="42"/>
       <c r="J11" s="21"/>
       <c r="K11" s="21"/>
       <c r="L11" s="21"/>
@@ -2361,7 +2403,7 @@
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
+      <c r="I12" s="42"/>
       <c r="J12" s="21"/>
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
@@ -2426,7 +2468,7 @@
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
+      <c r="I14" s="42"/>
       <c r="J14" s="21"/>
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
@@ -2446,7 +2488,7 @@
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
+      <c r="I15" s="42"/>
       <c r="J15" s="21"/>
       <c r="K15" s="21"/>
       <c r="L15" s="21"/>
@@ -2729,7 +2771,7 @@
         <f>F26/E26</f>
         <v>1.5485231750558507E-3</v>
       </c>
-      <c r="I26" s="19">
+      <c r="I26" s="41">
         <f>H26</f>
         <v>1.5485231750558507E-3</v>
       </c>
@@ -2759,7 +2801,7 @@
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
+      <c r="I27" s="42"/>
       <c r="J27" s="21"/>
       <c r="K27" s="21"/>
       <c r="L27" s="21"/>
@@ -2777,7 +2819,7 @@
       <c r="F28" s="21"/>
       <c r="G28" s="21"/>
       <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
+      <c r="I28" s="42"/>
       <c r="J28" s="21"/>
       <c r="K28" s="21"/>
       <c r="L28" s="21"/>
@@ -2807,7 +2849,7 @@
         <f>F29/E29</f>
         <v>6.0310727707206184E-2</v>
       </c>
-      <c r="I29" s="21">
+      <c r="I29" s="42">
         <f>H29</f>
         <v>6.0310727707206184E-2</v>
       </c>
@@ -2837,7 +2879,7 @@
       <c r="F30" s="21"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
+      <c r="I30" s="42"/>
       <c r="J30" s="21"/>
       <c r="K30" s="21"/>
       <c r="L30" s="21"/>
@@ -2855,7 +2897,7 @@
       <c r="F31" s="21"/>
       <c r="G31" s="21"/>
       <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
+      <c r="I31" s="42"/>
       <c r="J31" s="21"/>
       <c r="K31" s="21"/>
       <c r="L31" s="21"/>
@@ -2885,7 +2927,7 @@
         <f>F32/E32</f>
         <v>1.9134112591256396E-3</v>
       </c>
-      <c r="I32" s="21">
+      <c r="I32" s="42">
         <f>H32</f>
         <v>1.9134112591256396E-3</v>
       </c>
@@ -2915,7 +2957,7 @@
       <c r="F33" s="21"/>
       <c r="G33" s="21"/>
       <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
+      <c r="I33" s="42"/>
       <c r="J33" s="21"/>
       <c r="K33" s="21"/>
       <c r="L33" s="21"/>
@@ -2933,7 +2975,7 @@
       <c r="F34" s="21"/>
       <c r="G34" s="21"/>
       <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
+      <c r="I34" s="42"/>
       <c r="J34" s="21"/>
       <c r="K34" s="21"/>
       <c r="L34" s="21"/>
@@ -2963,7 +3005,7 @@
         <f>F35/E35</f>
         <v>2.3260389703177856E-3</v>
       </c>
-      <c r="I35" s="21">
+      <c r="I35" s="42">
         <f>H35</f>
         <v>2.3260389703177856E-3</v>
       </c>
@@ -2993,7 +3035,7 @@
       <c r="F36" s="21"/>
       <c r="G36" s="21"/>
       <c r="H36" s="21"/>
-      <c r="I36" s="21"/>
+      <c r="I36" s="42"/>
       <c r="J36" s="21"/>
       <c r="K36" s="21"/>
       <c r="L36" s="21"/>
@@ -3023,7 +3065,7 @@
         <f>F37/E37</f>
         <v>2.8169383823426438E-3</v>
       </c>
-      <c r="I37" s="21">
+      <c r="I37" s="42">
         <f>H37</f>
         <v>2.8169383823426438E-3</v>
       </c>
@@ -3079,7 +3121,7 @@
         <f>F40/E40</f>
         <v>4.5570746283256349E-5</v>
       </c>
-      <c r="I40" s="19">
+      <c r="I40" s="41">
         <f>H40</f>
         <v>4.5570746283256349E-5</v>
       </c>
@@ -3135,7 +3177,7 @@
         <f>F43/E43</f>
         <v>3.9516327434572507E-3</v>
       </c>
-      <c r="I43" s="19">
+      <c r="I43" s="41">
         <f>H43</f>
         <v>3.9516327434572507E-3</v>
       </c>
@@ -3191,7 +3233,7 @@
         <f>F46/E46</f>
         <v>3.2129373662930657E-3</v>
       </c>
-      <c r="I46" s="19">
+      <c r="I46" s="41">
         <f>H46</f>
         <v>3.2129373662930657E-3</v>
       </c>
@@ -3239,7 +3281,7 @@
         <f>F48/E48</f>
         <v>2.9240516858113411E-4</v>
       </c>
-      <c r="I48" s="19">
+      <c r="I48" s="41">
         <f>H48</f>
         <v>2.9240516858113411E-4</v>
       </c>
@@ -3269,7 +3311,7 @@
       <c r="F49" s="21"/>
       <c r="G49" s="21"/>
       <c r="H49" s="21"/>
-      <c r="I49" s="21"/>
+      <c r="I49" s="42"/>
       <c r="J49" s="21"/>
       <c r="K49" s="21"/>
       <c r="L49" s="21"/>
@@ -3287,7 +3329,7 @@
       <c r="F50" s="21"/>
       <c r="G50" s="21"/>
       <c r="H50" s="21"/>
-      <c r="I50" s="21"/>
+      <c r="I50" s="42"/>
       <c r="J50" s="21"/>
       <c r="K50" s="21"/>
       <c r="L50" s="21"/>
@@ -3317,7 +3359,7 @@
         <f>F51/E51</f>
         <v>1.9654864659024053E-4</v>
       </c>
-      <c r="I51" s="21">
+      <c r="I51" s="42">
         <f>H51</f>
         <v>1.9654864659024053E-4</v>
       </c>
@@ -3347,7 +3389,7 @@
       <c r="F52" s="21"/>
       <c r="G52" s="21"/>
       <c r="H52" s="21"/>
-      <c r="I52" s="21"/>
+      <c r="I52" s="42"/>
       <c r="J52" s="21"/>
       <c r="K52" s="21"/>
       <c r="L52" s="21"/>
@@ -3365,7 +3407,7 @@
       <c r="F53" s="21"/>
       <c r="G53" s="21"/>
       <c r="H53" s="21"/>
-      <c r="I53" s="21"/>
+      <c r="I53" s="42"/>
       <c r="J53" s="21"/>
       <c r="K53" s="21"/>
       <c r="L53" s="21"/>
@@ -3395,7 +3437,7 @@
         <f>F54/E54</f>
         <v>9.2813475730791674E-4</v>
       </c>
-      <c r="I54" s="21">
+      <c r="I54" s="42">
         <f>H54</f>
         <v>9.2813475730791674E-4</v>
       </c>
@@ -3425,7 +3467,7 @@
       <c r="F55" s="21"/>
       <c r="G55" s="21"/>
       <c r="H55" s="21"/>
-      <c r="I55" s="21"/>
+      <c r="I55" s="42"/>
       <c r="J55" s="21"/>
       <c r="K55" s="21"/>
       <c r="L55" s="21"/>
@@ -3443,7 +3485,7 @@
       <c r="F56" s="21"/>
       <c r="G56" s="21"/>
       <c r="H56" s="21"/>
-      <c r="I56" s="21"/>
+      <c r="I56" s="42"/>
       <c r="J56" s="21"/>
       <c r="K56" s="21"/>
       <c r="L56" s="21"/>
@@ -3473,7 +3515,7 @@
         <f>F57/E57</f>
         <v>1.0739199325851458E-3</v>
       </c>
-      <c r="I57" s="21">
+      <c r="I57" s="42">
         <f>H57</f>
         <v>1.0739199325851458E-3</v>
       </c>
@@ -3503,7 +3545,7 @@
       <c r="F58" s="21"/>
       <c r="G58" s="21"/>
       <c r="H58" s="21"/>
-      <c r="I58" s="21"/>
+      <c r="I58" s="42"/>
       <c r="J58" s="21"/>
       <c r="K58" s="21"/>
       <c r="L58" s="21"/>
@@ -3521,7 +3563,7 @@
       <c r="F59" s="21"/>
       <c r="G59" s="21"/>
       <c r="H59" s="21"/>
-      <c r="I59" s="21"/>
+      <c r="I59" s="42"/>
       <c r="J59" s="21"/>
       <c r="K59" s="21"/>
       <c r="L59" s="21"/>
@@ -3551,7 +3593,7 @@
         <f>F60/E60</f>
         <v>1.0713401027559516E-4</v>
       </c>
-      <c r="I60" s="21">
+      <c r="I60" s="42">
         <f>H60</f>
         <v>1.0713401027559516E-4</v>
       </c>
@@ -3581,7 +3623,7 @@
       <c r="F61" s="21"/>
       <c r="G61" s="21"/>
       <c r="H61" s="21"/>
-      <c r="I61" s="21"/>
+      <c r="I61" s="42"/>
       <c r="J61" s="21"/>
       <c r="K61" s="21"/>
       <c r="L61" s="21"/>
@@ -3611,7 +3653,7 @@
         <f>F62/E62</f>
         <v>2.7913508749383576E-4</v>
       </c>
-      <c r="I62" s="21">
+      <c r="I62" s="42">
         <f>H62</f>
         <v>2.7913508749383576E-4</v>
       </c>
@@ -3667,7 +3709,7 @@
         <f>F65/E65</f>
         <v>7.8553545343008153E-4</v>
       </c>
-      <c r="I65" s="19">
+      <c r="I65" s="41">
         <f>H65</f>
         <v>7.8553545343008153E-4</v>
       </c>
@@ -3723,7 +3765,7 @@
         <f>F68/E68</f>
         <v>2.4239239552542855E-3</v>
       </c>
-      <c r="I68" s="19">
+      <c r="I68" s="41">
         <f>H68</f>
         <v>2.4239239552542855E-3</v>
       </c>
@@ -3779,7 +3821,7 @@
         <f>F71/E71</f>
         <v>1.208312187927063E-3</v>
       </c>
-      <c r="I71" s="19">
+      <c r="I71" s="41">
         <f>H71</f>
         <v>1.208312187927063E-3</v>
       </c>
@@ -3835,7 +3877,7 @@
         <f>F74/E74</f>
         <v>3.2071220365040595E-3</v>
       </c>
-      <c r="I74" s="19">
+      <c r="I74" s="41">
         <f>H74</f>
         <v>3.2071220365040595E-3</v>
       </c>
@@ -3883,7 +3925,7 @@
         <f>F76/E76</f>
         <v>8.016290911164102E-4</v>
       </c>
-      <c r="I76" s="19">
+      <c r="I76" s="41">
         <f>H76</f>
         <v>8.016290911164102E-4</v>
       </c>
@@ -3913,7 +3955,7 @@
       <c r="F77" s="21"/>
       <c r="G77" s="21"/>
       <c r="H77" s="21"/>
-      <c r="I77" s="21"/>
+      <c r="I77" s="42"/>
       <c r="J77" s="21"/>
       <c r="K77" s="21"/>
       <c r="L77" s="21"/>
@@ -3931,7 +3973,7 @@
       <c r="F78" s="21"/>
       <c r="G78" s="21"/>
       <c r="H78" s="21"/>
-      <c r="I78" s="21"/>
+      <c r="I78" s="42"/>
       <c r="J78" s="21"/>
       <c r="K78" s="21"/>
       <c r="L78" s="21"/>
@@ -3961,7 +4003,7 @@
         <f>F79/E79</f>
         <v>6.481955817528709E-3</v>
       </c>
-      <c r="I79" s="21">
+      <c r="I79" s="42">
         <f>H79</f>
         <v>6.481955817528709E-3</v>
       </c>
@@ -3993,7 +4035,7 @@
       <c r="F80" s="34"/>
       <c r="G80" s="34"/>
       <c r="H80" s="34"/>
-      <c r="I80" s="34"/>
+      <c r="I80" s="43"/>
       <c r="J80" s="34"/>
       <c r="K80" s="34"/>
       <c r="L80" s="34"/>
@@ -4013,7 +4055,7 @@
       <c r="F81" s="34"/>
       <c r="G81" s="34"/>
       <c r="H81" s="34"/>
-      <c r="I81" s="34"/>
+      <c r="I81" s="43"/>
       <c r="J81" s="34"/>
       <c r="K81" s="34"/>
       <c r="L81" s="34"/>
@@ -4045,7 +4087,7 @@
         <f>F82/E82</f>
         <v>2.5099988987789643E-3</v>
       </c>
-      <c r="I82" s="34">
+      <c r="I82" s="43">
         <f>H82</f>
         <v>2.5099988987789643E-3</v>
       </c>
@@ -4075,7 +4117,7 @@
       <c r="F83" s="21"/>
       <c r="G83" s="21"/>
       <c r="H83" s="21"/>
-      <c r="I83" s="21"/>
+      <c r="I83" s="42"/>
       <c r="J83" s="21"/>
       <c r="K83" s="21"/>
       <c r="L83" s="21"/>
@@ -4105,7 +4147,7 @@
         <f>F84/E84</f>
         <v>9.9861125297410667E-4</v>
       </c>
-      <c r="I84" s="21">
+      <c r="I84" s="42">
         <f>H84</f>
         <v>9.9861125297410667E-4</v>
       </c>
@@ -4163,7 +4205,7 @@
         <f>F87/E87</f>
         <v>6.9033861326643589E-2</v>
       </c>
-      <c r="I87" s="19">
+      <c r="I87" s="41">
         <f>H87</f>
         <v>6.9033861326643589E-2</v>
       </c>
@@ -4211,7 +4253,7 @@
         <f>F89/E89</f>
         <v>1.3614826728260334E-3</v>
       </c>
-      <c r="I89" s="19">
+      <c r="I89" s="41">
         <f>H89</f>
         <v>1.3614826728260334E-3</v>
       </c>
@@ -4267,7 +4309,7 @@
         <f>F92/E92</f>
         <v>8.506148501435629E-3</v>
       </c>
-      <c r="I92" s="19">
+      <c r="I92" s="41">
         <f>H92</f>
         <v>8.506148501435629E-3</v>
       </c>
@@ -4323,7 +4365,7 @@
         <f>F95/E95</f>
         <v>7.34988132167842E-3</v>
       </c>
-      <c r="I95" s="19">
+      <c r="I95" s="41">
         <f>H95</f>
         <v>7.34988132167842E-3</v>
       </c>
@@ -4371,7 +4413,7 @@
         <f>F97/E97</f>
         <v>5.5071677323326133E-3</v>
       </c>
-      <c r="I97" s="19">
+      <c r="I97" s="41">
         <f>H97</f>
         <v>5.5071677323326133E-3</v>
       </c>
@@ -4401,7 +4443,7 @@
       <c r="F98" s="21"/>
       <c r="G98" s="21"/>
       <c r="H98" s="21"/>
-      <c r="I98" s="21"/>
+      <c r="I98" s="42"/>
       <c r="J98" s="21"/>
       <c r="K98" s="21"/>
       <c r="L98" s="21"/>
@@ -4419,7 +4461,7 @@
       <c r="F99" s="21"/>
       <c r="G99" s="21"/>
       <c r="H99" s="21"/>
-      <c r="I99" s="21"/>
+      <c r="I99" s="42"/>
       <c r="J99" s="21"/>
       <c r="K99" s="21"/>
       <c r="L99" s="21"/>
@@ -4449,7 +4491,7 @@
         <f>F100/E100</f>
         <v>2.4527851881584973E-3</v>
       </c>
-      <c r="I100" s="21">
+      <c r="I100" s="42">
         <f>H100</f>
         <v>2.4527851881584973E-3</v>
       </c>
@@ -4479,7 +4521,7 @@
       <c r="F101" s="21"/>
       <c r="G101" s="21"/>
       <c r="H101" s="21"/>
-      <c r="I101" s="21"/>
+      <c r="I101" s="42"/>
       <c r="J101" s="21"/>
       <c r="K101" s="21"/>
       <c r="L101" s="21"/>
@@ -4497,7 +4539,7 @@
       <c r="F102" s="21"/>
       <c r="G102" s="21"/>
       <c r="H102" s="21"/>
-      <c r="I102" s="21"/>
+      <c r="I102" s="42"/>
       <c r="J102" s="21"/>
       <c r="K102" s="21"/>
       <c r="L102" s="21"/>
@@ -4515,7 +4557,7 @@
       <c r="F103" s="21"/>
       <c r="G103" s="21"/>
       <c r="H103" s="21"/>
-      <c r="I103" s="21"/>
+      <c r="I103" s="42"/>
       <c r="J103" s="21"/>
       <c r="K103" s="21"/>
       <c r="L103" s="21"/>
@@ -4545,7 +4587,7 @@
         <f>F104/E104</f>
         <v>1.6918464026616708E-3</v>
       </c>
-      <c r="I104" s="21">
+      <c r="I104" s="42">
         <f>H104</f>
         <v>1.6918464026616708E-3</v>
       </c>
@@ -4575,7 +4617,7 @@
       <c r="F105" s="21"/>
       <c r="G105" s="21"/>
       <c r="H105" s="21"/>
-      <c r="I105" s="21"/>
+      <c r="I105" s="42"/>
       <c r="J105" s="21"/>
       <c r="K105" s="21"/>
       <c r="L105" s="21"/>
@@ -4593,7 +4635,7 @@
       <c r="F106" s="21"/>
       <c r="G106" s="21"/>
       <c r="H106" s="21"/>
-      <c r="I106" s="21"/>
+      <c r="I106" s="42"/>
       <c r="J106" s="21"/>
       <c r="K106" s="21"/>
       <c r="L106" s="21"/>
@@ -4623,7 +4665,7 @@
         <f>F107/E107</f>
         <v>2.9638016489000074E-3</v>
       </c>
-      <c r="I107" s="21">
+      <c r="I107" s="42">
         <f>H107</f>
         <v>2.9638016489000074E-3</v>
       </c>
@@ -4653,7 +4695,7 @@
       <c r="F108" s="21"/>
       <c r="G108" s="21"/>
       <c r="H108" s="21"/>
-      <c r="I108" s="21"/>
+      <c r="I108" s="42"/>
       <c r="J108" s="21"/>
       <c r="K108" s="21"/>
       <c r="L108" s="21"/>
@@ -4683,7 +4725,7 @@
         <f>F109/E109</f>
         <v>3.2835259320596714E-2</v>
       </c>
-      <c r="I109" s="21">
+      <c r="I109" s="42">
         <f>H109</f>
         <v>3.2835259320596714E-2</v>
       </c>
@@ -4747,7 +4789,7 @@
         <f>F113/E113</f>
         <v>2.5317167045649223E-3</v>
       </c>
-      <c r="I113" s="19">
+      <c r="I113" s="41">
         <f>H113</f>
         <v>2.5317167045649223E-3</v>
       </c>
@@ -4803,7 +4845,7 @@
         <f>F116/E116</f>
         <v>2.5807081117182116E-3</v>
       </c>
-      <c r="I116" s="19">
+      <c r="I116" s="41">
         <f>H116</f>
         <v>2.5807081117182116E-3</v>
       </c>
@@ -4859,7 +4901,7 @@
         <f>F119/E119</f>
         <v>8.1486630447944828E-3</v>
       </c>
-      <c r="I119" s="19">
+      <c r="I119" s="41">
         <f>H119</f>
         <v>8.1486630447944828E-3</v>
       </c>
@@ -4915,7 +4957,7 @@
         <f>F122/E122</f>
         <v>2.0291745206109254E-3</v>
       </c>
-      <c r="I122" s="19">
+      <c r="I122" s="41">
         <f>H122</f>
         <v>2.0291745206109254E-3</v>
       </c>
@@ -4971,7 +5013,7 @@
         <f>F125/E125</f>
         <v>2.4147568018663191E-3</v>
       </c>
-      <c r="I125" s="19">
+      <c r="I125" s="41">
         <f>H125</f>
         <v>2.4147568018663191E-3</v>
       </c>
@@ -5027,7 +5069,7 @@
         <f>F128/E128</f>
         <v>2.0862706605093095E-3</v>
       </c>
-      <c r="I128" s="19">
+      <c r="I128" s="41">
         <f>H128</f>
         <v>2.0862706605093095E-3</v>
       </c>
@@ -5057,7 +5099,7 @@
       <c r="F129" s="21"/>
       <c r="G129" s="21"/>
       <c r="H129" s="21"/>
-      <c r="I129" s="21"/>
+      <c r="I129" s="42"/>
       <c r="J129" s="21"/>
       <c r="K129" s="21"/>
       <c r="L129" s="21"/>
@@ -5075,7 +5117,7 @@
       <c r="F130" s="21"/>
       <c r="G130" s="21"/>
       <c r="H130" s="21"/>
-      <c r="I130" s="21"/>
+      <c r="I130" s="42"/>
       <c r="J130" s="21"/>
       <c r="K130" s="21"/>
       <c r="L130" s="21"/>
@@ -5093,7 +5135,7 @@
       <c r="F131" s="21"/>
       <c r="G131" s="21"/>
       <c r="H131" s="21"/>
-      <c r="I131" s="21"/>
+      <c r="I131" s="42"/>
       <c r="J131" s="21"/>
       <c r="K131" s="21"/>
       <c r="L131" s="21"/>
@@ -5123,7 +5165,7 @@
         <f>F132/E132</f>
         <v>1.4243648801158428E-3</v>
       </c>
-      <c r="I132" s="21">
+      <c r="I132" s="42">
         <f>H132</f>
         <v>1.4243648801158428E-3</v>
       </c>
@@ -5153,7 +5195,7 @@
       <c r="F133" s="21"/>
       <c r="G133" s="21"/>
       <c r="H133" s="21"/>
-      <c r="I133" s="21"/>
+      <c r="I133" s="42"/>
       <c r="J133" s="21"/>
       <c r="K133" s="21"/>
       <c r="L133" s="21"/>
@@ -5171,7 +5213,7 @@
       <c r="F134" s="21"/>
       <c r="G134" s="21"/>
       <c r="H134" s="21"/>
-      <c r="I134" s="21"/>
+      <c r="I134" s="42"/>
       <c r="J134" s="21"/>
       <c r="K134" s="21"/>
       <c r="L134" s="21"/>
@@ -5201,7 +5243,7 @@
         <f>F135/E135</f>
         <v>8.9374793968448893E-4</v>
       </c>
-      <c r="I135" s="21">
+      <c r="I135" s="42">
         <f>H135</f>
         <v>8.9374793968448893E-4</v>
       </c>
@@ -5231,7 +5273,7 @@
       <c r="F136" s="21"/>
       <c r="G136" s="21"/>
       <c r="H136" s="21"/>
-      <c r="I136" s="21"/>
+      <c r="I136" s="42"/>
       <c r="J136" s="21"/>
       <c r="K136" s="21"/>
       <c r="L136" s="21"/>
@@ -5249,7 +5291,7 @@
       <c r="F137" s="21"/>
       <c r="G137" s="21"/>
       <c r="H137" s="21"/>
-      <c r="I137" s="21"/>
+      <c r="I137" s="42"/>
       <c r="J137" s="21"/>
       <c r="K137" s="21"/>
       <c r="L137" s="21"/>
@@ -5279,7 +5321,7 @@
         <f>F138/E138</f>
         <v>2.2354617350271586E-2</v>
       </c>
-      <c r="I138" s="21">
+      <c r="I138" s="42">
         <f>H138</f>
         <v>2.2354617350271586E-2</v>
       </c>
@@ -5309,7 +5351,7 @@
       <c r="F139" s="21"/>
       <c r="G139" s="21"/>
       <c r="H139" s="21"/>
-      <c r="I139" s="21"/>
+      <c r="I139" s="42"/>
       <c r="J139" s="21"/>
       <c r="K139" s="21"/>
       <c r="L139" s="21"/>
@@ -5327,7 +5369,7 @@
       <c r="F140" s="21"/>
       <c r="G140" s="21"/>
       <c r="H140" s="21"/>
-      <c r="I140" s="21"/>
+      <c r="I140" s="42"/>
       <c r="J140" s="21"/>
       <c r="K140" s="21"/>
       <c r="L140" s="21"/>
@@ -5357,7 +5399,7 @@
         <f>F141/E141</f>
         <v>1.8538282061799391E-3</v>
       </c>
-      <c r="I141" s="21">
+      <c r="I141" s="42">
         <f>H141</f>
         <v>1.8538282061799391E-3</v>
       </c>
@@ -5387,7 +5429,7 @@
       <c r="F142" s="21"/>
       <c r="G142" s="21"/>
       <c r="H142" s="21"/>
-      <c r="I142" s="21"/>
+      <c r="I142" s="42"/>
       <c r="J142" s="21"/>
       <c r="K142" s="21"/>
       <c r="L142" s="21"/>
@@ -5405,7 +5447,7 @@
       <c r="F143" s="21"/>
       <c r="G143" s="21"/>
       <c r="H143" s="21"/>
-      <c r="I143" s="21"/>
+      <c r="I143" s="42"/>
       <c r="J143" s="21"/>
       <c r="K143" s="21"/>
       <c r="L143" s="21"/>
@@ -5435,7 +5477,7 @@
         <f>F144/E144</f>
         <v>1.5039945776039549E-3</v>
       </c>
-      <c r="I144" s="21">
+      <c r="I144" s="42">
         <f>H144</f>
         <v>1.5039945776039549E-3</v>
       </c>
@@ -5499,7 +5541,7 @@
         <f>F148/E148</f>
         <v>7.5764778878594592E-4</v>
       </c>
-      <c r="I148" s="19">
+      <c r="I148" s="41">
         <f>H148</f>
         <v>7.5764778878594592E-4</v>
       </c>
@@ -5555,7 +5597,7 @@
         <f>F151/E151</f>
         <v>4.4314480602057361E-4</v>
       </c>
-      <c r="I151" s="19">
+      <c r="I151" s="41">
         <f>H151</f>
         <v>4.4314480602057361E-4</v>
       </c>
@@ -5611,7 +5653,7 @@
         <f>F154/E154</f>
         <v>8.2210747542610743E-4</v>
       </c>
-      <c r="I154" s="19">
+      <c r="I154" s="41">
         <f>H154</f>
         <v>8.2210747542610743E-4</v>
       </c>
@@ -5667,7 +5709,7 @@
         <f>F157/E157</f>
         <v>1.2920342854077838E-3</v>
       </c>
-      <c r="I157" s="19">
+      <c r="I157" s="41">
         <f>H157</f>
         <v>1.2920342854077838E-3</v>
       </c>
@@ -5723,7 +5765,7 @@
         <f>F160/E160</f>
         <v>1.2484727322683003E-3</v>
       </c>
-      <c r="I160" s="19">
+      <c r="I160" s="41">
         <f>H160</f>
         <v>1.2484727322683003E-3</v>
       </c>
@@ -5779,7 +5821,7 @@
         <f>F163/E163</f>
         <v>6.7287746634621609E-4</v>
       </c>
-      <c r="I163" s="19">
+      <c r="I163" s="41">
         <f>H163</f>
         <v>6.7287746634621609E-4</v>
       </c>
@@ -5875,7 +5917,7 @@
         <f>F171/E171</f>
         <v>2.8545299800126255E-3</v>
       </c>
-      <c r="I171" s="19">
+      <c r="I171" s="41">
         <f>H171</f>
         <v>2.8545299800126255E-3</v>
       </c>
@@ -5939,7 +5981,7 @@
         <f>F175/E175</f>
         <v>1.2109296631623401E-3</v>
       </c>
-      <c r="I175" s="19">
+      <c r="I175" s="41">
         <f>H175</f>
         <v>1.2109296631623401E-3</v>
       </c>
@@ -5954,6 +5996,246 @@
       <c r="L175" s="19">
         <f>K175-J175</f>
         <v>5.3446747965799659</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A176" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="B176" s="19">
+        <v>2053.3155707137898</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A177" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="B177" s="19">
+        <v>2121.1126006919999</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A178" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="B178" s="19">
+        <v>2114.3140912812701</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A179" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="B179" s="19">
+        <v>2131.1655775745298</v>
+      </c>
+      <c r="E179" s="19">
+        <f>AVERAGE(B177:B179)</f>
+        <v>2122.1974231826002</v>
+      </c>
+      <c r="F179" s="19">
+        <f>_xlfn.STDEV.S(B177:B179)</f>
+        <v>8.4779583302859081</v>
+      </c>
+      <c r="G179" s="19">
+        <f>2*F179</f>
+        <v>16.955916660571816</v>
+      </c>
+      <c r="H179" s="19">
+        <f>F179/E179</f>
+        <v>3.9948961570086868E-3</v>
+      </c>
+      <c r="I179" s="41">
+        <f>H179</f>
+        <v>3.9948961570086868E-3</v>
+      </c>
+      <c r="J179" s="19">
+        <f>MIN(B177:B179)</f>
+        <v>2114.3140912812701</v>
+      </c>
+      <c r="K179" s="19">
+        <f>MAX(B177:B179)</f>
+        <v>2131.1655775745298</v>
+      </c>
+      <c r="L179" s="19">
+        <f>K179-J179</f>
+        <v>16.851486293259768</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A180" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="B180" s="19">
+        <v>2136.7025174391802</v>
+      </c>
+    </row>
+    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A181" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B181" s="19">
+        <v>2137.4028738178399</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A182" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="B182" s="19">
+        <v>2137.7465696149202</v>
+      </c>
+      <c r="E182" s="19">
+        <f>AVERAGE(B180:B182)</f>
+        <v>2137.2839869573136</v>
+      </c>
+      <c r="F182" s="19">
+        <f>_xlfn.STDEV.S(B180:B182)</f>
+        <v>0.5320825129820187</v>
+      </c>
+      <c r="G182" s="19">
+        <f>2*F182</f>
+        <v>1.0641650259640374</v>
+      </c>
+      <c r="H182" s="19">
+        <f>F182/E182</f>
+        <v>2.4895265029309632E-4</v>
+      </c>
+      <c r="I182" s="41">
+        <f>H182</f>
+        <v>2.4895265029309632E-4</v>
+      </c>
+      <c r="J182" s="19">
+        <f>MIN(B180:B182)</f>
+        <v>2136.7025174391802</v>
+      </c>
+      <c r="K182" s="19">
+        <f>MAX(B180:B182)</f>
+        <v>2137.7465696149202</v>
+      </c>
+      <c r="L182" s="19">
+        <f>K182-J182</f>
+        <v>1.0440521757400347</v>
+      </c>
+    </row>
+    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A183" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="B183" s="19">
+        <v>2112.5960733162501</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A184" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="B184" s="19">
+        <v>2105.44065001114</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A185" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="B185" s="19">
+        <v>2115.54491941581</v>
+      </c>
+      <c r="E185" s="19">
+        <f>AVERAGE(B183:B185)</f>
+        <v>2111.1938809143999</v>
+      </c>
+      <c r="F185" s="19">
+        <f>_xlfn.STDEV.S(B183:B185)</f>
+        <v>5.1960247015764276</v>
+      </c>
+      <c r="G185" s="19">
+        <f>2*F185</f>
+        <v>10.392049403152855</v>
+      </c>
+      <c r="H185" s="19">
+        <f>F185/E185</f>
+        <v>2.4611783638392921E-3</v>
+      </c>
+      <c r="I185" s="41">
+        <f>H185</f>
+        <v>2.4611783638392921E-3</v>
+      </c>
+      <c r="J185" s="19">
+        <f>MIN(B183:B185)</f>
+        <v>2105.44065001114</v>
+      </c>
+      <c r="K185" s="19">
+        <f>MAX(B183:B185)</f>
+        <v>2115.54491941581</v>
+      </c>
+      <c r="L185" s="19">
+        <f>K185-J185</f>
+        <v>10.104269404670049</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A186" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="B186" s="19">
+        <v>1798.38269926629</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A187" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="B187" s="19">
+        <v>2167.3314732691902</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A188" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="B188" s="19">
+        <v>2162.0931306789098</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A189" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="B189" s="19">
+        <v>2163.2411120153602</v>
+      </c>
+      <c r="E189" s="19">
+        <f>AVERAGE(B187:B189)</f>
+        <v>2164.2219053211534</v>
+      </c>
+      <c r="F189" s="19">
+        <f>_xlfn.STDEV.S(B187:B189)</f>
+        <v>2.7534569008435299</v>
+      </c>
+      <c r="G189" s="19">
+        <f>2*F189</f>
+        <v>5.5069138016870598</v>
+      </c>
+      <c r="H189" s="19">
+        <f>F189/E189</f>
+        <v>1.272261820321488E-3</v>
+      </c>
+      <c r="I189" s="41">
+        <f>H189</f>
+        <v>1.272261820321488E-3</v>
+      </c>
+      <c r="J189" s="19">
+        <f>MIN(B187:B189)</f>
+        <v>2162.0931306789098</v>
+      </c>
+      <c r="K189" s="19">
+        <f>MAX(B187:B189)</f>
+        <v>2167.3314732691902</v>
+      </c>
+      <c r="L189" s="19">
+        <f>K189-J189</f>
+        <v>5.2383425902803538</v>
       </c>
     </row>
   </sheetData>
@@ -5963,11 +6245,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M64"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6062,7 +6344,7 @@
         <v>2238.04</v>
       </c>
       <c r="D3" s="16">
-        <f t="shared" ref="D3:D64" si="0">B3-C3</f>
+        <f t="shared" ref="D3:D66" si="0">B3-C3</f>
         <v>9.4963699999998425</v>
       </c>
       <c r="E3" s="9">
@@ -6070,8 +6352,8 @@
         <v>90.181043176897006</v>
       </c>
       <c r="G3">
-        <f>SQRT(SUM(E2:E46)/ROWS(E2:E46))</f>
-        <v>26.314116840039855</v>
+        <f>SQRT(SUM(E2:E70)/ROWS(E2:E70))</f>
+        <v>25.04641374184385</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -6142,7 +6424,7 @@
       </c>
       <c r="G5">
         <f>SQRT(G3^2+G4^2)</f>
-        <v>26.319453738086381</v>
+        <v>25.052020703480675</v>
       </c>
       <c r="H5" t="s">
         <v>32</v>
@@ -6205,7 +6487,7 @@
         <v>7.0384999999987485E-2</v>
       </c>
       <c r="E7" s="37">
-        <f t="shared" ref="E7:E64" si="1">D7^2</f>
+        <f t="shared" ref="E7:E70" si="1">D7^2</f>
         <v>4.9540482249982379E-3</v>
       </c>
     </row>
@@ -7310,7 +7592,7 @@
         <v>2234.9084845810298</v>
       </c>
       <c r="C62" s="11">
-        <f t="shared" ref="C62:C64" si="9">$L$4</f>
+        <f t="shared" ref="C62:C67" si="9">$L$4</f>
         <v>2212</v>
       </c>
       <c r="D62" s="36">
@@ -7360,6 +7642,126 @@
       <c r="E64" s="37">
         <f t="shared" si="1"/>
         <v>615.17108105747434</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>204</v>
+      </c>
+      <c r="B65" s="11">
+        <v>2220.1114998255798</v>
+      </c>
+      <c r="C65" s="11">
+        <f t="shared" si="9"/>
+        <v>2212</v>
+      </c>
+      <c r="D65" s="36">
+        <f t="shared" si="0"/>
+        <v>8.1114998255798128</v>
+      </c>
+      <c r="E65" s="37">
+        <f t="shared" si="1"/>
+        <v>65.79642942038133</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>205</v>
+      </c>
+      <c r="B66" s="11">
+        <v>2223.29862647973</v>
+      </c>
+      <c r="C66" s="11">
+        <f t="shared" si="9"/>
+        <v>2212</v>
+      </c>
+      <c r="D66" s="36">
+        <f t="shared" si="0"/>
+        <v>11.298626479730046</v>
+      </c>
+      <c r="E66" s="37">
+        <f t="shared" si="1"/>
+        <v>127.65896032845698</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>206</v>
+      </c>
+      <c r="B67" s="11">
+        <v>2217.9539516831501</v>
+      </c>
+      <c r="C67" s="11">
+        <f t="shared" si="9"/>
+        <v>2212</v>
+      </c>
+      <c r="D67" s="36">
+        <f t="shared" ref="D67" si="10">B67-C67</f>
+        <v>5.9539516831500805</v>
+      </c>
+      <c r="E67" s="37">
+        <f t="shared" si="1"/>
+        <v>35.44954064528568</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>226</v>
+      </c>
+      <c r="B68" s="11">
+        <v>2167.3314732691902</v>
+      </c>
+      <c r="C68" s="11">
+        <f t="shared" ref="C68:C70" si="11">$L$5</f>
+        <v>2144.1720766939966</v>
+      </c>
+      <c r="D68" s="36">
+        <f>B68-C68</f>
+        <v>23.159396575193568</v>
+      </c>
+      <c r="E68" s="37">
+        <f t="shared" si="1"/>
+        <v>536.35764972708762</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>227</v>
+      </c>
+      <c r="B69" s="11">
+        <v>2162.0931306789098</v>
+      </c>
+      <c r="C69" s="11">
+        <f t="shared" si="11"/>
+        <v>2144.1720766939966</v>
+      </c>
+      <c r="D69" s="36">
+        <f>B69-C69</f>
+        <v>17.921053984913215</v>
+      </c>
+      <c r="E69" s="37">
+        <f t="shared" si="1"/>
+        <v>321.16417593017383</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>228</v>
+      </c>
+      <c r="B70" s="11">
+        <v>2163.2411120153602</v>
+      </c>
+      <c r="C70" s="11">
+        <f t="shared" si="11"/>
+        <v>2144.1720766939966</v>
+      </c>
+      <c r="D70" s="36">
+        <f>B70-C70</f>
+        <v>19.069035321363572</v>
+      </c>
+      <c r="E70" s="37">
+        <f t="shared" si="1"/>
+        <v>363.62810808741148</v>
       </c>
     </row>
   </sheetData>
@@ -7376,9 +7778,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="G32" sqref="G32:I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8512,8 +8914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8574,17 +8976,17 @@
         <v>2144.1720766939966</v>
       </c>
       <c r="D2" s="36">
-        <f t="shared" ref="D2:D25" si="0">B2-C2</f>
+        <f t="shared" ref="D2:D28" si="0">B2-C2</f>
         <v>14.417764500503381</v>
       </c>
       <c r="E2" s="37">
-        <f t="shared" ref="E2:E25" si="1">D2^2</f>
+        <f t="shared" ref="E2:E28" si="1">D2^2</f>
         <v>207.8719331919755</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2">
-        <f>SQRT(SUM(E2:E13)/ROWS(E2:E13))</f>
-        <v>28.34133544917686</v>
+        <f>SQRT(SUM(E2:E28)/ROWS(E2:E28))</f>
+        <v>26.197093884566602</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -8656,7 +9058,7 @@
       </c>
       <c r="G4">
         <f>SQRT(G2^2+G3^2)</f>
-        <v>28.34629067519715</v>
+        <v>26.202454617779551</v>
       </c>
       <c r="H4" t="s">
         <v>32</v>
@@ -8695,7 +9097,7 @@
       </c>
       <c r="G5">
         <f>G4/L5</f>
-        <v>1.3220156620499897E-2</v>
+        <v>1.2220313333330946E-2</v>
       </c>
       <c r="H5" t="s">
         <v>31</v>
@@ -8741,7 +9143,7 @@
         <v>2192.0776138154802</v>
       </c>
       <c r="C7" s="13">
-        <f t="shared" ref="C7:C25" si="3">$L$5</f>
+        <f t="shared" ref="C7:C28" si="3">$L$5</f>
         <v>2144.1720766939966</v>
       </c>
       <c r="D7" s="17">
@@ -9104,6 +9506,12 @@
         <f t="shared" si="1"/>
         <v>541.38053925422037</v>
       </c>
+      <c r="G24" t="s">
+        <v>229</v>
+      </c>
+      <c r="H24" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -9123,6 +9531,101 @@
       <c r="E25" s="37">
         <f t="shared" si="1"/>
         <v>764.16382344027829</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>226</v>
+      </c>
+      <c r="B26" s="11">
+        <v>2167.3314732691902</v>
+      </c>
+      <c r="C26" s="11">
+        <f t="shared" si="3"/>
+        <v>2144.1720766939966</v>
+      </c>
+      <c r="D26" s="36">
+        <f t="shared" si="0"/>
+        <v>23.159396575193568</v>
+      </c>
+      <c r="E26" s="37">
+        <f t="shared" si="1"/>
+        <v>536.35764972708762</v>
+      </c>
+      <c r="G26">
+        <f>SQRT(SUM(E26:E28)/ROWS(E26:E28))</f>
+        <v>20.175479620442506</v>
+      </c>
+      <c r="H26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>227</v>
+      </c>
+      <c r="B27" s="11">
+        <v>2162.0931306789098</v>
+      </c>
+      <c r="C27" s="11">
+        <f t="shared" si="3"/>
+        <v>2144.1720766939966</v>
+      </c>
+      <c r="D27" s="36">
+        <f t="shared" si="0"/>
+        <v>17.921053984913215</v>
+      </c>
+      <c r="E27" s="37">
+        <f t="shared" si="1"/>
+        <v>321.16417593017383</v>
+      </c>
+      <c r="G27">
+        <v>0.53</v>
+      </c>
+      <c r="H27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>228</v>
+      </c>
+      <c r="B28" s="11">
+        <v>2163.2411120153602</v>
+      </c>
+      <c r="C28" s="11">
+        <f t="shared" si="3"/>
+        <v>2144.1720766939966</v>
+      </c>
+      <c r="D28" s="36">
+        <f t="shared" si="0"/>
+        <v>19.069035321363572</v>
+      </c>
+      <c r="E28" s="37">
+        <f t="shared" si="1"/>
+        <v>363.62810808741148</v>
+      </c>
+      <c r="G28">
+        <f>SQRT(G26^2+G27^2)</f>
+        <v>20.182439840487344</v>
+      </c>
+      <c r="H28" t="s">
+        <v>32</v>
+      </c>
+      <c r="I28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <f>G28/L5</f>
+        <v>9.4126959584352708E-3</v>
+      </c>
+      <c r="H29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I29" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
reviewed data from standards processing with Karina. In looking at the data the bay standard for alkalinity would be better checked against it's settled value after it has been fixed with mercuric chloride rather than with the raw conditions it was collected under. That being the case our uncertainty improved! Falling under the accepted value of 10
</commit_message>
<xml_diff>
--- a/check sample work/TA QAQC/20201110 results summary both probes.xlsx
+++ b/check sample work/TA QAQC/20201110 results summary both probes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11316" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="example to follow" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="QAQC crm &amp; baystd assessment" sheetId="3" r:id="rId3"/>
     <sheet name="QAQC crms assessment" sheetId="4" r:id="rId4"/>
     <sheet name="QAQC baystds assessment" sheetId="5" r:id="rId5"/>
+    <sheet name="Bay Std second look" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="230">
   <si>
     <t>sample</t>
   </si>
@@ -1177,7 +1178,7 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4025766" cy="3371398"/>
+    <xdr:ext cx="3423497" cy="2867025"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
@@ -1199,8 +1200,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5330825" y="0"/>
-          <a:ext cx="4025766" cy="3371398"/>
+          <a:off x="5473700" y="0"/>
+          <a:ext cx="3423497" cy="2867025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1520,20 +1521,20 @@
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.28515625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
-    <col min="13" max="13" width="51.140625" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" customWidth="1"/>
+    <col min="13" max="13" width="51.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1571,7 +1572,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1585,7 +1586,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1596,7 +1597,7 @@
         <v>2247.5363699999998</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1640,7 +1641,7 @@
       </c>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1651,7 +1652,7 @@
         <v>2114.1481899999999</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1662,7 +1663,7 @@
         <v>2138.9193500000001</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1706,7 +1707,7 @@
       </c>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1717,7 +1718,7 @@
         <v>2135.2389699999999</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1728,7 +1729,7 @@
         <v>2133.48756</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1772,7 +1773,7 @@
       </c>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1783,7 +1784,7 @@
         <v>2124.9360900000001</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1794,7 +1795,7 @@
         <v>2132.3921700000001</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1838,7 +1839,7 @@
       </c>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1849,7 +1850,7 @@
         <v>2249.3508299999999</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1860,7 +1861,7 @@
         <v>2250.2915600000001</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1907,10 +1908,10 @@
       </c>
       <c r="M16" s="3"/>
     </row>
-    <row r="20" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:14" x14ac:dyDescent="0.3">
       <c r="N20" s="4"/>
     </row>
-    <row r="21" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
         <v>34</v>
       </c>
@@ -1921,7 +1922,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E22">
         <f>2238.04</f>
         <v>2238.04</v>
@@ -1935,7 +1936,7 @@
         <v>21.704231088401922</v>
       </c>
     </row>
-    <row r="23" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E23">
         <f t="shared" ref="E23:E26" si="0">2238.04</f>
         <v>2238.04</v>
@@ -1949,7 +1950,7 @@
         <v>90.181043176897006</v>
       </c>
     </row>
-    <row r="24" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E24">
         <f t="shared" si="0"/>
         <v>2238.04</v>
@@ -1963,7 +1964,7 @@
         <v>62.986127504401573</v>
       </c>
     </row>
-    <row r="25" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E25">
         <f>2238.04</f>
         <v>2238.04</v>
@@ -1977,7 +1978,7 @@
         <v>127.93487528889766</v>
       </c>
     </row>
-    <row r="26" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E26">
         <f t="shared" si="0"/>
         <v>2238.04</v>
@@ -1991,7 +1992,7 @@
         <v>150.10072243360378</v>
       </c>
     </row>
-    <row r="29" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:14" x14ac:dyDescent="0.3">
       <c r="G29">
         <f>SQRT(SUM(G22:G26)/5)</f>
         <v>9.5174261173092578</v>
@@ -2000,7 +2001,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:14" x14ac:dyDescent="0.3">
       <c r="F30" s="3"/>
       <c r="G30">
         <v>0.53</v>
@@ -2009,7 +2010,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:14" x14ac:dyDescent="0.3">
       <c r="G31">
         <f>SQRT(G29^2+G30^2)</f>
         <v>9.5321718353395397</v>
@@ -2021,7 +2022,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:14" x14ac:dyDescent="0.3">
       <c r="G32">
         <f>G31/E26</f>
         <v>4.2591606206053246E-3</v>
@@ -2033,12 +2034,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:13" x14ac:dyDescent="0.3">
       <c r="M36" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="4:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D37" s="1" t="s">
         <v>38</v>
       </c>
@@ -2053,27 +2054,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M189"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A193" sqref="A193"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.28515625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="20.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" style="18" customWidth="1"/>
     <col min="5" max="5" width="10" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="19"/>
+    <col min="6" max="7" width="9.109375" style="19"/>
     <col min="8" max="8" width="13" style="19" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="41"/>
-    <col min="10" max="10" width="11.42578125" style="19" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" style="19"/>
-    <col min="13" max="13" width="51.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="41"/>
+    <col min="10" max="10" width="11.44140625" style="19" customWidth="1"/>
+    <col min="11" max="12" width="9.109375" style="19"/>
+    <col min="13" max="13" width="51.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -2111,7 +2112,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>40</v>
       </c>
@@ -2133,7 +2134,7 @@
       <c r="K2" s="21"/>
       <c r="L2" s="21"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>41</v>
       </c>
@@ -2153,7 +2154,7 @@
       <c r="K3" s="21"/>
       <c r="L3" s="21"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>42</v>
       </c>
@@ -2198,7 +2199,7 @@
       </c>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
         <v>6</v>
       </c>
@@ -2218,7 +2219,7 @@
       <c r="K5" s="21"/>
       <c r="L5" s="21"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
         <v>7</v>
       </c>
@@ -2238,7 +2239,7 @@
       <c r="K6" s="21"/>
       <c r="L6" s="21"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>8</v>
       </c>
@@ -2283,7 +2284,7 @@
       </c>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
         <v>9</v>
       </c>
@@ -2303,7 +2304,7 @@
       <c r="K8" s="21"/>
       <c r="L8" s="21"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
         <v>10</v>
       </c>
@@ -2323,7 +2324,7 @@
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
         <v>11</v>
       </c>
@@ -2368,7 +2369,7 @@
       </c>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
         <v>12</v>
       </c>
@@ -2388,7 +2389,7 @@
       <c r="K11" s="21"/>
       <c r="L11" s="21"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
         <v>13</v>
       </c>
@@ -2408,7 +2409,7 @@
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
         <v>14</v>
       </c>
@@ -2453,7 +2454,7 @@
       </c>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>43</v>
       </c>
@@ -2473,7 +2474,7 @@
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
         <v>44</v>
       </c>
@@ -2493,7 +2494,7 @@
       <c r="K15" s="21"/>
       <c r="L15" s="21"/>
     </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>45</v>
       </c>
@@ -2540,7 +2541,7 @@
       </c>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="30" t="s">
         <v>54</v>
       </c>
@@ -2558,7 +2559,7 @@
       <c r="I17" s="33"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
         <v>56</v>
       </c>
@@ -2602,7 +2603,7 @@
       </c>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
         <v>48</v>
       </c>
@@ -2616,7 +2617,7 @@
       <c r="I19" s="33"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
         <v>49</v>
       </c>
@@ -2630,7 +2631,7 @@
       <c r="I20" s="33"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
         <v>50</v>
       </c>
@@ -2671,7 +2672,7 @@
       </c>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="19" t="s">
         <v>51</v>
       </c>
@@ -2685,7 +2686,7 @@
       <c r="I22" s="33"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="19" t="s">
         <v>52</v>
       </c>
@@ -2699,7 +2700,7 @@
       <c r="I23" s="33"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="19" t="s">
         <v>53</v>
       </c>
@@ -2740,7 +2741,7 @@
       </c>
       <c r="M24" s="3"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
         <v>55</v>
       </c>
@@ -2748,7 +2749,7 @@
         <v>2278.2465769999999</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
         <v>57</v>
       </c>
@@ -2788,7 +2789,7 @@
         <v>4.9946979999999712</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="21" t="s">
         <v>65</v>
       </c>
@@ -2806,7 +2807,7 @@
       <c r="K27" s="21"/>
       <c r="L27" s="21"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
         <v>108</v>
       </c>
@@ -2824,7 +2825,7 @@
       <c r="K28" s="21"/>
       <c r="L28" s="21"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="21" t="s">
         <v>109</v>
       </c>
@@ -2866,7 +2867,7 @@
         <v>202.47002357553993</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="21" t="s">
         <v>66</v>
       </c>
@@ -2884,7 +2885,7 @@
       <c r="K30" s="21"/>
       <c r="L30" s="21"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="21" t="s">
         <v>67</v>
       </c>
@@ -2902,7 +2903,7 @@
       <c r="K31" s="21"/>
       <c r="L31" s="21"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="21" t="s">
         <v>68</v>
       </c>
@@ -2944,7 +2945,7 @@
         <v>8.0012203823998789</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="s">
         <v>69</v>
       </c>
@@ -2962,7 +2963,7 @@
       <c r="K33" s="21"/>
       <c r="L33" s="21"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="21" t="s">
         <v>70</v>
       </c>
@@ -2980,7 +2981,7 @@
       <c r="K34" s="21"/>
       <c r="L34" s="21"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
         <v>71</v>
       </c>
@@ -3022,7 +3023,7 @@
         <v>9.1970026297599361</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="21" t="s">
         <v>110</v>
       </c>
@@ -3040,7 +3041,7 @@
       <c r="K36" s="21"/>
       <c r="L36" s="21"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="21" t="s">
         <v>111</v>
       </c>
@@ -3082,7 +3083,7 @@
         <v>8.9153114503401412</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="19" t="s">
         <v>65</v>
       </c>
@@ -3090,7 +3091,7 @@
         <v>1624.2912168376199</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="19" t="s">
         <v>112</v>
       </c>
@@ -3098,7 +3099,7 @@
         <v>2241.6865483083102</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="19" t="s">
         <v>113</v>
       </c>
@@ -3138,7 +3139,7 @@
         <v>0.14446479651041955</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="19" t="s">
         <v>72</v>
       </c>
@@ -3146,7 +3147,7 @@
         <v>2125.89715188732</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="19" t="s">
         <v>73</v>
       </c>
@@ -3154,7 +3155,7 @@
         <v>2109.3231506451998</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="19" t="s">
         <v>74</v>
       </c>
@@ -3194,7 +3195,7 @@
         <v>16.574001242120175</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="19" t="s">
         <v>75</v>
       </c>
@@ -3202,7 +3203,7 @@
         <v>2122.2192108210402</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="19" t="s">
         <v>76</v>
       </c>
@@ -3210,7 +3211,7 @@
         <v>2123.5923451169101</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="19" t="s">
         <v>77</v>
       </c>
@@ -3250,7 +3251,7 @@
         <v>12.418599309430192</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="19" t="s">
         <v>114</v>
       </c>
@@ -3258,7 +3259,7 @@
         <v>2236.1095817401701</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="19" t="s">
         <v>115</v>
       </c>
@@ -3298,7 +3299,7 @@
         <v>0.92449238705012249</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="21" t="s">
         <v>65</v>
       </c>
@@ -3316,7 +3317,7 @@
       <c r="K49" s="21"/>
       <c r="L49" s="21"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="21" t="s">
         <v>116</v>
       </c>
@@ -3334,7 +3335,7 @@
       <c r="K50" s="21"/>
       <c r="L50" s="21"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="21" t="s">
         <v>117</v>
       </c>
@@ -3376,7 +3377,7 @@
         <v>0.62477194547000181</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="21" t="s">
         <v>78</v>
       </c>
@@ -3394,7 +3395,7 @@
       <c r="K52" s="21"/>
       <c r="L52" s="21"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="21" t="s">
         <v>79</v>
       </c>
@@ -3412,7 +3413,7 @@
       <c r="K53" s="21"/>
       <c r="L53" s="21"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="21" t="s">
         <v>80</v>
       </c>
@@ -3454,7 +3455,7 @@
         <v>3.6758375283698115</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="21" t="s">
         <v>81</v>
       </c>
@@ -3472,7 +3473,7 @@
       <c r="K55" s="21"/>
       <c r="L55" s="21"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="21" t="s">
         <v>82</v>
       </c>
@@ -3490,7 +3491,7 @@
       <c r="K56" s="21"/>
       <c r="L56" s="21"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="21" t="s">
         <v>83</v>
       </c>
@@ -3532,7 +3533,7 @@
         <v>4.6240391373403327</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="21" t="s">
         <v>84</v>
       </c>
@@ -3550,7 +3551,7 @@
       <c r="K58" s="21"/>
       <c r="L58" s="21"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="21" t="s">
         <v>85</v>
       </c>
@@ -3568,7 +3569,7 @@
       <c r="K59" s="21"/>
       <c r="L59" s="21"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="21" t="s">
         <v>86</v>
       </c>
@@ -3610,7 +3611,7 @@
         <v>0.46416779767014305</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="21" t="s">
         <v>118</v>
       </c>
@@ -3628,7 +3629,7 @@
       <c r="K61" s="21"/>
       <c r="L61" s="21"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="21" t="s">
         <v>119</v>
       </c>
@@ -3670,7 +3671,7 @@
         <v>0.88344358794984146</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="19" t="s">
         <v>65</v>
       </c>
@@ -3678,7 +3679,7 @@
         <v>1592.1393647914399</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="19" t="s">
         <v>120</v>
       </c>
@@ -3686,7 +3687,7 @@
         <v>2247.3720067191798</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="19" t="s">
         <v>121</v>
       </c>
@@ -3726,7 +3727,7 @@
         <v>2.4952530231798846</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="19" t="s">
         <v>87</v>
       </c>
@@ -3734,7 +3735,7 @@
         <v>2234.7435887859501</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="19" t="s">
         <v>88</v>
       </c>
@@ -3742,7 +3743,7 @@
         <v>2227.2541142131499</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="19" t="s">
         <v>89</v>
       </c>
@@ -3782,7 +3783,7 @@
         <v>10.515290785639991</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="19" t="s">
         <v>90</v>
       </c>
@@ -3790,7 +3791,7 @@
         <v>2233.5328075264601</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="19" t="s">
         <v>91</v>
       </c>
@@ -3798,7 +3799,7 @@
         <v>2235.2718356786399</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="19" t="s">
         <v>92</v>
       </c>
@@ -3838,7 +3839,7 @@
         <v>5.2933858786800556</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="19" t="s">
         <v>93</v>
       </c>
@@ -3846,7 +3847,7 @@
         <v>2231.41222642809</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="19" t="s">
         <v>94</v>
       </c>
@@ -3854,7 +3855,7 @@
         <v>2218.87534925306</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="19" t="s">
         <v>95</v>
       </c>
@@ -3894,7 +3895,7 @@
         <v>12.536877175029986</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="19" t="s">
         <v>122</v>
       </c>
@@ -3902,7 +3903,7 @@
         <v>2241.6593895374199</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="19" t="s">
         <v>123</v>
       </c>
@@ -3942,7 +3943,7 @@
         <v>2.5427539370703016</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="21" t="s">
         <v>65</v>
       </c>
@@ -3960,7 +3961,7 @@
       <c r="K77" s="21"/>
       <c r="L77" s="21"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="21" t="s">
         <v>124</v>
       </c>
@@ -3978,7 +3979,7 @@
       <c r="K78" s="21"/>
       <c r="L78" s="21"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="21" t="s">
         <v>125</v>
       </c>
@@ -4020,7 +4021,7 @@
         <v>19.982069738440259</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="34" t="s">
         <v>128</v>
       </c>
@@ -4040,7 +4041,7 @@
       <c r="K80" s="34"/>
       <c r="L80" s="34"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="34" t="s">
         <v>130</v>
       </c>
@@ -4060,7 +4061,7 @@
       <c r="K81" s="34"/>
       <c r="L81" s="34"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="34" t="s">
         <v>131</v>
       </c>
@@ -4104,7 +4105,7 @@
         <v>9.7230443598400598</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="21" t="s">
         <v>126</v>
       </c>
@@ -4122,7 +4123,7 @@
       <c r="K83" s="21"/>
       <c r="L83" s="21"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="21" t="s">
         <v>127</v>
       </c>
@@ -4164,7 +4165,7 @@
         <v>3.114767579850195</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="19" t="s">
         <v>65</v>
       </c>
@@ -4172,7 +4173,7 @@
         <v>1767.4127862110699</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="30" t="s">
         <v>132</v>
       </c>
@@ -4182,7 +4183,7 @@
       <c r="C86" s="30"/>
       <c r="D86" s="31"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="19" t="s">
         <v>133</v>
       </c>
@@ -4222,7 +4223,7 @@
         <v>200.93180595105991</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="19" t="s">
         <v>136</v>
       </c>
@@ -4230,7 +4231,7 @@
         <v>2223.7491846081298</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" s="19" t="s">
         <v>137</v>
       </c>
@@ -4270,7 +4271,7 @@
         <v>4.2857932929500748</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="19" t="s">
         <v>96</v>
       </c>
@@ -4278,7 +4279,7 @@
         <v>2176.50294375658</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" s="19" t="s">
         <v>97</v>
       </c>
@@ -4286,7 +4287,7 @@
         <v>2186.08511792934</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" s="19" t="s">
         <v>98</v>
       </c>
@@ -4326,7 +4327,7 @@
         <v>35.996994867829926</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="19" t="s">
         <v>99</v>
       </c>
@@ -4334,7 +4335,7 @@
         <v>2103.7936989664699</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" s="19" t="s">
         <v>100</v>
       </c>
@@ -4342,7 +4343,7 @@
         <v>2076.5450829193901</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" s="19" t="s">
         <v>101</v>
       </c>
@@ -4382,7 +4383,7 @@
         <v>27.24861604707985</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" s="19" t="s">
         <v>134</v>
       </c>
@@ -4390,7 +4391,7 @@
         <v>2157.74591479522</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="19" t="s">
         <v>135</v>
       </c>
@@ -4430,7 +4431,7 @@
         <v>16.870894775150191</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" s="21" t="s">
         <v>65</v>
       </c>
@@ -4448,7 +4449,7 @@
       <c r="K98" s="21"/>
       <c r="L98" s="21"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" s="21" t="s">
         <v>139</v>
       </c>
@@ -4466,7 +4467,7 @@
       <c r="K99" s="21"/>
       <c r="L99" s="21"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" s="21" t="s">
         <v>140</v>
       </c>
@@ -4508,7 +4509,7 @@
         <v>7.5272198213497177</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" s="21" t="s">
         <v>138</v>
       </c>
@@ -4526,7 +4527,7 @@
       <c r="K101" s="21"/>
       <c r="L101" s="21"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" s="21" t="s">
         <v>102</v>
       </c>
@@ -4544,7 +4545,7 @@
       <c r="K102" s="21"/>
       <c r="L102" s="21"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" s="21" t="s">
         <v>103</v>
       </c>
@@ -4562,7 +4563,7 @@
       <c r="K103" s="21"/>
       <c r="L103" s="21"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" s="21" t="s">
         <v>104</v>
       </c>
@@ -4604,7 +4605,7 @@
         <v>7.1066143973698672</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="21" t="s">
         <v>105</v>
       </c>
@@ -4622,7 +4623,7 @@
       <c r="K105" s="21"/>
       <c r="L105" s="21"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" s="21" t="s">
         <v>106</v>
       </c>
@@ -4640,7 +4641,7 @@
       <c r="K106" s="21"/>
       <c r="L106" s="21"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" s="21" t="s">
         <v>107</v>
       </c>
@@ -4682,7 +4683,7 @@
         <v>12.227740629090022</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" s="21" t="s">
         <v>141</v>
       </c>
@@ -4700,7 +4701,7 @@
       <c r="K108" s="21"/>
       <c r="L108" s="21"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" s="21" t="s">
         <v>142</v>
       </c>
@@ -4742,7 +4743,7 @@
         <v>104.21104304512983</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" s="19" t="s">
         <v>65</v>
       </c>
@@ -4750,7 +4751,7 @@
         <v>1712.82598863931</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" s="19" t="s">
         <v>162</v>
       </c>
@@ -4758,7 +4759,7 @@
         <v>2156.3511491220902</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" s="19" t="s">
         <v>163</v>
       </c>
@@ -4766,7 +4767,7 @@
         <v>2167.2565757031798</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" s="19" t="s">
         <v>164</v>
       </c>
@@ -4806,7 +4807,7 @@
         <v>10.905426581089614</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" s="19" t="s">
         <v>153</v>
       </c>
@@ -4814,7 +4815,7 @@
         <v>2095.24484288339</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" s="19" t="s">
         <v>154</v>
       </c>
@@ -4822,7 +4823,7 @@
         <v>2100.3120996130501</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" s="19" t="s">
         <v>155</v>
       </c>
@@ -4862,7 +4863,7 @@
         <v>10.806316414660159</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" s="19" t="s">
         <v>156</v>
       </c>
@@ -4870,7 +4871,7 @@
         <v>2218.8993800551598</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" s="19" t="s">
         <v>157</v>
       </c>
@@ -4878,7 +4879,7 @@
         <v>2186.6045565018098</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" s="19" t="s">
         <v>158</v>
       </c>
@@ -4918,7 +4919,7 @@
         <v>32.294823553349943</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" s="19" t="s">
         <v>159</v>
       </c>
@@ -4926,7 +4927,7 @@
         <v>2186.45070089</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" s="19" t="s">
         <v>160</v>
       </c>
@@ -4934,7 +4935,7 @@
         <v>2194.8913127686101</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122" s="19" t="s">
         <v>161</v>
       </c>
@@ -4974,7 +4975,7 @@
         <v>8.4406118786100706</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123" s="19" t="s">
         <v>165</v>
       </c>
@@ -4982,7 +4983,7 @@
         <v>2173.0418402661999</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" s="19" t="s">
         <v>166</v>
       </c>
@@ -4990,7 +4991,7 @@
         <v>2182.96053312513</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" s="19" t="s">
         <v>167</v>
       </c>
@@ -5030,7 +5031,7 @@
         <v>9.9186928589301715</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126" s="19" t="s">
         <v>168</v>
       </c>
@@ -5038,7 +5039,7 @@
         <v>2232.7275708530301</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127" s="19" t="s">
         <v>169</v>
       </c>
@@ -5046,7 +5047,7 @@
         <v>2225.3939498013601</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" s="19" t="s">
         <v>170</v>
       </c>
@@ -5086,7 +5087,7 @@
         <v>8.6111939932702626</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129" s="21" t="s">
         <v>65</v>
       </c>
@@ -5104,7 +5105,7 @@
       <c r="K129" s="21"/>
       <c r="L129" s="21"/>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130" s="21" t="s">
         <v>171</v>
       </c>
@@ -5122,7 +5123,7 @@
       <c r="K130" s="21"/>
       <c r="L130" s="21"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131" s="21" t="s">
         <v>172</v>
       </c>
@@ -5140,7 +5141,7 @@
       <c r="K131" s="21"/>
       <c r="L131" s="21"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132" s="21" t="s">
         <v>173</v>
       </c>
@@ -5182,7 +5183,7 @@
         <v>6.1719923844798359</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A133" s="21" t="s">
         <v>174</v>
       </c>
@@ -5200,7 +5201,7 @@
       <c r="K133" s="21"/>
       <c r="L133" s="21"/>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134" s="21" t="s">
         <v>175</v>
       </c>
@@ -5218,7 +5219,7 @@
       <c r="K134" s="21"/>
       <c r="L134" s="21"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A135" s="21" t="s">
         <v>176</v>
       </c>
@@ -5260,7 +5261,7 @@
         <v>3.7418551294699682</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A136" s="21" t="s">
         <v>177</v>
       </c>
@@ -5278,7 +5279,7 @@
       <c r="K136" s="21"/>
       <c r="L136" s="21"/>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137" s="21" t="s">
         <v>178</v>
       </c>
@@ -5296,7 +5297,7 @@
       <c r="K137" s="21"/>
       <c r="L137" s="21"/>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138" s="21" t="s">
         <v>179</v>
       </c>
@@ -5338,7 +5339,7 @@
         <v>99.351645211729647</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A139" s="21" t="s">
         <v>180</v>
       </c>
@@ -5356,7 +5357,7 @@
       <c r="K139" s="21"/>
       <c r="L139" s="21"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A140" s="21" t="s">
         <v>181</v>
       </c>
@@ -5374,7 +5375,7 @@
       <c r="K140" s="21"/>
       <c r="L140" s="21"/>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A141" s="21" t="s">
         <v>182</v>
       </c>
@@ -5416,7 +5417,7 @@
         <v>7.6350153611201677</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A142" s="21" t="s">
         <v>183</v>
       </c>
@@ -5434,7 +5435,7 @@
       <c r="K142" s="21"/>
       <c r="L142" s="21"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143" s="21" t="s">
         <v>184</v>
       </c>
@@ -5452,7 +5453,7 @@
       <c r="K143" s="21"/>
       <c r="L143" s="21"/>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A144" s="21" t="s">
         <v>185</v>
       </c>
@@ -5494,7 +5495,7 @@
         <v>5.9110954046300321</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145" s="19" t="s">
         <v>65</v>
       </c>
@@ -5502,7 +5503,7 @@
         <v>1732.26717091612</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A146" s="19" t="s">
         <v>186</v>
       </c>
@@ -5510,7 +5511,7 @@
         <v>2171.6037363503101</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A147" s="19" t="s">
         <v>187</v>
       </c>
@@ -5518,7 +5519,7 @@
         <v>2168.3325368241499</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A148" s="19" t="s">
         <v>188</v>
       </c>
@@ -5558,7 +5559,7 @@
         <v>3.2711995261602169</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A149" s="19" t="s">
         <v>189</v>
       </c>
@@ -5566,7 +5567,7 @@
         <v>2205.29339655284</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A150" s="19" t="s">
         <v>190</v>
       </c>
@@ -5574,7 +5575,7 @@
         <v>2203.5715719336199</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A151" s="19" t="s">
         <v>191</v>
       </c>
@@ -5614,7 +5615,7 @@
         <v>1.721824619220115</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A152" s="19" t="s">
         <v>192</v>
       </c>
@@ -5622,7 +5623,7 @@
         <v>2209.2654099239599</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A153" s="19" t="s">
         <v>193</v>
       </c>
@@ -5630,7 +5631,7 @@
         <v>2205.6468945710899</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A154" s="19" t="s">
         <v>194</v>
       </c>
@@ -5670,7 +5671,7 @@
         <v>3.618515352869963</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A155" s="19" t="s">
         <v>195</v>
       </c>
@@ -5678,7 +5679,7 @@
         <v>2201.95312729751</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A156" s="19" t="s">
         <v>196</v>
       </c>
@@ -5686,7 +5687,7 @@
         <v>2201.7544015737499</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A157" s="19" t="s">
         <v>197</v>
       </c>
@@ -5726,7 +5727,7 @@
         <v>5.0274952043100711</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A158" s="19" t="s">
         <v>198</v>
       </c>
@@ -5734,7 +5735,7 @@
         <v>2172.39686499658</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A159" s="19" t="s">
         <v>199</v>
       </c>
@@ -5742,7 +5743,7 @@
         <v>2167.4396622854201</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A160" s="19" t="s">
         <v>200</v>
       </c>
@@ -5782,7 +5783,7 @@
         <v>4.95720271115988</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A161" s="19" t="s">
         <v>201</v>
       </c>
@@ -5790,7 +5791,7 @@
         <v>2234.9084845810298</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A162" s="19" t="s">
         <v>202</v>
       </c>
@@ -5798,7 +5799,7 @@
         <v>2233.8319039288199</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A163" s="19" t="s">
         <v>203</v>
       </c>
@@ -5838,7 +5839,7 @@
         <v>2.9707386936402145</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A164" s="19" t="s">
         <v>215</v>
       </c>
@@ -5846,7 +5847,7 @@
         <v>2791.47452987631</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A165" s="19" t="s">
         <v>207</v>
       </c>
@@ -5854,7 +5855,7 @@
         <v>2253.5400879193598</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A166" s="19" t="s">
         <v>208</v>
       </c>
@@ -5862,7 +5863,7 @@
         <v>2250.3490168078902</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A167" s="19" t="s">
         <v>209</v>
       </c>
@@ -5870,7 +5871,7 @@
         <v>2261.73917919109</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A168" s="19" t="s">
         <v>210</v>
       </c>
@@ -5878,7 +5879,7 @@
         <v>2241.4624109891101</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A169" s="19" t="s">
         <v>211</v>
       </c>
@@ -5886,7 +5887,7 @@
         <v>2258.1304930768201</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A170" s="19" t="s">
         <v>212</v>
       </c>
@@ -5894,7 +5895,7 @@
         <v>2251.4238491137899</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A171" s="19" t="s">
         <v>213</v>
       </c>
@@ -5934,7 +5935,7 @@
         <v>20.276768201979849</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A172" s="19" t="s">
         <v>214</v>
       </c>
@@ -5942,7 +5943,7 @@
         <v>2424.3536009301201</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A173" s="19" t="s">
         <v>204</v>
       </c>
@@ -5950,7 +5951,7 @@
         <v>2220.1114998255798</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A174" s="19" t="s">
         <v>205</v>
       </c>
@@ -5958,7 +5959,7 @@
         <v>2223.29862647973</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A175" s="19" t="s">
         <v>206</v>
       </c>
@@ -5998,7 +5999,7 @@
         <v>5.3446747965799659</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A176" s="19" t="s">
         <v>215</v>
       </c>
@@ -6006,7 +6007,7 @@
         <v>2053.3155707137898</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A177" s="19" t="s">
         <v>217</v>
       </c>
@@ -6014,7 +6015,7 @@
         <v>2121.1126006919999</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A178" s="19" t="s">
         <v>218</v>
       </c>
@@ -6022,7 +6023,7 @@
         <v>2114.3140912812701</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A179" s="19" t="s">
         <v>219</v>
       </c>
@@ -6062,7 +6063,7 @@
         <v>16.851486293259768</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A180" s="19" t="s">
         <v>220</v>
       </c>
@@ -6070,7 +6071,7 @@
         <v>2136.7025174391802</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A181" s="19" t="s">
         <v>221</v>
       </c>
@@ -6078,7 +6079,7 @@
         <v>2137.4028738178399</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A182" s="19" t="s">
         <v>222</v>
       </c>
@@ -6118,7 +6119,7 @@
         <v>1.0440521757400347</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A183" s="19" t="s">
         <v>223</v>
       </c>
@@ -6126,7 +6127,7 @@
         <v>2112.5960733162501</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A184" s="19" t="s">
         <v>224</v>
       </c>
@@ -6134,7 +6135,7 @@
         <v>2105.44065001114</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A185" s="19" t="s">
         <v>225</v>
       </c>
@@ -6174,7 +6175,7 @@
         <v>10.104269404670049</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A186" s="19" t="s">
         <v>214</v>
       </c>
@@ -6182,7 +6183,7 @@
         <v>1798.38269926629</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A187" s="19" t="s">
         <v>226</v>
       </c>
@@ -6190,7 +6191,7 @@
         <v>2167.3314732691902</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A188" s="19" t="s">
         <v>227</v>
       </c>
@@ -6198,7 +6199,7 @@
         <v>2162.0931306789098</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A189" s="19" t="s">
         <v>228</v>
       </c>
@@ -6248,29 +6249,29 @@
   <dimension ref="A1:M70"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="103" style="6" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" style="11" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="12" customWidth="1"/>
-    <col min="14" max="14" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" style="11" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="12" customWidth="1"/>
+    <col min="14" max="14" width="59.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -6301,7 +6302,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>40</v>
       </c>
@@ -6332,7 +6333,7 @@
         <v>33.311999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>41</v>
       </c>
@@ -6368,7 +6369,7 @@
         <v>33.661000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>42</v>
       </c>
@@ -6403,7 +6404,7 @@
         <v>33.524999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>43</v>
       </c>
@@ -6442,7 +6443,7 @@
         <v>27.53</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>44</v>
       </c>
@@ -6471,7 +6472,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -6491,7 +6492,7 @@
         <v>4.9540482249982379E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -6511,7 +6512,7 @@
         <v>1616.5688340569229</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -6531,7 +6532,7 @@
         <v>2043.1552616256156</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>108</v>
       </c>
@@ -6551,7 +6552,7 @@
         <v>1194.6338725265152</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>110</v>
       </c>
@@ -6571,7 +6572,7 @@
         <v>460.54747632980491</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>111</v>
       </c>
@@ -6591,7 +6592,7 @@
         <v>922.68201761768364</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>112</v>
       </c>
@@ -6611,7 +6612,7 @@
         <v>881.29115046163486</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>113</v>
       </c>
@@ -6631,7 +6632,7 @@
         <v>872.73469821815206</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>114</v>
       </c>
@@ -6651,7 +6652,7 @@
         <v>581.27193168594556</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>115</v>
       </c>
@@ -6671,7 +6672,7 @@
         <v>537.54836831215925</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>116</v>
       </c>
@@ -6691,7 +6692,7 @@
         <v>1296.1908027475388</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>117</v>
       </c>
@@ -6711,7 +6712,7 @@
         <v>1251.5942514404196</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>118</v>
       </c>
@@ -6737,7 +6738,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>119</v>
       </c>
@@ -6763,7 +6764,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>120</v>
       </c>
@@ -6783,7 +6784,7 @@
         <v>1251.1788593417016</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>121</v>
       </c>
@@ -6803,7 +6804,7 @@
         <v>1080.8809335874446</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>122</v>
       </c>
@@ -6823,7 +6824,7 @@
         <v>879.67938773241201</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>123</v>
       </c>
@@ -6843,7 +6844,7 @@
         <v>1036.9780443516509</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>124</v>
       </c>
@@ -6863,7 +6864,7 @@
         <v>1778.9155994712464</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>125</v>
       </c>
@@ -6883,7 +6884,7 @@
         <v>492.6234913924153</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>126</v>
       </c>
@@ -6903,7 +6904,7 @@
         <v>24.072827949184788</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>127</v>
       </c>
@@ -6923,7 +6924,7 @@
         <v>64.339238860453506</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>133</v>
       </c>
@@ -6943,7 +6944,7 @@
         <v>207.8719331919755</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>136</v>
       </c>
@@ -6963,7 +6964,7 @@
         <v>138.04333895591375</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>137</v>
       </c>
@@ -6984,7 +6985,7 @@
       </c>
       <c r="F31" s="7"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>134</v>
       </c>
@@ -7004,7 +7005,7 @@
         <v>184.24908079822336</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>135</v>
       </c>
@@ -7024,7 +7025,7 @@
         <v>926.88175991374135</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>139</v>
       </c>
@@ -7044,7 +7045,7 @@
         <v>486.91166620058681</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
         <v>140</v>
       </c>
@@ -7064,7 +7065,7 @@
         <v>875.76309877890378</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
         <v>138</v>
       </c>
@@ -7084,7 +7085,7 @@
         <v>303.23018266722977</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
         <v>141</v>
       </c>
@@ -7104,7 +7105,7 @@
         <v>2294.9404868978409</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>162</v>
       </c>
@@ -7124,7 +7125,7 @@
         <v>148.32980520874986</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>163</v>
       </c>
@@ -7144,7 +7145,7 @@
         <v>532.89409450498101</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>164</v>
       </c>
@@ -7164,7 +7165,7 @@
         <v>283.20100953040998</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>165</v>
       </c>
@@ -7184,7 +7185,7 @@
         <v>833.46324871491561</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>166</v>
       </c>
@@ -7204,7 +7205,7 @@
         <v>1504.5443523099382</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>167</v>
       </c>
@@ -7224,7 +7225,7 @@
         <v>1359.7250044629604</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>168</v>
       </c>
@@ -7244,7 +7245,7 @@
         <v>429.63219346738299</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>169</v>
       </c>
@@ -7264,7 +7265,7 @@
         <v>179.39789128135487</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>170</v>
       </c>
@@ -7284,7 +7285,7 @@
         <v>146.80658820772371</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>171</v>
       </c>
@@ -7304,7 +7305,7 @@
         <v>804.34807109832093</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
         <v>172</v>
       </c>
@@ -7324,7 +7325,7 @@
         <v>625.20915402841661</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
         <v>173</v>
       </c>
@@ -7344,7 +7345,7 @@
         <v>492.3534281993272</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
         <v>180</v>
       </c>
@@ -7364,7 +7365,7 @@
         <v>695.82572169514754</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
         <v>181</v>
       </c>
@@ -7384,7 +7385,7 @@
         <v>611.69319324915011</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
         <v>182</v>
       </c>
@@ -7404,7 +7405,7 @@
         <v>351.31854287090141</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="s">
         <v>183</v>
       </c>
@@ -7424,7 +7425,7 @@
         <v>380.30484808213612</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
         <v>184</v>
       </c>
@@ -7444,7 +7445,7 @@
         <v>636.11390476472218</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -7464,7 +7465,7 @@
         <v>372.88394874373085</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>186</v>
       </c>
@@ -7484,7 +7485,7 @@
         <v>752.49595149981849</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>187</v>
       </c>
@@ -7504,7 +7505,7 @@
         <v>583.72783370072705</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>188</v>
       </c>
@@ -7524,7 +7525,7 @@
         <v>650.68824789365851</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>198</v>
       </c>
@@ -7544,7 +7545,7 @@
         <v>796.63867472564982</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>199</v>
       </c>
@@ -7564,7 +7565,7 @@
         <v>541.38053925422037</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>200</v>
       </c>
@@ -7584,7 +7585,7 @@
         <v>764.16382344027829</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>201</v>
       </c>
@@ -7604,7 +7605,7 @@
         <v>524.79866579928125</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>202</v>
       </c>
@@ -7624,7 +7625,7 @@
         <v>476.6320291572211</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>203</v>
       </c>
@@ -7644,7 +7645,7 @@
         <v>615.17108105747434</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>204</v>
       </c>
@@ -7664,7 +7665,7 @@
         <v>65.79642942038133</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>205</v>
       </c>
@@ -7684,7 +7685,7 @@
         <v>127.65896032845698</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>206</v>
       </c>
@@ -7704,7 +7705,7 @@
         <v>35.44954064528568</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>226</v>
       </c>
@@ -7724,7 +7725,7 @@
         <v>536.35764972708762</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>227</v>
       </c>
@@ -7744,7 +7745,7 @@
         <v>321.16417593017383</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>228</v>
       </c>
@@ -7780,29 +7781,29 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G32" sqref="G32:I37"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" customWidth="1"/>
     <col min="11" max="11" width="103" style="6" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" style="11" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" style="12" customWidth="1"/>
-    <col min="15" max="15" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" style="11" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" style="12" customWidth="1"/>
+    <col min="15" max="15" width="59.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
@@ -7833,7 +7834,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>56</v>
       </c>
@@ -7871,7 +7872,7 @@
         <v>33.311999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>40</v>
       </c>
@@ -7906,7 +7907,7 @@
         <v>33.661000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>41</v>
       </c>
@@ -7945,7 +7946,7 @@
         <v>33.524999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
         <v>42</v>
       </c>
@@ -7983,7 +7984,7 @@
         <v>27.53</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
@@ -8003,7 +8004,7 @@
         <v>127.93487528889766</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>44</v>
       </c>
@@ -8026,7 +8027,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
@@ -8046,7 +8047,7 @@
         <v>1616.5688340569229</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
         <v>57</v>
       </c>
@@ -8073,7 +8074,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
         <v>108</v>
       </c>
@@ -8099,7 +8100,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
         <v>110</v>
       </c>
@@ -8129,7 +8130,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
         <v>111</v>
       </c>
@@ -8159,7 +8160,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>112</v>
       </c>
@@ -8179,7 +8180,7 @@
         <v>881.29115046163486</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>113</v>
       </c>
@@ -8199,7 +8200,7 @@
         <v>872.73469821815206</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>114</v>
       </c>
@@ -8222,7 +8223,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>115</v>
       </c>
@@ -8242,7 +8243,7 @@
         <v>537.54836831215925</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="23" t="s">
         <v>116</v>
       </c>
@@ -8269,7 +8270,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="23" t="s">
         <v>117</v>
       </c>
@@ -8295,7 +8296,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="23" t="s">
         <v>118</v>
       </c>
@@ -8331,7 +8332,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="23" t="s">
         <v>119</v>
       </c>
@@ -8367,7 +8368,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
         <v>120</v>
       </c>
@@ -8387,7 +8388,7 @@
         <v>1251.1788593417016</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
         <v>121</v>
       </c>
@@ -8410,7 +8411,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
         <v>122</v>
       </c>
@@ -8430,7 +8431,7 @@
         <v>879.67938773241201</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
         <v>123</v>
       </c>
@@ -8457,7 +8458,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="23" t="s">
         <v>124</v>
       </c>
@@ -8483,7 +8484,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
         <v>125</v>
       </c>
@@ -8513,7 +8514,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="21" t="s">
         <v>126</v>
       </c>
@@ -8543,7 +8544,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
         <v>127</v>
       </c>
@@ -8563,7 +8564,7 @@
         <v>64.339238860453506</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="19" t="s">
         <v>136</v>
       </c>
@@ -8583,7 +8584,7 @@
         <v>138.04333895591375</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="19" t="s">
         <v>137</v>
       </c>
@@ -8603,7 +8604,7 @@
         <v>257.12051628811935</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="21" t="s">
         <v>138</v>
       </c>
@@ -8624,7 +8625,7 @@
       </c>
       <c r="F31" s="7"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="19" t="s">
         <v>168</v>
       </c>
@@ -8650,7 +8651,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="19" t="s">
         <v>169</v>
       </c>
@@ -8670,7 +8671,7 @@
         <v>179.39789128135487</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
         <v>170</v>
       </c>
@@ -8697,7 +8698,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
         <v>183</v>
       </c>
@@ -8723,7 +8724,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="21" t="s">
         <v>184</v>
       </c>
@@ -8753,7 +8754,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="21" t="s">
         <v>185</v>
       </c>
@@ -8783,7 +8784,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="19" t="s">
         <v>201</v>
       </c>
@@ -8803,7 +8804,7 @@
         <v>524.79866579928125</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="19" t="s">
         <v>202</v>
       </c>
@@ -8823,7 +8824,7 @@
         <v>476.6320291572211</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="19" t="s">
         <v>203</v>
       </c>
@@ -8843,7 +8844,7 @@
         <v>615.17108105747434</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="39" t="s">
         <v>204</v>
       </c>
@@ -8863,7 +8864,7 @@
         <v>65.79642942038133</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="39" t="s">
         <v>205</v>
       </c>
@@ -8883,7 +8884,7 @@
         <v>127.65896032845698</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="39" t="s">
         <v>206</v>
       </c>
@@ -8914,29 +8915,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="103" style="6" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" style="11" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="12" customWidth="1"/>
-    <col min="14" max="14" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" style="11" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="12" customWidth="1"/>
+    <col min="14" max="14" width="59.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -8964,7 +8965,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>133</v>
       </c>
@@ -9002,7 +9003,7 @@
         <v>33.311999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>134</v>
       </c>
@@ -9037,7 +9038,7 @@
         <v>33.661000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -9076,7 +9077,7 @@
         <v>33.524999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>139</v>
       </c>
@@ -9115,7 +9116,7 @@
         <v>27.53</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>140</v>
       </c>
@@ -9135,7 +9136,7 @@
         <v>875.76309877890378</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>141</v>
       </c>
@@ -9155,7 +9156,7 @@
         <v>2294.9404868978409</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>162</v>
       </c>
@@ -9175,7 +9176,7 @@
         <v>148.32980520874986</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>163</v>
       </c>
@@ -9195,7 +9196,7 @@
         <v>532.89409450498101</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>164</v>
       </c>
@@ -9215,7 +9216,7 @@
         <v>283.20100953040998</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>165</v>
       </c>
@@ -9235,7 +9236,7 @@
         <v>833.46324871491561</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>166</v>
       </c>
@@ -9255,7 +9256,7 @@
         <v>1504.5443523099382</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>167</v>
       </c>
@@ -9275,7 +9276,7 @@
         <v>1359.7250044629604</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>171</v>
       </c>
@@ -9295,7 +9296,7 @@
         <v>804.34807109832093</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>172</v>
       </c>
@@ -9315,7 +9316,7 @@
         <v>625.20915402841661</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>173</v>
       </c>
@@ -9335,7 +9336,7 @@
         <v>492.3534281993272</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>180</v>
       </c>
@@ -9355,7 +9356,7 @@
         <v>695.82572169514754</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>181</v>
       </c>
@@ -9375,7 +9376,7 @@
         <v>611.69319324915011</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>182</v>
       </c>
@@ -9401,7 +9402,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>186</v>
       </c>
@@ -9427,7 +9428,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>187</v>
       </c>
@@ -9447,7 +9448,7 @@
         <v>583.72783370072705</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>188</v>
       </c>
@@ -9467,7 +9468,7 @@
         <v>650.68824789365851</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>198</v>
       </c>
@@ -9487,7 +9488,7 @@
         <v>796.63867472564982</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>199</v>
       </c>
@@ -9513,7 +9514,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>200</v>
       </c>
@@ -9533,7 +9534,7 @@
         <v>764.16382344027829</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>226</v>
       </c>
@@ -9560,7 +9561,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>227</v>
       </c>
@@ -9586,7 +9587,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>228</v>
       </c>
@@ -9616,7 +9617,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G29">
         <f>G28/L5</f>
         <v>9.4126959584352708E-3</v>
@@ -9628,7 +9629,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F31" s="7"/>
     </row>
   </sheetData>
@@ -9636,4 +9637,709 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" style="11" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="11">
+        <v>2158.5898411945</v>
+      </c>
+      <c r="C2" s="11">
+        <f>$L$5</f>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D2" s="36">
+        <f t="shared" ref="D2:D28" si="0">B2-C2</f>
+        <v>-5.0610139921968766</v>
+      </c>
+      <c r="E2" s="37">
+        <f t="shared" ref="E2:E28" si="1">D2^2</f>
+        <v>25.613862629212566</v>
+      </c>
+      <c r="G2">
+        <f>SQRT(SUM(E2:E28)/ROWS(E2:E28))</f>
+        <v>9.472145335222498</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" s="11">
+        <v>2403.7199999999998</v>
+      </c>
+      <c r="M2" s="12">
+        <v>33.311999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="11">
+        <v>2157.74591479522</v>
+      </c>
+      <c r="C3" s="11">
+        <f t="shared" ref="C3:C28" si="2">$L$5</f>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D3" s="36">
+        <f t="shared" si="0"/>
+        <v>-5.9049403914768845</v>
+      </c>
+      <c r="E3" s="37">
+        <f t="shared" si="1"/>
+        <v>34.868321026895181</v>
+      </c>
+      <c r="G3">
+        <v>0.53</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" s="11">
+        <v>2238.04</v>
+      </c>
+      <c r="M3" s="12">
+        <v>33.661000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="11">
+        <v>2174.6168095703702</v>
+      </c>
+      <c r="C4" s="11">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D4" s="36">
+        <f t="shared" si="0"/>
+        <v>10.965954383673306</v>
+      </c>
+      <c r="E4" s="37">
+        <f t="shared" si="1"/>
+        <v>120.25215554480381</v>
+      </c>
+      <c r="G4">
+        <f>SQRT(G2^2+G3^2)</f>
+        <v>9.4869614340724144</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L4" s="11">
+        <v>2212</v>
+      </c>
+      <c r="M4" s="12">
+        <v>33.524999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="13">
+        <v>2166.2381517006802</v>
+      </c>
+      <c r="C5" s="13">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D5" s="16">
+        <f t="shared" si="0"/>
+        <v>2.5872965139833468</v>
+      </c>
+      <c r="E5" s="9">
+        <f t="shared" si="1"/>
+        <v>6.6941032512703789</v>
+      </c>
+      <c r="G5">
+        <f>G4/L5</f>
+        <v>4.3847007068309107E-3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" t="s">
+        <v>146</v>
+      </c>
+      <c r="L5" s="11">
+        <f>AVERAGE(B2:B4)</f>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="M5" s="12">
+        <v>27.53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="13">
+        <v>2173.7653715220299</v>
+      </c>
+      <c r="C6" s="13">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D6" s="16">
+        <f t="shared" si="0"/>
+        <v>10.114516335333064</v>
+      </c>
+      <c r="E6" s="9">
+        <f t="shared" si="1"/>
+        <v>102.30344069771941</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" s="13">
+        <v>2192.0776138154802</v>
+      </c>
+      <c r="C7" s="13">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D7" s="17">
+        <f t="shared" si="0"/>
+        <v>28.426758628783318</v>
+      </c>
+      <c r="E7" s="9">
+        <f t="shared" si="1"/>
+        <v>808.08060613910686</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="11">
+        <v>2156.3511491220902</v>
+      </c>
+      <c r="C8" s="11">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D8" s="36">
+        <f t="shared" si="0"/>
+        <v>-7.2997060646066529</v>
+      </c>
+      <c r="E8" s="37">
+        <f t="shared" si="1"/>
+        <v>53.285708629655147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9" s="11">
+        <v>2167.2565757031798</v>
+      </c>
+      <c r="C9" s="11">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D9" s="36">
+        <f t="shared" si="0"/>
+        <v>3.6057205164829611</v>
+      </c>
+      <c r="E9" s="37">
+        <f t="shared" si="1"/>
+        <v>13.001220442986153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>164</v>
+      </c>
+      <c r="B10" s="11">
+        <v>2161.00065386292</v>
+      </c>
+      <c r="C10" s="11">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D10" s="36">
+        <f t="shared" si="0"/>
+        <v>-2.6502013237768551</v>
+      </c>
+      <c r="E10" s="37">
+        <f t="shared" si="1"/>
+        <v>7.023567056548595</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11" s="11">
+        <v>2173.0418402661999</v>
+      </c>
+      <c r="C11" s="11">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D11" s="36">
+        <f t="shared" si="0"/>
+        <v>9.3909850795030252</v>
+      </c>
+      <c r="E11" s="37">
+        <f t="shared" si="1"/>
+        <v>88.190600763448444</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B12" s="11">
+        <v>2182.96053312513</v>
+      </c>
+      <c r="C12" s="11">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D12" s="36">
+        <f t="shared" si="0"/>
+        <v>19.309677938433197</v>
+      </c>
+      <c r="E12" s="37">
+        <f t="shared" si="1"/>
+        <v>372.86366208601373</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" s="11">
+        <v>2181.0465259029402</v>
+      </c>
+      <c r="C13" s="11">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D13" s="36">
+        <f t="shared" si="0"/>
+        <v>17.39567071624333</v>
+      </c>
+      <c r="E13" s="37">
+        <f t="shared" si="1"/>
+        <v>302.60935966796575</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B14" s="13">
+        <v>2172.5331075479398</v>
+      </c>
+      <c r="C14" s="13">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D14" s="16">
+        <f t="shared" si="0"/>
+        <v>8.8822523612429904</v>
+      </c>
+      <c r="E14" s="9">
+        <f t="shared" si="1"/>
+        <v>78.894407008806681</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B15" s="13">
+        <v>2169.1762594246602</v>
+      </c>
+      <c r="C15" s="13">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D15" s="16">
+        <f t="shared" si="0"/>
+        <v>5.5254042379633574</v>
+      </c>
+      <c r="E15" s="9">
+        <f t="shared" si="1"/>
+        <v>30.530091992903429</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B16" s="13">
+        <v>2166.36111516346</v>
+      </c>
+      <c r="C16" s="13">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D16" s="16">
+        <f t="shared" si="0"/>
+        <v>2.7102599767631546</v>
+      </c>
+      <c r="E16" s="9">
+        <f t="shared" si="1"/>
+        <v>7.3455091416442153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B17" s="13">
+        <v>2170.5505854027001</v>
+      </c>
+      <c r="C17" s="13">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D17" s="16">
+        <f t="shared" si="0"/>
+        <v>6.8997302160032632</v>
+      </c>
+      <c r="E17" s="9">
+        <f t="shared" si="1"/>
+        <v>47.606277053628439</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B18" s="13">
+        <v>2168.9045087064201</v>
+      </c>
+      <c r="C18" s="13">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D18" s="16">
+        <f t="shared" si="0"/>
+        <v>5.2536535197232297</v>
+      </c>
+      <c r="E18" s="9">
+        <f t="shared" si="1"/>
+        <v>27.600875305300281</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B19" s="13">
+        <v>2162.9155700415799</v>
+      </c>
+      <c r="C19" s="13">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D19" s="16">
+        <f t="shared" si="0"/>
+        <v>-0.73528514511690446</v>
+      </c>
+      <c r="E19" s="9">
+        <f t="shared" si="1"/>
+        <v>0.54064424462958727</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>186</v>
+      </c>
+      <c r="B20" s="11">
+        <v>2171.6037363503101</v>
+      </c>
+      <c r="C20" s="11">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D20" s="36">
+        <f t="shared" si="0"/>
+        <v>7.9528811636132559</v>
+      </c>
+      <c r="E20" s="37">
+        <f t="shared" si="1"/>
+        <v>63.248318802554536</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>187</v>
+      </c>
+      <c r="B21" s="11">
+        <v>2168.3325368241499</v>
+      </c>
+      <c r="C21" s="11">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D21" s="36">
+        <f t="shared" si="0"/>
+        <v>4.681681637453039</v>
+      </c>
+      <c r="E21" s="37">
+        <f t="shared" si="1"/>
+        <v>21.918142954464969</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>188</v>
+      </c>
+      <c r="B22" s="11">
+        <v>2169.6806683425698</v>
+      </c>
+      <c r="C22" s="11">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D22" s="36">
+        <f t="shared" si="0"/>
+        <v>6.0298131558729438</v>
+      </c>
+      <c r="E22" s="37">
+        <f t="shared" si="1"/>
+        <v>36.358646694738432</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>198</v>
+      </c>
+      <c r="B23" s="11">
+        <v>2172.39686499658</v>
+      </c>
+      <c r="C23" s="11">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D23" s="36">
+        <f t="shared" si="0"/>
+        <v>8.7460098098831622</v>
+      </c>
+      <c r="E23" s="37">
+        <f t="shared" si="1"/>
+        <v>76.492687594572502</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>199</v>
+      </c>
+      <c r="B24" s="11">
+        <v>2167.4396622854201</v>
+      </c>
+      <c r="C24" s="11">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D24" s="36">
+        <f t="shared" si="0"/>
+        <v>3.7888070987232823</v>
+      </c>
+      <c r="E24" s="37">
+        <f t="shared" si="1"/>
+        <v>14.355059231335936</v>
+      </c>
+      <c r="G24" t="s">
+        <v>229</v>
+      </c>
+      <c r="H24" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>200</v>
+      </c>
+      <c r="B25" s="11">
+        <v>2171.8155899193498</v>
+      </c>
+      <c r="C25" s="11">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D25" s="36">
+        <f t="shared" si="0"/>
+        <v>8.1647347326529598</v>
+      </c>
+      <c r="E25" s="37">
+        <f t="shared" si="1"/>
+        <v>66.662893254589605</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>226</v>
+      </c>
+      <c r="B26" s="11">
+        <v>2167.3314732691902</v>
+      </c>
+      <c r="C26" s="11">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D26" s="36">
+        <f t="shared" si="0"/>
+        <v>3.6806180824933108</v>
+      </c>
+      <c r="E26" s="37">
+        <f t="shared" si="1"/>
+        <v>13.546949469176736</v>
+      </c>
+      <c r="G26">
+        <f>SQRT(SUM(E26:E28)/ROWS(E26:E28))</f>
+        <v>2.3195793137114444</v>
+      </c>
+      <c r="H26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>227</v>
+      </c>
+      <c r="B27" s="11">
+        <v>2162.0931306789098</v>
+      </c>
+      <c r="C27" s="11">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D27" s="36">
+        <f t="shared" si="0"/>
+        <v>-1.557724507787043</v>
+      </c>
+      <c r="E27" s="37">
+        <f t="shared" si="1"/>
+        <v>2.4265056421603854</v>
+      </c>
+      <c r="G27">
+        <v>0.53</v>
+      </c>
+      <c r="H27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>228</v>
+      </c>
+      <c r="B28" s="11">
+        <v>2163.2411120153602</v>
+      </c>
+      <c r="C28" s="11">
+        <f t="shared" si="2"/>
+        <v>2163.6508551866968</v>
+      </c>
+      <c r="D28" s="36">
+        <f t="shared" si="0"/>
+        <v>-0.40974317133668592</v>
+      </c>
+      <c r="E28" s="37">
+        <f t="shared" si="1"/>
+        <v>0.16788946645704475</v>
+      </c>
+      <c r="G28">
+        <f>SQRT(G26^2+G27^2)</f>
+        <v>2.3793587776117446</v>
+      </c>
+      <c r="H28" t="s">
+        <v>32</v>
+      </c>
+      <c r="I28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G29">
+        <f>G28/L5</f>
+        <v>1.0996962711927174E-3</v>
+      </c>
+      <c r="H29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Uploaded the most recent data from the last alkalinity standard run. As well as the training session with MJ.
I double checked to see if the same min/max issue was happening in the alkalinity data file and I found no issues.

Most of the data looked pretty good. The first replicate of the Dickson standard was a bit off so I decided to exclude that and use the second two replicates.
</commit_message>
<xml_diff>
--- a/check sample work/TA QAQC/20201110 results summary both probes.xlsx
+++ b/check sample work/TA QAQC/20201110 results summary both probes.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\915712257\Documents\R\rye-tech-sfsu\2021-season-summary\check sample work\TA QAQC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rye-Tech\Documents\R\rye-tech-home\2021-season-summary\check sample work\TA QAQC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152E138B-6AE8-4BD5-92C8-BFDC1667FFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11316" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="example to follow" sheetId="1" r:id="rId1"/>
@@ -19,25 +20,17 @@
     <sheet name="QAQC baystds assessment" sheetId="5" r:id="rId5"/>
     <sheet name="Bay Std second look" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="246">
   <si>
     <t>sample</t>
   </si>
@@ -727,12 +720,60 @@
   </si>
   <si>
     <t>baystd1</t>
+  </si>
+  <si>
+    <t>P-0084-1</t>
+  </si>
+  <si>
+    <t>P-0084-2</t>
+  </si>
+  <si>
+    <t>BAYSTD1-04072021</t>
+  </si>
+  <si>
+    <t>SAC-3</t>
+  </si>
+  <si>
+    <t>DIC-CRM186-04272021-1</t>
+  </si>
+  <si>
+    <t>DIC-CRM186-04272021-2</t>
+  </si>
+  <si>
+    <t>DIC-CRM186-04272021-3</t>
+  </si>
+  <si>
+    <t>BAYSTD1-04272021-1</t>
+  </si>
+  <si>
+    <t>BAYSTD1-04272021-2</t>
+  </si>
+  <si>
+    <t>BAYSTD1-04272021-3</t>
+  </si>
+  <si>
+    <t>BAYSTD2-04272021-1</t>
+  </si>
+  <si>
+    <t>BAYSTD2-04272021-2</t>
+  </si>
+  <si>
+    <t>BAYSTD2-04272021-3</t>
+  </si>
+  <si>
+    <t>not sure what happened here, might be worth excluding</t>
+  </si>
+  <si>
+    <t>BayStd2</t>
+  </si>
+  <si>
+    <t>using only two values in the calulations to the right</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -1514,27 +1555,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1"/>
-    <col min="13" max="13" width="51.109375" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="13" max="13" width="51.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1572,7 +1613,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1586,7 +1627,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1597,7 +1638,7 @@
         <v>2247.5363699999998</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1641,7 +1682,7 @@
       </c>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1652,7 +1693,7 @@
         <v>2114.1481899999999</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1663,7 +1704,7 @@
         <v>2138.9193500000001</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1707,7 +1748,7 @@
       </c>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1718,7 +1759,7 @@
         <v>2135.2389699999999</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1729,7 +1770,7 @@
         <v>2133.48756</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1773,7 +1814,7 @@
       </c>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1784,7 +1825,7 @@
         <v>2124.9360900000001</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1795,7 +1836,7 @@
         <v>2132.3921700000001</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1839,7 +1880,7 @@
       </c>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1850,7 +1891,7 @@
         <v>2249.3508299999999</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1861,7 +1902,7 @@
         <v>2250.2915600000001</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1908,10 +1949,10 @@
       </c>
       <c r="M16" s="3"/>
     </row>
-    <row r="20" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:14" x14ac:dyDescent="0.25">
       <c r="N20" s="4"/>
     </row>
-    <row r="21" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>34</v>
       </c>
@@ -1922,7 +1963,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E22">
         <f>2238.04</f>
         <v>2238.04</v>
@@ -1936,7 +1977,7 @@
         <v>21.704231088401922</v>
       </c>
     </row>
-    <row r="23" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E23">
         <f t="shared" ref="E23:E26" si="0">2238.04</f>
         <v>2238.04</v>
@@ -1950,7 +1991,7 @@
         <v>90.181043176897006</v>
       </c>
     </row>
-    <row r="24" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E24">
         <f t="shared" si="0"/>
         <v>2238.04</v>
@@ -1964,7 +2005,7 @@
         <v>62.986127504401573</v>
       </c>
     </row>
-    <row r="25" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E25">
         <f>2238.04</f>
         <v>2238.04</v>
@@ -1978,7 +2019,7 @@
         <v>127.93487528889766</v>
       </c>
     </row>
-    <row r="26" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E26">
         <f t="shared" si="0"/>
         <v>2238.04</v>
@@ -1992,7 +2033,7 @@
         <v>150.10072243360378</v>
       </c>
     </row>
-    <row r="29" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:14" x14ac:dyDescent="0.25">
       <c r="G29">
         <f>SQRT(SUM(G22:G26)/5)</f>
         <v>9.5174261173092578</v>
@@ -2001,7 +2042,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:14" x14ac:dyDescent="0.25">
       <c r="F30" s="3"/>
       <c r="G30">
         <v>0.53</v>
@@ -2010,7 +2051,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:14" x14ac:dyDescent="0.25">
       <c r="G31">
         <f>SQRT(G29^2+G30^2)</f>
         <v>9.5321718353395397</v>
@@ -2022,7 +2063,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="5:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:14" x14ac:dyDescent="0.25">
       <c r="G32">
         <f>G31/E26</f>
         <v>4.2591606206053246E-3</v>
@@ -2034,12 +2075,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:13" x14ac:dyDescent="0.25">
       <c r="M36" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="4:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:13" ht="45" x14ac:dyDescent="0.25">
       <c r="D37" s="1" t="s">
         <v>38</v>
       </c>
@@ -2051,30 +2092,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M189"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M206"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A186" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D199" sqref="D199"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" style="18" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" style="18" customWidth="1"/>
     <col min="5" max="5" width="10" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.109375" style="19"/>
+    <col min="6" max="7" width="9.140625" style="19"/>
     <col min="8" max="8" width="13" style="19" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" style="41"/>
-    <col min="10" max="10" width="11.44140625" style="19" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" style="19"/>
-    <col min="13" max="13" width="51.109375" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="41"/>
+    <col min="10" max="10" width="11.42578125" style="19" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" style="19"/>
+    <col min="13" max="13" width="51.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -2112,7 +2153,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>40</v>
       </c>
@@ -2134,7 +2175,7 @@
       <c r="K2" s="21"/>
       <c r="L2" s="21"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>41</v>
       </c>
@@ -2154,7 +2195,7 @@
       <c r="K3" s="21"/>
       <c r="L3" s="21"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>42</v>
       </c>
@@ -2199,7 +2240,7 @@
       </c>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>6</v>
       </c>
@@ -2219,7 +2260,7 @@
       <c r="K5" s="21"/>
       <c r="L5" s="21"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>7</v>
       </c>
@@ -2239,7 +2280,7 @@
       <c r="K6" s="21"/>
       <c r="L6" s="21"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>8</v>
       </c>
@@ -2284,7 +2325,7 @@
       </c>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>9</v>
       </c>
@@ -2304,7 +2345,7 @@
       <c r="K8" s="21"/>
       <c r="L8" s="21"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>10</v>
       </c>
@@ -2324,7 +2365,7 @@
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>11</v>
       </c>
@@ -2369,7 +2410,7 @@
       </c>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>12</v>
       </c>
@@ -2389,7 +2430,7 @@
       <c r="K11" s="21"/>
       <c r="L11" s="21"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>13</v>
       </c>
@@ -2409,7 +2450,7 @@
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>14</v>
       </c>
@@ -2454,7 +2495,7 @@
       </c>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>43</v>
       </c>
@@ -2474,7 +2515,7 @@
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>44</v>
       </c>
@@ -2494,7 +2535,7 @@
       <c r="K15" s="21"/>
       <c r="L15" s="21"/>
     </row>
-    <row r="16" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>45</v>
       </c>
@@ -2541,7 +2582,7 @@
       </c>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
         <v>54</v>
       </c>
@@ -2559,7 +2600,7 @@
       <c r="I17" s="33"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>56</v>
       </c>
@@ -2603,7 +2644,7 @@
       </c>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>48</v>
       </c>
@@ -2617,7 +2658,7 @@
       <c r="I19" s="33"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>49</v>
       </c>
@@ -2631,7 +2672,7 @@
       <c r="I20" s="33"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>50</v>
       </c>
@@ -2672,7 +2713,7 @@
       </c>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>51</v>
       </c>
@@ -2686,7 +2727,7 @@
       <c r="I22" s="33"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>52</v>
       </c>
@@ -2700,7 +2741,7 @@
       <c r="I23" s="33"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>53</v>
       </c>
@@ -2741,7 +2782,7 @@
       </c>
       <c r="M24" s="3"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>55</v>
       </c>
@@ -2749,7 +2790,7 @@
         <v>2278.2465769999999</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>57</v>
       </c>
@@ -2789,7 +2830,7 @@
         <v>4.9946979999999712</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
         <v>65</v>
       </c>
@@ -2807,7 +2848,7 @@
       <c r="K27" s="21"/>
       <c r="L27" s="21"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
         <v>108</v>
       </c>
@@ -2825,7 +2866,7 @@
       <c r="K28" s="21"/>
       <c r="L28" s="21"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
         <v>109</v>
       </c>
@@ -2867,7 +2908,7 @@
         <v>202.47002357553993</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
         <v>66</v>
       </c>
@@ -2885,7 +2926,7 @@
       <c r="K30" s="21"/>
       <c r="L30" s="21"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
         <v>67</v>
       </c>
@@ -2903,7 +2944,7 @@
       <c r="K31" s="21"/>
       <c r="L31" s="21"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
         <v>68</v>
       </c>
@@ -2945,7 +2986,7 @@
         <v>8.0012203823998789</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
         <v>69</v>
       </c>
@@ -2963,7 +3004,7 @@
       <c r="K33" s="21"/>
       <c r="L33" s="21"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
         <v>70</v>
       </c>
@@ -2981,7 +3022,7 @@
       <c r="K34" s="21"/>
       <c r="L34" s="21"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
         <v>71</v>
       </c>
@@ -3023,7 +3064,7 @@
         <v>9.1970026297599361</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
         <v>110</v>
       </c>
@@ -3041,7 +3082,7 @@
       <c r="K36" s="21"/>
       <c r="L36" s="21"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
         <v>111</v>
       </c>
@@ -3083,7 +3124,7 @@
         <v>8.9153114503401412</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>65</v>
       </c>
@@ -3091,7 +3132,7 @@
         <v>1624.2912168376199</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
         <v>112</v>
       </c>
@@ -3099,7 +3140,7 @@
         <v>2241.6865483083102</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>113</v>
       </c>
@@ -3139,7 +3180,7 @@
         <v>0.14446479651041955</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>72</v>
       </c>
@@ -3147,7 +3188,7 @@
         <v>2125.89715188732</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
         <v>73</v>
       </c>
@@ -3155,7 +3196,7 @@
         <v>2109.3231506451998</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>74</v>
       </c>
@@ -3195,7 +3236,7 @@
         <v>16.574001242120175</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
         <v>75</v>
       </c>
@@ -3203,7 +3244,7 @@
         <v>2122.2192108210402</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>76</v>
       </c>
@@ -3211,7 +3252,7 @@
         <v>2123.5923451169101</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
         <v>77</v>
       </c>
@@ -3251,7 +3292,7 @@
         <v>12.418599309430192</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>114</v>
       </c>
@@ -3259,7 +3300,7 @@
         <v>2236.1095817401701</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
         <v>115</v>
       </c>
@@ -3299,7 +3340,7 @@
         <v>0.92449238705012249</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="21" t="s">
         <v>65</v>
       </c>
@@ -3317,7 +3358,7 @@
       <c r="K49" s="21"/>
       <c r="L49" s="21"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="21" t="s">
         <v>116</v>
       </c>
@@ -3335,7 +3376,7 @@
       <c r="K50" s="21"/>
       <c r="L50" s="21"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="21" t="s">
         <v>117</v>
       </c>
@@ -3377,7 +3418,7 @@
         <v>0.62477194547000181</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
         <v>78</v>
       </c>
@@ -3395,7 +3436,7 @@
       <c r="K52" s="21"/>
       <c r="L52" s="21"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="21" t="s">
         <v>79</v>
       </c>
@@ -3413,7 +3454,7 @@
       <c r="K53" s="21"/>
       <c r="L53" s="21"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="21" t="s">
         <v>80</v>
       </c>
@@ -3455,7 +3496,7 @@
         <v>3.6758375283698115</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="21" t="s">
         <v>81</v>
       </c>
@@ -3473,7 +3514,7 @@
       <c r="K55" s="21"/>
       <c r="L55" s="21"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="21" t="s">
         <v>82</v>
       </c>
@@ -3491,7 +3532,7 @@
       <c r="K56" s="21"/>
       <c r="L56" s="21"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="21" t="s">
         <v>83</v>
       </c>
@@ -3533,7 +3574,7 @@
         <v>4.6240391373403327</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
         <v>84</v>
       </c>
@@ -3551,7 +3592,7 @@
       <c r="K58" s="21"/>
       <c r="L58" s="21"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="21" t="s">
         <v>85</v>
       </c>
@@ -3569,7 +3610,7 @@
       <c r="K59" s="21"/>
       <c r="L59" s="21"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="21" t="s">
         <v>86</v>
       </c>
@@ -3611,7 +3652,7 @@
         <v>0.46416779767014305</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="21" t="s">
         <v>118</v>
       </c>
@@ -3629,7 +3670,7 @@
       <c r="K61" s="21"/>
       <c r="L61" s="21"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="21" t="s">
         <v>119</v>
       </c>
@@ -3671,7 +3712,7 @@
         <v>0.88344358794984146</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="19" t="s">
         <v>65</v>
       </c>
@@ -3679,7 +3720,7 @@
         <v>1592.1393647914399</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="19" t="s">
         <v>120</v>
       </c>
@@ -3687,7 +3728,7 @@
         <v>2247.3720067191798</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="19" t="s">
         <v>121</v>
       </c>
@@ -3727,7 +3768,7 @@
         <v>2.4952530231798846</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="19" t="s">
         <v>87</v>
       </c>
@@ -3735,7 +3776,7 @@
         <v>2234.7435887859501</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="19" t="s">
         <v>88</v>
       </c>
@@ -3743,7 +3784,7 @@
         <v>2227.2541142131499</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="19" t="s">
         <v>89</v>
       </c>
@@ -3783,7 +3824,7 @@
         <v>10.515290785639991</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="19" t="s">
         <v>90</v>
       </c>
@@ -3791,7 +3832,7 @@
         <v>2233.5328075264601</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="19" t="s">
         <v>91</v>
       </c>
@@ -3799,7 +3840,7 @@
         <v>2235.2718356786399</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="19" t="s">
         <v>92</v>
       </c>
@@ -3839,7 +3880,7 @@
         <v>5.2933858786800556</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="19" t="s">
         <v>93</v>
       </c>
@@ -3847,7 +3888,7 @@
         <v>2231.41222642809</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="19" t="s">
         <v>94</v>
       </c>
@@ -3855,7 +3896,7 @@
         <v>2218.87534925306</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="19" t="s">
         <v>95</v>
       </c>
@@ -3895,7 +3936,7 @@
         <v>12.536877175029986</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="19" t="s">
         <v>122</v>
       </c>
@@ -3903,7 +3944,7 @@
         <v>2241.6593895374199</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="19" t="s">
         <v>123</v>
       </c>
@@ -3943,7 +3984,7 @@
         <v>2.5427539370703016</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="21" t="s">
         <v>65</v>
       </c>
@@ -3961,7 +4002,7 @@
       <c r="K77" s="21"/>
       <c r="L77" s="21"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="21" t="s">
         <v>124</v>
       </c>
@@ -3979,7 +4020,7 @@
       <c r="K78" s="21"/>
       <c r="L78" s="21"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="21" t="s">
         <v>125</v>
       </c>
@@ -4021,7 +4062,7 @@
         <v>19.982069738440259</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="34" t="s">
         <v>128</v>
       </c>
@@ -4041,7 +4082,7 @@
       <c r="K80" s="34"/>
       <c r="L80" s="34"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="34" t="s">
         <v>130</v>
       </c>
@@ -4061,7 +4102,7 @@
       <c r="K81" s="34"/>
       <c r="L81" s="34"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="34" t="s">
         <v>131</v>
       </c>
@@ -4105,7 +4146,7 @@
         <v>9.7230443598400598</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="21" t="s">
         <v>126</v>
       </c>
@@ -4123,7 +4164,7 @@
       <c r="K83" s="21"/>
       <c r="L83" s="21"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="21" t="s">
         <v>127</v>
       </c>
@@ -4165,7 +4206,7 @@
         <v>3.114767579850195</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="19" t="s">
         <v>65</v>
       </c>
@@ -4173,7 +4214,7 @@
         <v>1767.4127862110699</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="30" t="s">
         <v>132</v>
       </c>
@@ -4183,7 +4224,7 @@
       <c r="C86" s="30"/>
       <c r="D86" s="31"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="19" t="s">
         <v>133</v>
       </c>
@@ -4223,7 +4264,7 @@
         <v>200.93180595105991</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="19" t="s">
         <v>136</v>
       </c>
@@ -4231,7 +4272,7 @@
         <v>2223.7491846081298</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="19" t="s">
         <v>137</v>
       </c>
@@ -4271,7 +4312,7 @@
         <v>4.2857932929500748</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="19" t="s">
         <v>96</v>
       </c>
@@ -4279,7 +4320,7 @@
         <v>2176.50294375658</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="19" t="s">
         <v>97</v>
       </c>
@@ -4287,7 +4328,7 @@
         <v>2186.08511792934</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="19" t="s">
         <v>98</v>
       </c>
@@ -4327,7 +4368,7 @@
         <v>35.996994867829926</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="19" t="s">
         <v>99</v>
       </c>
@@ -4335,7 +4376,7 @@
         <v>2103.7936989664699</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="19" t="s">
         <v>100</v>
       </c>
@@ -4343,7 +4384,7 @@
         <v>2076.5450829193901</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="19" t="s">
         <v>101</v>
       </c>
@@ -4383,7 +4424,7 @@
         <v>27.24861604707985</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="19" t="s">
         <v>134</v>
       </c>
@@ -4391,7 +4432,7 @@
         <v>2157.74591479522</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="19" t="s">
         <v>135</v>
       </c>
@@ -4431,7 +4472,7 @@
         <v>16.870894775150191</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="21" t="s">
         <v>65</v>
       </c>
@@ -4449,7 +4490,7 @@
       <c r="K98" s="21"/>
       <c r="L98" s="21"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="21" t="s">
         <v>139</v>
       </c>
@@ -4467,7 +4508,7 @@
       <c r="K99" s="21"/>
       <c r="L99" s="21"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="21" t="s">
         <v>140</v>
       </c>
@@ -4509,7 +4550,7 @@
         <v>7.5272198213497177</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="21" t="s">
         <v>138</v>
       </c>
@@ -4527,7 +4568,7 @@
       <c r="K101" s="21"/>
       <c r="L101" s="21"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="21" t="s">
         <v>102</v>
       </c>
@@ -4545,7 +4586,7 @@
       <c r="K102" s="21"/>
       <c r="L102" s="21"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="21" t="s">
         <v>103</v>
       </c>
@@ -4563,7 +4604,7 @@
       <c r="K103" s="21"/>
       <c r="L103" s="21"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="21" t="s">
         <v>104</v>
       </c>
@@ -4605,7 +4646,7 @@
         <v>7.1066143973698672</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="21" t="s">
         <v>105</v>
       </c>
@@ -4623,7 +4664,7 @@
       <c r="K105" s="21"/>
       <c r="L105" s="21"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="21" t="s">
         <v>106</v>
       </c>
@@ -4641,7 +4682,7 @@
       <c r="K106" s="21"/>
       <c r="L106" s="21"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="21" t="s">
         <v>107</v>
       </c>
@@ -4683,7 +4724,7 @@
         <v>12.227740629090022</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="21" t="s">
         <v>141</v>
       </c>
@@ -4701,7 +4742,7 @@
       <c r="K108" s="21"/>
       <c r="L108" s="21"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="21" t="s">
         <v>142</v>
       </c>
@@ -4743,7 +4784,7 @@
         <v>104.21104304512983</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="19" t="s">
         <v>65</v>
       </c>
@@ -4751,7 +4792,7 @@
         <v>1712.82598863931</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="19" t="s">
         <v>162</v>
       </c>
@@ -4759,7 +4800,7 @@
         <v>2156.3511491220902</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="19" t="s">
         <v>163</v>
       </c>
@@ -4767,7 +4808,7 @@
         <v>2167.2565757031798</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="19" t="s">
         <v>164</v>
       </c>
@@ -4807,7 +4848,7 @@
         <v>10.905426581089614</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="19" t="s">
         <v>153</v>
       </c>
@@ -4815,7 +4856,7 @@
         <v>2095.24484288339</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="19" t="s">
         <v>154</v>
       </c>
@@ -4823,7 +4864,7 @@
         <v>2100.3120996130501</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="19" t="s">
         <v>155</v>
       </c>
@@ -4863,7 +4904,7 @@
         <v>10.806316414660159</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="19" t="s">
         <v>156</v>
       </c>
@@ -4871,7 +4912,7 @@
         <v>2218.8993800551598</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="19" t="s">
         <v>157</v>
       </c>
@@ -4879,7 +4920,7 @@
         <v>2186.6045565018098</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="19" t="s">
         <v>158</v>
       </c>
@@ -4919,7 +4960,7 @@
         <v>32.294823553349943</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="19" t="s">
         <v>159</v>
       </c>
@@ -4927,7 +4968,7 @@
         <v>2186.45070089</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="19" t="s">
         <v>160</v>
       </c>
@@ -4935,7 +4976,7 @@
         <v>2194.8913127686101</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="19" t="s">
         <v>161</v>
       </c>
@@ -4975,7 +5016,7 @@
         <v>8.4406118786100706</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="19" t="s">
         <v>165</v>
       </c>
@@ -4983,7 +5024,7 @@
         <v>2173.0418402661999</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="19" t="s">
         <v>166</v>
       </c>
@@ -4991,7 +5032,7 @@
         <v>2182.96053312513</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="19" t="s">
         <v>167</v>
       </c>
@@ -5031,7 +5072,7 @@
         <v>9.9186928589301715</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="19" t="s">
         <v>168</v>
       </c>
@@ -5039,7 +5080,7 @@
         <v>2232.7275708530301</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="19" t="s">
         <v>169</v>
       </c>
@@ -5047,7 +5088,7 @@
         <v>2225.3939498013601</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="19" t="s">
         <v>170</v>
       </c>
@@ -5087,7 +5128,7 @@
         <v>8.6111939932702626</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="21" t="s">
         <v>65</v>
       </c>
@@ -5105,7 +5146,7 @@
       <c r="K129" s="21"/>
       <c r="L129" s="21"/>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="21" t="s">
         <v>171</v>
       </c>
@@ -5123,7 +5164,7 @@
       <c r="K130" s="21"/>
       <c r="L130" s="21"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="21" t="s">
         <v>172</v>
       </c>
@@ -5141,7 +5182,7 @@
       <c r="K131" s="21"/>
       <c r="L131" s="21"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="21" t="s">
         <v>173</v>
       </c>
@@ -5183,7 +5224,7 @@
         <v>6.1719923844798359</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="21" t="s">
         <v>174</v>
       </c>
@@ -5201,7 +5242,7 @@
       <c r="K133" s="21"/>
       <c r="L133" s="21"/>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="21" t="s">
         <v>175</v>
       </c>
@@ -5219,7 +5260,7 @@
       <c r="K134" s="21"/>
       <c r="L134" s="21"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="21" t="s">
         <v>176</v>
       </c>
@@ -5261,7 +5302,7 @@
         <v>3.7418551294699682</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="21" t="s">
         <v>177</v>
       </c>
@@ -5279,7 +5320,7 @@
       <c r="K136" s="21"/>
       <c r="L136" s="21"/>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="21" t="s">
         <v>178</v>
       </c>
@@ -5297,7 +5338,7 @@
       <c r="K137" s="21"/>
       <c r="L137" s="21"/>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="21" t="s">
         <v>179</v>
       </c>
@@ -5339,7 +5380,7 @@
         <v>99.351645211729647</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="21" t="s">
         <v>180</v>
       </c>
@@ -5357,7 +5398,7 @@
       <c r="K139" s="21"/>
       <c r="L139" s="21"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="21" t="s">
         <v>181</v>
       </c>
@@ -5375,7 +5416,7 @@
       <c r="K140" s="21"/>
       <c r="L140" s="21"/>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="21" t="s">
         <v>182</v>
       </c>
@@ -5417,7 +5458,7 @@
         <v>7.6350153611201677</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="21" t="s">
         <v>183</v>
       </c>
@@ -5435,7 +5476,7 @@
       <c r="K142" s="21"/>
       <c r="L142" s="21"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="21" t="s">
         <v>184</v>
       </c>
@@ -5453,7 +5494,7 @@
       <c r="K143" s="21"/>
       <c r="L143" s="21"/>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" s="21" t="s">
         <v>185</v>
       </c>
@@ -5495,7 +5536,7 @@
         <v>5.9110954046300321</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" s="19" t="s">
         <v>65</v>
       </c>
@@ -5503,7 +5544,7 @@
         <v>1732.26717091612</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="19" t="s">
         <v>186</v>
       </c>
@@ -5511,7 +5552,7 @@
         <v>2171.6037363503101</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="19" t="s">
         <v>187</v>
       </c>
@@ -5519,7 +5560,7 @@
         <v>2168.3325368241499</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="19" t="s">
         <v>188</v>
       </c>
@@ -5559,7 +5600,7 @@
         <v>3.2711995261602169</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="19" t="s">
         <v>189</v>
       </c>
@@ -5567,7 +5608,7 @@
         <v>2205.29339655284</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="19" t="s">
         <v>190</v>
       </c>
@@ -5575,7 +5616,7 @@
         <v>2203.5715719336199</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" s="19" t="s">
         <v>191</v>
       </c>
@@ -5615,7 +5656,7 @@
         <v>1.721824619220115</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" s="19" t="s">
         <v>192</v>
       </c>
@@ -5623,7 +5664,7 @@
         <v>2209.2654099239599</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" s="19" t="s">
         <v>193</v>
       </c>
@@ -5631,7 +5672,7 @@
         <v>2205.6468945710899</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" s="19" t="s">
         <v>194</v>
       </c>
@@ -5671,7 +5712,7 @@
         <v>3.618515352869963</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" s="19" t="s">
         <v>195</v>
       </c>
@@ -5679,7 +5720,7 @@
         <v>2201.95312729751</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" s="19" t="s">
         <v>196</v>
       </c>
@@ -5687,7 +5728,7 @@
         <v>2201.7544015737499</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" s="19" t="s">
         <v>197</v>
       </c>
@@ -5727,7 +5768,7 @@
         <v>5.0274952043100711</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" s="19" t="s">
         <v>198</v>
       </c>
@@ -5735,7 +5776,7 @@
         <v>2172.39686499658</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" s="19" t="s">
         <v>199</v>
       </c>
@@ -5743,7 +5784,7 @@
         <v>2167.4396622854201</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160" s="19" t="s">
         <v>200</v>
       </c>
@@ -5783,7 +5824,7 @@
         <v>4.95720271115988</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A161" s="19" t="s">
         <v>201</v>
       </c>
@@ -5791,7 +5832,7 @@
         <v>2234.9084845810298</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A162" s="19" t="s">
         <v>202</v>
       </c>
@@ -5799,7 +5840,7 @@
         <v>2233.8319039288199</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A163" s="19" t="s">
         <v>203</v>
       </c>
@@ -5839,7 +5880,7 @@
         <v>2.9707386936402145</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A164" s="19" t="s">
         <v>215</v>
       </c>
@@ -5847,7 +5888,7 @@
         <v>2791.47452987631</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A165" s="19" t="s">
         <v>207</v>
       </c>
@@ -5855,7 +5896,7 @@
         <v>2253.5400879193598</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A166" s="19" t="s">
         <v>208</v>
       </c>
@@ -5863,7 +5904,7 @@
         <v>2250.3490168078902</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A167" s="19" t="s">
         <v>209</v>
       </c>
@@ -5871,7 +5912,7 @@
         <v>2261.73917919109</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A168" s="19" t="s">
         <v>210</v>
       </c>
@@ -5879,7 +5920,7 @@
         <v>2241.4624109891101</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A169" s="19" t="s">
         <v>211</v>
       </c>
@@ -5887,7 +5928,7 @@
         <v>2258.1304930768201</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A170" s="19" t="s">
         <v>212</v>
       </c>
@@ -5895,7 +5936,7 @@
         <v>2251.4238491137899</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A171" s="19" t="s">
         <v>213</v>
       </c>
@@ -5935,7 +5976,7 @@
         <v>20.276768201979849</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A172" s="19" t="s">
         <v>214</v>
       </c>
@@ -5943,7 +5984,7 @@
         <v>2424.3536009301201</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A173" s="19" t="s">
         <v>204</v>
       </c>
@@ -5951,7 +5992,7 @@
         <v>2220.1114998255798</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A174" s="19" t="s">
         <v>205</v>
       </c>
@@ -5959,7 +6000,7 @@
         <v>2223.29862647973</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A175" s="19" t="s">
         <v>206</v>
       </c>
@@ -5999,7 +6040,7 @@
         <v>5.3446747965799659</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A176" s="19" t="s">
         <v>215</v>
       </c>
@@ -6007,7 +6048,7 @@
         <v>2053.3155707137898</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A177" s="19" t="s">
         <v>217</v>
       </c>
@@ -6015,7 +6056,7 @@
         <v>2121.1126006919999</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A178" s="19" t="s">
         <v>218</v>
       </c>
@@ -6023,7 +6064,7 @@
         <v>2114.3140912812701</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A179" s="19" t="s">
         <v>219</v>
       </c>
@@ -6063,7 +6104,7 @@
         <v>16.851486293259768</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A180" s="19" t="s">
         <v>220</v>
       </c>
@@ -6071,7 +6112,7 @@
         <v>2136.7025174391802</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A181" s="19" t="s">
         <v>221</v>
       </c>
@@ -6079,7 +6120,7 @@
         <v>2137.4028738178399</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A182" s="19" t="s">
         <v>222</v>
       </c>
@@ -6119,7 +6160,7 @@
         <v>1.0440521757400347</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A183" s="19" t="s">
         <v>223</v>
       </c>
@@ -6127,7 +6168,7 @@
         <v>2112.5960733162501</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A184" s="19" t="s">
         <v>224</v>
       </c>
@@ -6135,7 +6176,7 @@
         <v>2105.44065001114</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A185" s="19" t="s">
         <v>225</v>
       </c>
@@ -6175,7 +6216,7 @@
         <v>10.104269404670049</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A186" s="19" t="s">
         <v>214</v>
       </c>
@@ -6183,7 +6224,7 @@
         <v>1798.38269926629</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A187" s="19" t="s">
         <v>226</v>
       </c>
@@ -6191,7 +6232,7 @@
         <v>2167.3314732691902</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A188" s="19" t="s">
         <v>227</v>
       </c>
@@ -6199,7 +6240,7 @@
         <v>2162.0931306789098</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A189" s="19" t="s">
         <v>228</v>
       </c>
@@ -6237,6 +6278,276 @@
       <c r="L189" s="19">
         <f>K189-J189</f>
         <v>5.2383425902803538</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A190" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="B190" s="19">
+        <v>2290.3416417366602</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A191" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="B191" s="19">
+        <v>2185.6742415221702</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A192" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="B192" s="19">
+        <v>2450.9836064696501</v>
+      </c>
+    </row>
+    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A193" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="B193" s="19">
+        <v>2203.76908601887</v>
+      </c>
+    </row>
+    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A194" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="B194" s="19">
+        <v>2339.16249328406</v>
+      </c>
+      <c r="E194" s="21">
+        <f>AVERAGE(B193:B194)</f>
+        <v>2271.465789651465</v>
+      </c>
+      <c r="F194" s="21">
+        <f>_xlfn.STDEV.S(B193:B194)</f>
+        <v>95.737596405167849</v>
+      </c>
+      <c r="G194" s="21">
+        <f>2*F194</f>
+        <v>191.4751928103357</v>
+      </c>
+      <c r="H194" s="21">
+        <f>F194/E194</f>
+        <v>4.2147936738179043E-2</v>
+      </c>
+      <c r="I194" s="42">
+        <f>H194</f>
+        <v>4.2147936738179043E-2</v>
+      </c>
+      <c r="J194" s="21">
+        <f>MIN(B193:B194)</f>
+        <v>2203.76908601887</v>
+      </c>
+      <c r="K194" s="21">
+        <f>MAX(B193:B194)</f>
+        <v>2339.16249328406</v>
+      </c>
+      <c r="L194" s="21">
+        <f>K194-J194</f>
+        <v>135.39340726519004</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A195" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="B195" s="19">
+        <v>2380.6235945409098</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A196" s="30" t="s">
+        <v>234</v>
+      </c>
+      <c r="B196" s="30">
+        <v>2250.7575623355901</v>
+      </c>
+      <c r="D196" s="18" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A197" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="B197" s="19">
+        <v>2203.22618654695</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A198" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="B198" s="19">
+        <v>2200.2796088885002</v>
+      </c>
+      <c r="D198" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="E198" s="21">
+        <f>AVERAGE(B197:B198)</f>
+        <v>2201.7528977177253</v>
+      </c>
+      <c r="F198" s="21">
+        <f>_xlfn.STDEV.S(B197:B198)</f>
+        <v>2.0835450435826104</v>
+      </c>
+      <c r="G198" s="21">
+        <f>2*F198</f>
+        <v>4.1670900871652208</v>
+      </c>
+      <c r="H198" s="21">
+        <f>F198/E198</f>
+        <v>9.4631193434211174E-4</v>
+      </c>
+      <c r="I198" s="42">
+        <f>H198</f>
+        <v>9.4631193434211174E-4</v>
+      </c>
+      <c r="J198" s="21">
+        <f>MIN(B197:B198)</f>
+        <v>2200.2796088885002</v>
+      </c>
+      <c r="K198" s="21">
+        <f>MAX(B197:B198)</f>
+        <v>2203.22618654695</v>
+      </c>
+      <c r="L198" s="21">
+        <f>K198-J198</f>
+        <v>2.9465776584497689</v>
+      </c>
+    </row>
+    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A199" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="B199" s="19">
+        <v>2398.0314183502901</v>
+      </c>
+    </row>
+    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A200" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="B200" s="19">
+        <v>2188.0548117417202</v>
+      </c>
+    </row>
+    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A201" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="B201" s="19">
+        <v>2182.1633268279402</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A202" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="B202" s="19">
+        <v>2179.9038352182201</v>
+      </c>
+      <c r="E202" s="19">
+        <f>AVERAGE(B200:B202)</f>
+        <v>2183.3739912626265</v>
+      </c>
+      <c r="F202" s="19">
+        <f>_xlfn.STDEV.S(B200:B202)</f>
+        <v>4.2081927061059838</v>
+      </c>
+      <c r="G202" s="19">
+        <f>2*F202</f>
+        <v>8.4163854122119677</v>
+      </c>
+      <c r="H202" s="19">
+        <f>F202/E202</f>
+        <v>1.9273806150234582E-3</v>
+      </c>
+      <c r="I202" s="41">
+        <f>H202</f>
+        <v>1.9273806150234582E-3</v>
+      </c>
+      <c r="J202" s="19">
+        <f>MIN(B200:B202)</f>
+        <v>2179.9038352182201</v>
+      </c>
+      <c r="K202" s="19">
+        <f>MAX(B200:B202)</f>
+        <v>2188.0548117417202</v>
+      </c>
+      <c r="L202" s="19">
+        <f>K202-J202</f>
+        <v>8.1509765235000486</v>
+      </c>
+    </row>
+    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A203" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="B203" s="19">
+        <v>2110.5869142463098</v>
+      </c>
+    </row>
+    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A204" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="B204" s="19">
+        <v>2253.49247123941</v>
+      </c>
+    </row>
+    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A205" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="B205" s="19">
+        <v>2256.3586638595498</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A206" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="B206" s="19">
+        <v>2252.4539135216601</v>
+      </c>
+      <c r="E206" s="19">
+        <f>AVERAGE(B204:B206)</f>
+        <v>2254.1016828735396</v>
+      </c>
+      <c r="F206" s="19">
+        <f>_xlfn.STDEV.S(B204:B206)</f>
+        <v>2.0224052293449852</v>
+      </c>
+      <c r="G206" s="19">
+        <f>2*F206</f>
+        <v>4.0448104586899705</v>
+      </c>
+      <c r="H206" s="19">
+        <f>F206/E206</f>
+        <v>8.9721117938513465E-4</v>
+      </c>
+      <c r="I206" s="41">
+        <f>H206</f>
+        <v>8.9721117938513465E-4</v>
+      </c>
+      <c r="J206" s="19">
+        <f>MIN(B204:B206)</f>
+        <v>2252.4539135216601</v>
+      </c>
+      <c r="K206" s="19">
+        <f>MAX(B204:B206)</f>
+        <v>2256.3586638595498</v>
+      </c>
+      <c r="L206" s="19">
+        <f>K206-J206</f>
+        <v>3.904750337889709</v>
       </c>
     </row>
   </sheetData>
@@ -6245,7 +6556,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M70"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -6253,25 +6564,25 @@
       <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="103" style="6" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" style="11" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="12" customWidth="1"/>
-    <col min="14" max="14" width="59.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" style="11" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="12" customWidth="1"/>
+    <col min="14" max="14" width="59.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -6302,7 +6613,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>40</v>
       </c>
@@ -6333,7 +6644,7 @@
         <v>33.311999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>41</v>
       </c>
@@ -6369,7 +6680,7 @@
         <v>33.661000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>42</v>
       </c>
@@ -6404,7 +6715,7 @@
         <v>33.524999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>43</v>
       </c>
@@ -6443,7 +6754,7 @@
         <v>27.53</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>44</v>
       </c>
@@ -6472,7 +6783,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -6492,7 +6803,7 @@
         <v>4.9540482249982379E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -6512,7 +6823,7 @@
         <v>1616.5688340569229</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -6532,7 +6843,7 @@
         <v>2043.1552616256156</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>108</v>
       </c>
@@ -6552,7 +6863,7 @@
         <v>1194.6338725265152</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>110</v>
       </c>
@@ -6572,7 +6883,7 @@
         <v>460.54747632980491</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>111</v>
       </c>
@@ -6592,7 +6903,7 @@
         <v>922.68201761768364</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>112</v>
       </c>
@@ -6612,7 +6923,7 @@
         <v>881.29115046163486</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>113</v>
       </c>
@@ -6632,7 +6943,7 @@
         <v>872.73469821815206</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>114</v>
       </c>
@@ -6652,7 +6963,7 @@
         <v>581.27193168594556</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>115</v>
       </c>
@@ -6672,7 +6983,7 @@
         <v>537.54836831215925</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>116</v>
       </c>
@@ -6692,7 +7003,7 @@
         <v>1296.1908027475388</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>117</v>
       </c>
@@ -6712,7 +7023,7 @@
         <v>1251.5942514404196</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>118</v>
       </c>
@@ -6738,7 +7049,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>119</v>
       </c>
@@ -6764,7 +7075,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>120</v>
       </c>
@@ -6784,7 +7095,7 @@
         <v>1251.1788593417016</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>121</v>
       </c>
@@ -6804,7 +7115,7 @@
         <v>1080.8809335874446</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>122</v>
       </c>
@@ -6824,7 +7135,7 @@
         <v>879.67938773241201</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>123</v>
       </c>
@@ -6844,7 +7155,7 @@
         <v>1036.9780443516509</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>124</v>
       </c>
@@ -6864,7 +7175,7 @@
         <v>1778.9155994712464</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>125</v>
       </c>
@@ -6884,7 +7195,7 @@
         <v>492.6234913924153</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>126</v>
       </c>
@@ -6904,7 +7215,7 @@
         <v>24.072827949184788</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>127</v>
       </c>
@@ -6924,7 +7235,7 @@
         <v>64.339238860453506</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>133</v>
       </c>
@@ -6944,7 +7255,7 @@
         <v>207.8719331919755</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>136</v>
       </c>
@@ -6964,7 +7275,7 @@
         <v>138.04333895591375</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>137</v>
       </c>
@@ -6985,7 +7296,7 @@
       </c>
       <c r="F31" s="7"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>134</v>
       </c>
@@ -7005,7 +7316,7 @@
         <v>184.24908079822336</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>135</v>
       </c>
@@ -7025,7 +7336,7 @@
         <v>926.88175991374135</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>139</v>
       </c>
@@ -7045,7 +7356,7 @@
         <v>486.91166620058681</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>140</v>
       </c>
@@ -7065,7 +7376,7 @@
         <v>875.76309877890378</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>138</v>
       </c>
@@ -7085,7 +7396,7 @@
         <v>303.23018266722977</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>141</v>
       </c>
@@ -7105,7 +7416,7 @@
         <v>2294.9404868978409</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>162</v>
       </c>
@@ -7125,7 +7436,7 @@
         <v>148.32980520874986</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>163</v>
       </c>
@@ -7145,7 +7456,7 @@
         <v>532.89409450498101</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>164</v>
       </c>
@@ -7165,7 +7476,7 @@
         <v>283.20100953040998</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>165</v>
       </c>
@@ -7185,7 +7496,7 @@
         <v>833.46324871491561</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>166</v>
       </c>
@@ -7205,7 +7516,7 @@
         <v>1504.5443523099382</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>167</v>
       </c>
@@ -7225,7 +7536,7 @@
         <v>1359.7250044629604</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>168</v>
       </c>
@@ -7245,7 +7556,7 @@
         <v>429.63219346738299</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>169</v>
       </c>
@@ -7265,7 +7576,7 @@
         <v>179.39789128135487</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>170</v>
       </c>
@@ -7285,7 +7596,7 @@
         <v>146.80658820772371</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>171</v>
       </c>
@@ -7305,7 +7616,7 @@
         <v>804.34807109832093</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>172</v>
       </c>
@@ -7325,7 +7636,7 @@
         <v>625.20915402841661</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>173</v>
       </c>
@@ -7345,7 +7656,7 @@
         <v>492.3534281993272</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>180</v>
       </c>
@@ -7365,7 +7676,7 @@
         <v>695.82572169514754</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>181</v>
       </c>
@@ -7385,7 +7696,7 @@
         <v>611.69319324915011</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>182</v>
       </c>
@@ -7405,7 +7716,7 @@
         <v>351.31854287090141</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>183</v>
       </c>
@@ -7425,7 +7736,7 @@
         <v>380.30484808213612</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>184</v>
       </c>
@@ -7445,7 +7756,7 @@
         <v>636.11390476472218</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -7465,7 +7776,7 @@
         <v>372.88394874373085</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>186</v>
       </c>
@@ -7485,7 +7796,7 @@
         <v>752.49595149981849</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>187</v>
       </c>
@@ -7505,7 +7816,7 @@
         <v>583.72783370072705</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>188</v>
       </c>
@@ -7525,7 +7836,7 @@
         <v>650.68824789365851</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>198</v>
       </c>
@@ -7545,7 +7856,7 @@
         <v>796.63867472564982</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>199</v>
       </c>
@@ -7565,7 +7876,7 @@
         <v>541.38053925422037</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>200</v>
       </c>
@@ -7585,7 +7896,7 @@
         <v>764.16382344027829</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>201</v>
       </c>
@@ -7605,7 +7916,7 @@
         <v>524.79866579928125</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>202</v>
       </c>
@@ -7625,7 +7936,7 @@
         <v>476.6320291572211</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>203</v>
       </c>
@@ -7645,7 +7956,7 @@
         <v>615.17108105747434</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>204</v>
       </c>
@@ -7665,7 +7976,7 @@
         <v>65.79642942038133</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>205</v>
       </c>
@@ -7685,7 +7996,7 @@
         <v>127.65896032845698</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>206</v>
       </c>
@@ -7705,7 +8016,7 @@
         <v>35.44954064528568</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>226</v>
       </c>
@@ -7725,7 +8036,7 @@
         <v>536.35764972708762</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>227</v>
       </c>
@@ -7745,7 +8056,7 @@
         <v>321.16417593017383</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>228</v>
       </c>
@@ -7776,7 +8087,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -7784,26 +8095,26 @@
       <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
     <col min="11" max="11" width="103" style="6" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" style="11" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" style="12" customWidth="1"/>
-    <col min="15" max="15" width="59.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="11" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" style="12" customWidth="1"/>
+    <col min="15" max="15" width="59.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
@@ -7834,7 +8145,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>56</v>
       </c>
@@ -7872,7 +8183,7 @@
         <v>33.311999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>40</v>
       </c>
@@ -7907,7 +8218,7 @@
         <v>33.661000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>41</v>
       </c>
@@ -7946,7 +8257,7 @@
         <v>33.524999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>42</v>
       </c>
@@ -7984,7 +8295,7 @@
         <v>27.53</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
@@ -8004,7 +8315,7 @@
         <v>127.93487528889766</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>44</v>
       </c>
@@ -8027,7 +8338,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
@@ -8047,7 +8358,7 @@
         <v>1616.5688340569229</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>57</v>
       </c>
@@ -8074,7 +8385,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>108</v>
       </c>
@@ -8100,7 +8411,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>110</v>
       </c>
@@ -8130,7 +8441,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>111</v>
       </c>
@@ -8160,7 +8471,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>112</v>
       </c>
@@ -8180,7 +8491,7 @@
         <v>881.29115046163486</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>113</v>
       </c>
@@ -8200,7 +8511,7 @@
         <v>872.73469821815206</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>114</v>
       </c>
@@ -8223,7 +8534,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>115</v>
       </c>
@@ -8243,7 +8554,7 @@
         <v>537.54836831215925</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>116</v>
       </c>
@@ -8270,7 +8581,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>117</v>
       </c>
@@ -8296,7 +8607,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
         <v>118</v>
       </c>
@@ -8332,7 +8643,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
         <v>119</v>
       </c>
@@ -8368,7 +8679,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>120</v>
       </c>
@@ -8388,7 +8699,7 @@
         <v>1251.1788593417016</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>121</v>
       </c>
@@ -8411,7 +8722,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>122</v>
       </c>
@@ -8431,7 +8742,7 @@
         <v>879.67938773241201</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>123</v>
       </c>
@@ -8458,7 +8769,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
         <v>124</v>
       </c>
@@ -8484,7 +8795,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
         <v>125</v>
       </c>
@@ -8514,7 +8825,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
         <v>126</v>
       </c>
@@ -8544,7 +8855,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
         <v>127</v>
       </c>
@@ -8564,7 +8875,7 @@
         <v>64.339238860453506</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>136</v>
       </c>
@@ -8584,7 +8895,7 @@
         <v>138.04333895591375</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>137</v>
       </c>
@@ -8604,7 +8915,7 @@
         <v>257.12051628811935</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
         <v>138</v>
       </c>
@@ -8625,7 +8936,7 @@
       </c>
       <c r="F31" s="7"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>168</v>
       </c>
@@ -8651,7 +8962,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>169</v>
       </c>
@@ -8671,7 +8982,7 @@
         <v>179.39789128135487</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>170</v>
       </c>
@@ -8698,7 +9009,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
         <v>183</v>
       </c>
@@ -8724,7 +9035,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
         <v>184</v>
       </c>
@@ -8754,7 +9065,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
         <v>185</v>
       </c>
@@ -8784,7 +9095,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>201</v>
       </c>
@@ -8804,7 +9115,7 @@
         <v>524.79866579928125</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
         <v>202</v>
       </c>
@@ -8824,7 +9135,7 @@
         <v>476.6320291572211</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>203</v>
       </c>
@@ -8844,7 +9155,7 @@
         <v>615.17108105747434</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="39" t="s">
         <v>204</v>
       </c>
@@ -8864,7 +9175,7 @@
         <v>65.79642942038133</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="39" t="s">
         <v>205</v>
       </c>
@@ -8884,7 +9195,7 @@
         <v>127.65896032845698</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="39" t="s">
         <v>206</v>
       </c>
@@ -8912,32 +9223,32 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="103" style="6" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" style="11" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="12" customWidth="1"/>
-    <col min="14" max="14" width="59.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" style="11" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="12" customWidth="1"/>
+    <col min="14" max="14" width="59.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -8965,7 +9276,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>133</v>
       </c>
@@ -9003,7 +9314,7 @@
         <v>33.311999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>134</v>
       </c>
@@ -9038,7 +9349,7 @@
         <v>33.661000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -9077,7 +9388,7 @@
         <v>33.524999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>139</v>
       </c>
@@ -9116,7 +9427,7 @@
         <v>27.53</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>140</v>
       </c>
@@ -9135,8 +9446,17 @@
         <f t="shared" si="1"/>
         <v>875.76309877890378</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K6" t="s">
+        <v>244</v>
+      </c>
+      <c r="L6" s="11">
+        <v>2254.1016828735396</v>
+      </c>
+      <c r="M6" s="12">
+        <v>30.34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>141</v>
       </c>
@@ -9144,7 +9464,7 @@
         <v>2192.0776138154802</v>
       </c>
       <c r="C7" s="13">
-        <f t="shared" ref="C7:C28" si="3">$L$5</f>
+        <f t="shared" ref="C7:C29" si="3">$L$5</f>
         <v>2144.1720766939966</v>
       </c>
       <c r="D7" s="17">
@@ -9156,7 +9476,7 @@
         <v>2294.9404868978409</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>162</v>
       </c>
@@ -9176,7 +9496,7 @@
         <v>148.32980520874986</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>163</v>
       </c>
@@ -9196,7 +9516,7 @@
         <v>532.89409450498101</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>164</v>
       </c>
@@ -9216,7 +9536,7 @@
         <v>283.20100953040998</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>165</v>
       </c>
@@ -9236,7 +9556,7 @@
         <v>833.46324871491561</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>166</v>
       </c>
@@ -9256,7 +9576,7 @@
         <v>1504.5443523099382</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>167</v>
       </c>
@@ -9276,7 +9596,7 @@
         <v>1359.7250044629604</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>171</v>
       </c>
@@ -9296,7 +9616,7 @@
         <v>804.34807109832093</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>172</v>
       </c>
@@ -9316,7 +9636,7 @@
         <v>625.20915402841661</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>173</v>
       </c>
@@ -9336,7 +9656,7 @@
         <v>492.3534281993272</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>180</v>
       </c>
@@ -9356,7 +9676,7 @@
         <v>695.82572169514754</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>181</v>
       </c>
@@ -9376,7 +9696,7 @@
         <v>611.69319324915011</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>182</v>
       </c>
@@ -9402,7 +9722,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>186</v>
       </c>
@@ -9428,7 +9748,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>187</v>
       </c>
@@ -9448,7 +9768,7 @@
         <v>583.72783370072705</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>188</v>
       </c>
@@ -9468,7 +9788,7 @@
         <v>650.68824789365851</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>198</v>
       </c>
@@ -9488,7 +9808,7 @@
         <v>796.63867472564982</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>199</v>
       </c>
@@ -9514,7 +9834,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>200</v>
       </c>
@@ -9534,7 +9854,7 @@
         <v>764.16382344027829</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>226</v>
       </c>
@@ -9561,7 +9881,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>227</v>
       </c>
@@ -9587,7 +9907,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>228</v>
       </c>
@@ -9617,7 +9937,25 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>232</v>
+      </c>
+      <c r="B29" s="11">
+        <v>2185.6742415221702</v>
+      </c>
+      <c r="C29" s="11">
+        <f t="shared" si="3"/>
+        <v>2144.1720766939966</v>
+      </c>
+      <c r="D29" s="36">
+        <f t="shared" ref="D29" si="4">B29-C29</f>
+        <v>41.502164828173591</v>
+      </c>
+      <c r="E29" s="37">
+        <f t="shared" ref="E29" si="5">D29^2</f>
+        <v>1722.4296854248892</v>
+      </c>
       <c r="G29">
         <f>G28/L5</f>
         <v>9.4126959584352708E-3</v>
@@ -9629,7 +9967,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F31" s="7"/>
     </row>
   </sheetData>
@@ -9640,29 +9978,29 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" style="11" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="37" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" style="11" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -9688,7 +10026,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>133</v>
       </c>
@@ -9724,7 +10062,7 @@
         <v>33.311999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>134</v>
       </c>
@@ -9759,7 +10097,7 @@
         <v>33.661000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -9798,7 +10136,7 @@
         <v>33.524999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>139</v>
       </c>
@@ -9838,7 +10176,7 @@
         <v>27.53</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>140</v>
       </c>
@@ -9858,7 +10196,7 @@
         <v>102.30344069771941</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>141</v>
       </c>
@@ -9878,7 +10216,7 @@
         <v>808.08060613910686</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>162</v>
       </c>
@@ -9898,7 +10236,7 @@
         <v>53.285708629655147</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>163</v>
       </c>
@@ -9918,7 +10256,7 @@
         <v>13.001220442986153</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>164</v>
       </c>
@@ -9938,7 +10276,7 @@
         <v>7.023567056548595</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>165</v>
       </c>
@@ -9958,7 +10296,7 @@
         <v>88.190600763448444</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>166</v>
       </c>
@@ -9978,7 +10316,7 @@
         <v>372.86366208601373</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>167</v>
       </c>
@@ -9998,7 +10336,7 @@
         <v>302.60935966796575</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>171</v>
       </c>
@@ -10018,7 +10356,7 @@
         <v>78.894407008806681</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>172</v>
       </c>
@@ -10038,7 +10376,7 @@
         <v>30.530091992903429</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>173</v>
       </c>
@@ -10058,7 +10396,7 @@
         <v>7.3455091416442153</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>180</v>
       </c>
@@ -10078,7 +10416,7 @@
         <v>47.606277053628439</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>181</v>
       </c>
@@ -10098,7 +10436,7 @@
         <v>27.600875305300281</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>182</v>
       </c>
@@ -10118,7 +10456,7 @@
         <v>0.54064424462958727</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>186</v>
       </c>
@@ -10138,7 +10476,7 @@
         <v>63.248318802554536</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>187</v>
       </c>
@@ -10158,7 +10496,7 @@
         <v>21.918142954464969</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>188</v>
       </c>
@@ -10178,7 +10516,7 @@
         <v>36.358646694738432</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>198</v>
       </c>
@@ -10198,7 +10536,7 @@
         <v>76.492687594572502</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>199</v>
       </c>
@@ -10224,7 +10562,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>200</v>
       </c>
@@ -10244,7 +10582,7 @@
         <v>66.662893254589605</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>226</v>
       </c>
@@ -10271,7 +10609,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>227</v>
       </c>
@@ -10297,7 +10635,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>228</v>
       </c>
@@ -10327,7 +10665,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G29">
         <f>G28/L5</f>
         <v>1.0996962711927174E-3</v>

</xml_diff>

<commit_message>
Finished compiling Christian's alkalinity data. Most looked pretty good with only a few samples above 1% coefficient of variation.
</commit_message>
<xml_diff>
--- a/check sample work/TA QAQC/20201110 results summary both probes.xlsx
+++ b/check sample work/TA QAQC/20201110 results summary both probes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rye-Tech\Documents\R\rye-tech-home\2021-season-summary\check sample work\TA QAQC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152E138B-6AE8-4BD5-92C8-BFDC1667FFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B899AD-A7C8-4211-9C2D-49541F122BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="297">
   <si>
     <t>sample</t>
   </si>
@@ -768,6 +768,159 @@
   </si>
   <si>
     <t>using only two values in the calulations to the right</t>
+  </si>
+  <si>
+    <t>H2-702-1</t>
+  </si>
+  <si>
+    <t>H2-702-2</t>
+  </si>
+  <si>
+    <t>H2-702-3</t>
+  </si>
+  <si>
+    <t>H3-702-1</t>
+  </si>
+  <si>
+    <t>H3-702-2</t>
+  </si>
+  <si>
+    <t>H3-702-3</t>
+  </si>
+  <si>
+    <t>H2-719-1</t>
+  </si>
+  <si>
+    <t>H2-719-2</t>
+  </si>
+  <si>
+    <t>BAYSTD1-04202021-1</t>
+  </si>
+  <si>
+    <t>Christian's samples</t>
+  </si>
+  <si>
+    <t>H3-719-1</t>
+  </si>
+  <si>
+    <t>H3-719-2</t>
+  </si>
+  <si>
+    <t>T44-702-1</t>
+  </si>
+  <si>
+    <t>T44-702-2</t>
+  </si>
+  <si>
+    <t>T4-702-1</t>
+  </si>
+  <si>
+    <t>T4-702-2</t>
+  </si>
+  <si>
+    <t>T3-702-1</t>
+  </si>
+  <si>
+    <t>T3-702-2</t>
+  </si>
+  <si>
+    <t>BaySTD2-04282021-1</t>
+  </si>
+  <si>
+    <t>BaySTD2-04282021-2</t>
+  </si>
+  <si>
+    <t>BAYSTD2-05052021-1</t>
+  </si>
+  <si>
+    <t>BAYSTD2-05052021-2</t>
+  </si>
+  <si>
+    <t>T6-702-1</t>
+  </si>
+  <si>
+    <t>T6-702-2</t>
+  </si>
+  <si>
+    <t>T27-719-1</t>
+  </si>
+  <si>
+    <t>T27-719-2</t>
+  </si>
+  <si>
+    <t>T10-719-1</t>
+  </si>
+  <si>
+    <t>T10-719-2</t>
+  </si>
+  <si>
+    <t>T36-719-1</t>
+  </si>
+  <si>
+    <t>T36-719-2</t>
+  </si>
+  <si>
+    <t>T16-719-1</t>
+  </si>
+  <si>
+    <t>T16-719-2</t>
+  </si>
+  <si>
+    <t>T12-708-1</t>
+  </si>
+  <si>
+    <t>T12-708-2</t>
+  </si>
+  <si>
+    <t>T6-708-1</t>
+  </si>
+  <si>
+    <t>T6-708-2</t>
+  </si>
+  <si>
+    <t>T20-708-1</t>
+  </si>
+  <si>
+    <t>T20-708-2</t>
+  </si>
+  <si>
+    <t>BaySTD2-05122021-1</t>
+  </si>
+  <si>
+    <t>BaySTD2-05122021-2</t>
+  </si>
+  <si>
+    <t>Bay Standard Batch 2 started here</t>
+  </si>
+  <si>
+    <t>T8-714-1</t>
+  </si>
+  <si>
+    <t>T8-714-2</t>
+  </si>
+  <si>
+    <t>T14-714-1</t>
+  </si>
+  <si>
+    <t>T14-714-2</t>
+  </si>
+  <si>
+    <t>T38-714-1</t>
+  </si>
+  <si>
+    <t>T38-714-2</t>
+  </si>
+  <si>
+    <t>T21-708-1</t>
+  </si>
+  <si>
+    <t>T21-708-2</t>
+  </si>
+  <si>
+    <t>BaySTD2-05192021-1</t>
+  </si>
+  <si>
+    <t>BaySTD2-05192021-2</t>
   </si>
 </sst>
 </file>
@@ -860,7 +1013,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -933,6 +1086,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2093,11 +2247,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M206"/>
+  <dimension ref="A1:M266"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A186" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D199" sqref="D199"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A253" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A202" sqref="A202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6357,197 +6511,1671 @@
         <v>215</v>
       </c>
       <c r="B195" s="19">
-        <v>2380.6235945409098</v>
-      </c>
-    </row>
-    <row r="196" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A196" s="30" t="s">
-        <v>234</v>
-      </c>
-      <c r="B196" s="30">
-        <v>2250.7575623355901</v>
+        <v>2910.6442085056501</v>
+      </c>
+      <c r="D195" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A196" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="B196" s="19">
+        <v>2184.3870913115302</v>
       </c>
       <c r="D196" s="18" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
     </row>
     <row r="197" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A197" s="19" t="s">
-        <v>235</v>
-      </c>
-      <c r="B197" s="19">
-        <v>2203.22618654695</v>
-      </c>
-    </row>
-    <row r="198" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A198" s="19" t="s">
-        <v>236</v>
-      </c>
-      <c r="B198" s="19">
-        <v>2200.2796088885002</v>
-      </c>
-      <c r="D198" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="E198" s="21">
-        <f>AVERAGE(B197:B198)</f>
-        <v>2201.7528977177253</v>
-      </c>
-      <c r="F198" s="21">
-        <f>_xlfn.STDEV.S(B197:B198)</f>
-        <v>2.0835450435826104</v>
-      </c>
-      <c r="G198" s="21">
-        <f>2*F198</f>
-        <v>4.1670900871652208</v>
-      </c>
-      <c r="H198" s="21">
-        <f>F198/E198</f>
-        <v>9.4631193434211174E-4</v>
-      </c>
-      <c r="I198" s="42">
-        <f>H198</f>
-        <v>9.4631193434211174E-4</v>
-      </c>
-      <c r="J198" s="21">
-        <f>MIN(B197:B198)</f>
-        <v>2200.2796088885002</v>
-      </c>
-      <c r="K198" s="21">
-        <f>MAX(B197:B198)</f>
-        <v>2203.22618654695</v>
-      </c>
-      <c r="L198" s="21">
-        <f>K198-J198</f>
-        <v>2.9465776584497689</v>
-      </c>
+      <c r="A197" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="B197" s="30">
+        <v>2280.5081732143799</v>
+      </c>
+      <c r="C197" s="30"/>
+      <c r="D197" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="E197" s="30"/>
+      <c r="F197" s="30"/>
+      <c r="G197" s="30"/>
+      <c r="H197" s="30"/>
+      <c r="I197" s="44"/>
+      <c r="J197" s="30"/>
+      <c r="K197" s="30"/>
+      <c r="L197" s="30"/>
+    </row>
+    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A198" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="B198" s="30">
+        <v>2251.6546099120901</v>
+      </c>
+      <c r="C198" s="30"/>
+      <c r="D198" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="E198" s="30"/>
+      <c r="F198" s="30"/>
+      <c r="G198" s="30"/>
+      <c r="H198" s="30"/>
+      <c r="I198" s="44"/>
+      <c r="J198" s="30"/>
+      <c r="K198" s="30"/>
+      <c r="L198" s="30"/>
     </row>
     <row r="199" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A199" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="B199" s="19">
-        <v>2398.0314183502901</v>
+      <c r="A199" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="B199" s="30">
+        <v>2332.18478361088</v>
+      </c>
+      <c r="C199" s="30"/>
+      <c r="D199" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="E199" s="30">
+        <f>AVERAGE(B197:B199)</f>
+        <v>2288.1158555791167</v>
+      </c>
+      <c r="F199" s="30">
+        <f>_xlfn.STDEV.S(B197:B199)</f>
+        <v>40.800549533203139</v>
+      </c>
+      <c r="G199" s="30">
+        <f>2*F199</f>
+        <v>81.601099066406277</v>
+      </c>
+      <c r="H199" s="30">
+        <f>F199/E199</f>
+        <v>1.7831505093467662E-2</v>
+      </c>
+      <c r="I199" s="44">
+        <f>H199</f>
+        <v>1.7831505093467662E-2</v>
+      </c>
+      <c r="J199" s="30">
+        <f>MIN(B197:B199)</f>
+        <v>2251.6546099120901</v>
+      </c>
+      <c r="K199" s="30">
+        <f>MAX(B197:B199)</f>
+        <v>2332.18478361088</v>
+      </c>
+      <c r="L199" s="30">
+        <f>K199-J199</f>
+        <v>80.530173698789895</v>
       </c>
     </row>
     <row r="200" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A200" s="19" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="B200" s="19">
-        <v>2188.0548117417202</v>
+        <v>2299.0641468151998</v>
+      </c>
+      <c r="D200" s="18" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="201" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A201" s="19" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="B201" s="19">
-        <v>2182.1633268279402</v>
+        <v>2306.1521269356699</v>
+      </c>
+      <c r="D201" s="18" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="202" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A202" s="19" t="s">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="B202" s="19">
-        <v>2179.9038352182201</v>
+        <v>2284.04521702488</v>
+      </c>
+      <c r="D202" s="18" t="s">
+        <v>255</v>
       </c>
       <c r="E202" s="19">
         <f>AVERAGE(B200:B202)</f>
-        <v>2183.3739912626265</v>
+        <v>2296.4204969252501</v>
       </c>
       <c r="F202" s="19">
         <f>_xlfn.STDEV.S(B200:B202)</f>
-        <v>4.2081927061059838</v>
+        <v>11.288070251660352</v>
       </c>
       <c r="G202" s="19">
         <f>2*F202</f>
-        <v>8.4163854122119677</v>
+        <v>22.576140503320705</v>
       </c>
       <c r="H202" s="19">
         <f>F202/E202</f>
-        <v>1.9273806150234582E-3</v>
+        <v>4.9155066621179811E-3</v>
       </c>
       <c r="I202" s="41">
         <f>H202</f>
-        <v>1.9273806150234582E-3</v>
+        <v>4.9155066621179811E-3</v>
       </c>
       <c r="J202" s="19">
         <f>MIN(B200:B202)</f>
-        <v>2179.9038352182201</v>
+        <v>2284.04521702488</v>
       </c>
       <c r="K202" s="19">
         <f>MAX(B200:B202)</f>
-        <v>2188.0548117417202</v>
+        <v>2306.1521269356699</v>
       </c>
       <c r="L202" s="19">
         <f>K202-J202</f>
-        <v>8.1509765235000486</v>
+        <v>22.106909910789909</v>
       </c>
     </row>
     <row r="203" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A203" s="19" t="s">
-        <v>233</v>
+        <v>252</v>
       </c>
       <c r="B203" s="19">
-        <v>2110.5869142463098</v>
+        <v>2289.47979501486</v>
+      </c>
+      <c r="D203" s="18" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="204" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A204" s="19" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="B204" s="19">
-        <v>2253.49247123941</v>
+        <v>2295.8571451634498</v>
+      </c>
+      <c r="D204" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E204" s="21">
+        <f>AVERAGE(B203:B204)</f>
+        <v>2292.6684700891547</v>
+      </c>
+      <c r="F204" s="21">
+        <f>_xlfn.STDEV.S(B203:B204)</f>
+        <v>4.5094675360688932</v>
+      </c>
+      <c r="G204" s="21">
+        <f>2*F204</f>
+        <v>9.0189350721377863</v>
+      </c>
+      <c r="H204" s="21">
+        <f>F204/E204</f>
+        <v>1.9669078172011214E-3</v>
+      </c>
+      <c r="I204" s="42">
+        <f>H204</f>
+        <v>1.9669078172011214E-3</v>
+      </c>
+      <c r="J204" s="21">
+        <f>MIN(B203:B204)</f>
+        <v>2289.47979501486</v>
+      </c>
+      <c r="K204" s="21">
+        <f>MAX(B203:B204)</f>
+        <v>2295.8571451634498</v>
+      </c>
+      <c r="L204" s="21">
+        <f>K204-J204</f>
+        <v>6.3773501485898123</v>
       </c>
     </row>
     <row r="205" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A205" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="B205" s="19">
+        <v>2380.6235945409098</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A206" s="30" t="s">
+        <v>234</v>
+      </c>
+      <c r="B206" s="30">
+        <v>2250.7575623355901</v>
+      </c>
+      <c r="D206" s="18" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A207" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="B207" s="19">
+        <v>2203.22618654695</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A208" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="B208" s="19">
+        <v>2200.2796088885002</v>
+      </c>
+      <c r="D208" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="E208" s="21">
+        <f>AVERAGE(B207:B208)</f>
+        <v>2201.7528977177253</v>
+      </c>
+      <c r="F208" s="21">
+        <f>_xlfn.STDEV.S(B207:B208)</f>
+        <v>2.0835450435826104</v>
+      </c>
+      <c r="G208" s="21">
+        <f>2*F208</f>
+        <v>4.1670900871652208</v>
+      </c>
+      <c r="H208" s="21">
+        <f>F208/E208</f>
+        <v>9.4631193434211174E-4</v>
+      </c>
+      <c r="I208" s="42">
+        <f>H208</f>
+        <v>9.4631193434211174E-4</v>
+      </c>
+      <c r="J208" s="21">
+        <f>MIN(B207:B208)</f>
+        <v>2200.2796088885002</v>
+      </c>
+      <c r="K208" s="21">
+        <f>MAX(B207:B208)</f>
+        <v>2203.22618654695</v>
+      </c>
+      <c r="L208" s="21">
+        <f>K208-J208</f>
+        <v>2.9465776584497689</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A209" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="B209" s="19">
+        <v>2398.0314183502901</v>
+      </c>
+    </row>
+    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A210" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="B210" s="19">
+        <v>2188.0548117417202</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A211" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="B211" s="19">
+        <v>2182.1633268279402</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A212" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="B212" s="19">
+        <v>2179.9038352182201</v>
+      </c>
+      <c r="E212" s="19">
+        <f>AVERAGE(B210:B212)</f>
+        <v>2183.3739912626265</v>
+      </c>
+      <c r="F212" s="19">
+        <f>_xlfn.STDEV.S(B210:B212)</f>
+        <v>4.2081927061059838</v>
+      </c>
+      <c r="G212" s="19">
+        <f>2*F212</f>
+        <v>8.4163854122119677</v>
+      </c>
+      <c r="H212" s="19">
+        <f>F212/E212</f>
+        <v>1.9273806150234582E-3</v>
+      </c>
+      <c r="I212" s="41">
+        <f>H212</f>
+        <v>1.9273806150234582E-3</v>
+      </c>
+      <c r="J212" s="19">
+        <f>MIN(B210:B212)</f>
+        <v>2179.9038352182201</v>
+      </c>
+      <c r="K212" s="19">
+        <f>MAX(B210:B212)</f>
+        <v>2188.0548117417202</v>
+      </c>
+      <c r="L212" s="19">
+        <f>K212-J212</f>
+        <v>8.1509765235000486</v>
+      </c>
+    </row>
+    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A213" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="B213" s="19">
+        <v>2110.5869142463098</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A214" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="B214" s="19">
+        <v>2253.49247123941</v>
+      </c>
+      <c r="D214" s="18" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A215" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="B205" s="19">
+      <c r="B215" s="19">
         <v>2256.3586638595498</v>
       </c>
-    </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A206" s="19" t="s">
+      <c r="D215" s="18" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A216" s="19" t="s">
         <v>242</v>
       </c>
-      <c r="B206" s="19">
+      <c r="B216" s="19">
         <v>2252.4539135216601</v>
       </c>
-      <c r="E206" s="19">
-        <f>AVERAGE(B204:B206)</f>
+      <c r="D216" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="E216" s="19">
+        <f>AVERAGE(B214:B216)</f>
         <v>2254.1016828735396</v>
       </c>
-      <c r="F206" s="19">
-        <f>_xlfn.STDEV.S(B204:B206)</f>
+      <c r="F216" s="19">
+        <f>_xlfn.STDEV.S(B214:B216)</f>
         <v>2.0224052293449852</v>
       </c>
-      <c r="G206" s="19">
-        <f>2*F206</f>
+      <c r="G216" s="19">
+        <f>2*F216</f>
         <v>4.0448104586899705</v>
       </c>
-      <c r="H206" s="19">
-        <f>F206/E206</f>
+      <c r="H216" s="19">
+        <f>F216/E216</f>
         <v>8.9721117938513465E-4</v>
       </c>
-      <c r="I206" s="41">
-        <f>H206</f>
+      <c r="I216" s="41">
+        <f>H216</f>
         <v>8.9721117938513465E-4</v>
       </c>
-      <c r="J206" s="19">
-        <f>MIN(B204:B206)</f>
+      <c r="J216" s="19">
+        <f>MIN(B214:B216)</f>
         <v>2252.4539135216601</v>
       </c>
-      <c r="K206" s="19">
-        <f>MAX(B204:B206)</f>
+      <c r="K216" s="19">
+        <f>MAX(B214:B216)</f>
         <v>2256.3586638595498</v>
       </c>
-      <c r="L206" s="19">
-        <f>K206-J206</f>
+      <c r="L216" s="19">
+        <f>K216-J216</f>
         <v>3.904750337889709</v>
+      </c>
+    </row>
+    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A217" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="B217" s="19">
+        <v>2027.6002279962599</v>
+      </c>
+      <c r="D217" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A218" s="19" t="s">
+        <v>264</v>
+      </c>
+      <c r="B218" s="19">
+        <v>2251.7329711119401</v>
+      </c>
+      <c r="D218" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A219" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="B219" s="19">
+        <v>2243.0483384869099</v>
+      </c>
+      <c r="D219" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E219" s="21">
+        <f>AVERAGE(B218:B219)</f>
+        <v>2247.3906547994247</v>
+      </c>
+      <c r="F219" s="21">
+        <f>_xlfn.STDEV.S(B218:B219)</f>
+        <v>6.1409626212727737</v>
+      </c>
+      <c r="G219" s="21">
+        <f>2*F219</f>
+        <v>12.281925242545547</v>
+      </c>
+      <c r="H219" s="21">
+        <f>F219/E219</f>
+        <v>2.7324856086583856E-3</v>
+      </c>
+      <c r="I219" s="42">
+        <f>H219</f>
+        <v>2.7324856086583856E-3</v>
+      </c>
+      <c r="J219" s="21">
+        <f>MIN(B218:B219)</f>
+        <v>2243.0483384869099</v>
+      </c>
+      <c r="K219" s="21">
+        <f>MAX(B218:B219)</f>
+        <v>2251.7329711119401</v>
+      </c>
+      <c r="L219" s="21">
+        <f>K219-J219</f>
+        <v>8.68463262503019</v>
+      </c>
+    </row>
+    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A220" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="B220" s="19">
+        <v>2074.2815254131001</v>
+      </c>
+      <c r="D220" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A221" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="B221" s="19">
+        <v>2293.8479886776599</v>
+      </c>
+      <c r="D221" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A222" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="B222" s="19">
+        <v>2299.6645821031502</v>
+      </c>
+      <c r="D222" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E222" s="21">
+        <f>AVERAGE(B221:B222)</f>
+        <v>2296.7562853904051</v>
+      </c>
+      <c r="F222" s="21">
+        <f>_xlfn.STDEV.S(B221:B222)</f>
+        <v>4.1129526545692681</v>
+      </c>
+      <c r="G222" s="21">
+        <f>2*F222</f>
+        <v>8.2259053091385361</v>
+      </c>
+      <c r="H222" s="21">
+        <f>F222/E222</f>
+        <v>1.7907658207932777E-3</v>
+      </c>
+      <c r="I222" s="42">
+        <f>H222</f>
+        <v>1.7907658207932777E-3</v>
+      </c>
+      <c r="J222" s="21">
+        <f>MIN(B221:B222)</f>
+        <v>2293.8479886776599</v>
+      </c>
+      <c r="K222" s="21">
+        <f>MAX(B221:B222)</f>
+        <v>2299.6645821031502</v>
+      </c>
+      <c r="L222" s="21">
+        <f>K222-J222</f>
+        <v>5.8165934254902822</v>
+      </c>
+    </row>
+    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A223" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="B223" s="30">
+        <v>2275.85056164758</v>
+      </c>
+      <c r="C223" s="30"/>
+      <c r="D223" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="E223" s="30"/>
+      <c r="F223" s="30"/>
+      <c r="G223" s="30"/>
+      <c r="H223" s="30"/>
+      <c r="I223" s="44"/>
+      <c r="J223" s="30"/>
+      <c r="K223" s="30"/>
+      <c r="L223" s="30"/>
+    </row>
+    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A224" s="30" t="s">
+        <v>259</v>
+      </c>
+      <c r="B224" s="30">
+        <v>2242.8962162373</v>
+      </c>
+      <c r="C224" s="30"/>
+      <c r="D224" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="E224" s="30">
+        <f>AVERAGE(B223:B224)</f>
+        <v>2259.3733889424402</v>
+      </c>
+      <c r="F224" s="30">
+        <f>_xlfn.STDEV.S(B223:B224)</f>
+        <v>23.302241109172755</v>
+      </c>
+      <c r="G224" s="30">
+        <f>2*F224</f>
+        <v>46.60448221834551</v>
+      </c>
+      <c r="H224" s="30">
+        <f>F224/E224</f>
+        <v>1.0313585715055265E-2</v>
+      </c>
+      <c r="I224" s="44">
+        <f>H224</f>
+        <v>1.0313585715055265E-2</v>
+      </c>
+      <c r="J224" s="30">
+        <f>MIN(B223:B224)</f>
+        <v>2242.8962162373</v>
+      </c>
+      <c r="K224" s="30">
+        <f>MAX(B223:B224)</f>
+        <v>2275.85056164758</v>
+      </c>
+      <c r="L224" s="30">
+        <f>K224-J224</f>
+        <v>32.954345410279984</v>
+      </c>
+    </row>
+    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A225" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="B225" s="19">
+        <v>2285.8484447564501</v>
+      </c>
+      <c r="D225" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A226" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="B226" s="19">
+        <v>2280.64577097028</v>
+      </c>
+      <c r="D226" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E226" s="21">
+        <f>AVERAGE(B225:B226)</f>
+        <v>2283.2471078633653</v>
+      </c>
+      <c r="F226" s="21">
+        <f>_xlfn.STDEV.S(B225:B226)</f>
+        <v>3.6788459145024244</v>
+      </c>
+      <c r="G226" s="21">
+        <f>2*F226</f>
+        <v>7.3576918290048487</v>
+      </c>
+      <c r="H226" s="21">
+        <f>F226/E226</f>
+        <v>1.6112342382183255E-3</v>
+      </c>
+      <c r="I226" s="42">
+        <f>H226</f>
+        <v>1.6112342382183255E-3</v>
+      </c>
+      <c r="J226" s="21">
+        <f>MIN(B225:B226)</f>
+        <v>2280.64577097028</v>
+      </c>
+      <c r="K226" s="21">
+        <f>MAX(B225:B226)</f>
+        <v>2285.8484447564501</v>
+      </c>
+      <c r="L226" s="21">
+        <f>K226-J226</f>
+        <v>5.2026737861701804</v>
+      </c>
+    </row>
+    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A227" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="B227" s="19">
+        <v>2288.1536154372102</v>
+      </c>
+      <c r="D227" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A228" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="B228" s="19">
+        <v>2292.4782101573901</v>
+      </c>
+      <c r="D228" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E228" s="21">
+        <f>AVERAGE(B227:B228)</f>
+        <v>2290.3159127973004</v>
+      </c>
+      <c r="F228" s="21">
+        <f>_xlfn.STDEV.S(B227:B228)</f>
+        <v>3.0579502525227493</v>
+      </c>
+      <c r="G228" s="21">
+        <f>2*F228</f>
+        <v>6.1159005050454986</v>
+      </c>
+      <c r="H228" s="21">
+        <f>F228/E228</f>
+        <v>1.3351652649471798E-3</v>
+      </c>
+      <c r="I228" s="42">
+        <f>H228</f>
+        <v>1.3351652649471798E-3</v>
+      </c>
+      <c r="J228" s="21">
+        <f>MIN(B227:B228)</f>
+        <v>2288.1536154372102</v>
+      </c>
+      <c r="K228" s="21">
+        <f>MAX(B227:B228)</f>
+        <v>2292.4782101573901</v>
+      </c>
+      <c r="L228" s="21">
+        <f>K228-J228</f>
+        <v>4.3245947201799027</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A229" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="B229" s="19">
+        <v>2071.5652452823801</v>
+      </c>
+      <c r="D229" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A230" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B230" s="19">
+        <v>2257.8632567361501</v>
+      </c>
+      <c r="D230" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A231" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="B231" s="19">
+        <v>2228.2726380174099</v>
+      </c>
+      <c r="D231" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E231" s="21">
+        <f>AVERAGE(B230:B231)</f>
+        <v>2243.06794737678</v>
+      </c>
+      <c r="F231" s="21">
+        <f>_xlfn.STDEV.S(B230:B231)</f>
+        <v>20.923727155526777</v>
+      </c>
+      <c r="G231" s="21">
+        <f>2*F231</f>
+        <v>41.847454311053554</v>
+      </c>
+      <c r="H231" s="21">
+        <f>F231/E231</f>
+        <v>9.3281735758368924E-3</v>
+      </c>
+      <c r="I231" s="42">
+        <f>H231</f>
+        <v>9.3281735758368924E-3</v>
+      </c>
+      <c r="J231" s="21">
+        <f>MIN(B230:B231)</f>
+        <v>2228.2726380174099</v>
+      </c>
+      <c r="K231" s="21">
+        <f>MAX(B230:B231)</f>
+        <v>2257.8632567361501</v>
+      </c>
+      <c r="L231" s="21">
+        <f>K231-J231</f>
+        <v>29.590618718740188</v>
+      </c>
+    </row>
+    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A232" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="B232" s="19">
+        <v>2009.76651707358</v>
+      </c>
+      <c r="D232" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A233" s="30" t="s">
+        <v>268</v>
+      </c>
+      <c r="B233" s="30">
+        <v>2396.33435988671</v>
+      </c>
+      <c r="C233" s="30"/>
+      <c r="D233" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="E233" s="30"/>
+      <c r="F233" s="30"/>
+      <c r="G233" s="30"/>
+      <c r="H233" s="30"/>
+      <c r="I233" s="44"/>
+      <c r="J233" s="30"/>
+      <c r="K233" s="30"/>
+      <c r="L233" s="30"/>
+    </row>
+    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A234" s="30" t="s">
+        <v>269</v>
+      </c>
+      <c r="B234" s="30">
+        <v>2297.7711188746298</v>
+      </c>
+      <c r="C234" s="30"/>
+      <c r="D234" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="E234" s="30">
+        <f>AVERAGE(B233:B234)</f>
+        <v>2347.0527393806697</v>
+      </c>
+      <c r="F234" s="30">
+        <f>_xlfn.STDEV.S(B233:B234)</f>
+        <v>69.69473609536594</v>
+      </c>
+      <c r="G234" s="30">
+        <f>2*F234</f>
+        <v>139.38947219073188</v>
+      </c>
+      <c r="H234" s="30">
+        <f>F234/E234</f>
+        <v>2.9694576063832589E-2</v>
+      </c>
+      <c r="I234" s="44">
+        <f>H234</f>
+        <v>2.9694576063832589E-2</v>
+      </c>
+      <c r="J234" s="30">
+        <f>MIN(B233:B234)</f>
+        <v>2297.7711188746298</v>
+      </c>
+      <c r="K234" s="30">
+        <f>MAX(B233:B234)</f>
+        <v>2396.33435988671</v>
+      </c>
+      <c r="L234" s="30">
+        <f>K234-J234</f>
+        <v>98.563241012080198</v>
+      </c>
+    </row>
+    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A235" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="B235" s="30">
+        <v>2309.8694776061502</v>
+      </c>
+      <c r="C235" s="30"/>
+      <c r="D235" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="E235" s="30"/>
+      <c r="F235" s="30"/>
+      <c r="G235" s="30"/>
+      <c r="H235" s="30"/>
+      <c r="I235" s="44"/>
+      <c r="J235" s="30"/>
+      <c r="K235" s="30"/>
+      <c r="L235" s="30"/>
+    </row>
+    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A236" s="30" t="s">
+        <v>271</v>
+      </c>
+      <c r="B236" s="30">
+        <v>2259.1673548103699</v>
+      </c>
+      <c r="C236" s="30"/>
+      <c r="D236" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="E236" s="30">
+        <f>AVERAGE(B235:B236)</f>
+        <v>2284.5184162082601</v>
+      </c>
+      <c r="F236" s="30">
+        <f>_xlfn.STDEV.S(B235:B236)</f>
+        <v>35.851814849449262</v>
+      </c>
+      <c r="G236" s="30">
+        <f>2*F236</f>
+        <v>71.703629698898524</v>
+      </c>
+      <c r="H236" s="30">
+        <f>F236/E236</f>
+        <v>1.5693379661589454E-2</v>
+      </c>
+      <c r="I236" s="44">
+        <f>H236</f>
+        <v>1.5693379661589454E-2</v>
+      </c>
+      <c r="J236" s="30">
+        <f>MIN(B235:B236)</f>
+        <v>2259.1673548103699</v>
+      </c>
+      <c r="K236" s="30">
+        <f>MAX(B235:B236)</f>
+        <v>2309.8694776061502</v>
+      </c>
+      <c r="L236" s="30">
+        <f>K236-J236</f>
+        <v>50.702122795780269</v>
+      </c>
+    </row>
+    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A237" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="B237" s="19">
+        <v>2268.69147965308</v>
+      </c>
+      <c r="D237" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A238" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="B238" s="19">
+        <v>2265.82646728605</v>
+      </c>
+      <c r="D238" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E238" s="21">
+        <f>AVERAGE(B237:B238)</f>
+        <v>2267.2589734695648</v>
+      </c>
+      <c r="F238" s="21">
+        <f>_xlfn.STDEV.S(B237:B238)</f>
+        <v>2.0258696729102179</v>
+      </c>
+      <c r="G238" s="21">
+        <f>2*F238</f>
+        <v>4.0517393458204358</v>
+      </c>
+      <c r="H238" s="21">
+        <f>F238/E238</f>
+        <v>8.9353254154731551E-4</v>
+      </c>
+      <c r="I238" s="42">
+        <f>H238</f>
+        <v>8.9353254154731551E-4</v>
+      </c>
+      <c r="J238" s="21">
+        <f>MIN(B237:B238)</f>
+        <v>2265.82646728605</v>
+      </c>
+      <c r="K238" s="21">
+        <f>MAX(B237:B238)</f>
+        <v>2268.69147965308</v>
+      </c>
+      <c r="L238" s="21">
+        <f>K238-J238</f>
+        <v>2.8650123670299763</v>
+      </c>
+    </row>
+    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A239" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="B239" s="19">
+        <v>2260.5269915809099</v>
+      </c>
+      <c r="D239" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A240" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="B240" s="19">
+        <v>2261.1222034543098</v>
+      </c>
+      <c r="D240" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E240" s="21">
+        <f>AVERAGE(B239:B240)</f>
+        <v>2260.8245975176096</v>
+      </c>
+      <c r="F240" s="21">
+        <f>_xlfn.STDEV.S(B239:B240)</f>
+        <v>0.42087835192380108</v>
+      </c>
+      <c r="G240" s="21">
+        <f>2*F240</f>
+        <v>0.84175670384760215</v>
+      </c>
+      <c r="H240" s="21">
+        <f>F240/E240</f>
+        <v>1.8616143525062778E-4</v>
+      </c>
+      <c r="I240" s="42">
+        <f>H240</f>
+        <v>1.8616143525062778E-4</v>
+      </c>
+      <c r="J240" s="21">
+        <f>MIN(B239:B240)</f>
+        <v>2260.5269915809099</v>
+      </c>
+      <c r="K240" s="21">
+        <f>MAX(B239:B240)</f>
+        <v>2261.1222034543098</v>
+      </c>
+      <c r="L240" s="21">
+        <f>K240-J240</f>
+        <v>0.59521187339987591</v>
+      </c>
+    </row>
+    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A241" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="B241" s="19">
+        <v>1989.3161099464901</v>
+      </c>
+      <c r="D241" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A242" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="B242" s="19">
+        <v>2258.9954011299701</v>
+      </c>
+      <c r="D242" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A243" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="B243" s="19">
+        <v>2231.5640206609401</v>
+      </c>
+      <c r="D243" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E243" s="21">
+        <f>AVERAGE(B242:B243)</f>
+        <v>2245.2797108954551</v>
+      </c>
+      <c r="F243" s="21">
+        <f>_xlfn.STDEV.S(B242:B243)</f>
+        <v>19.396915146959362</v>
+      </c>
+      <c r="G243" s="21">
+        <f>2*F243</f>
+        <v>38.793830293918724</v>
+      </c>
+      <c r="H243" s="21">
+        <f>F243/E243</f>
+        <v>8.6389749360998528E-3</v>
+      </c>
+      <c r="I243" s="42">
+        <f>H243</f>
+        <v>8.6389749360998528E-3</v>
+      </c>
+      <c r="J243" s="21">
+        <f>MIN(B242:B243)</f>
+        <v>2231.5640206609401</v>
+      </c>
+      <c r="K243" s="21">
+        <f>MAX(B242:B243)</f>
+        <v>2258.9954011299701</v>
+      </c>
+      <c r="L243" s="21">
+        <f>K243-J243</f>
+        <v>27.431380469030046</v>
+      </c>
+    </row>
+    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A244" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="B244" s="19">
+        <v>1863.6783774078101</v>
+      </c>
+      <c r="D244" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A245" s="30" t="s">
+        <v>276</v>
+      </c>
+      <c r="B245" s="30">
+        <v>2161.0006654414201</v>
+      </c>
+      <c r="C245" s="30"/>
+      <c r="D245" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="E245" s="30"/>
+      <c r="F245" s="30"/>
+      <c r="G245" s="30"/>
+      <c r="H245" s="30"/>
+      <c r="I245" s="44"/>
+      <c r="J245" s="30"/>
+      <c r="K245" s="30"/>
+      <c r="L245" s="30"/>
+    </row>
+    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A246" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="B246" s="30">
+        <v>2267.5799306727399</v>
+      </c>
+      <c r="C246" s="30"/>
+      <c r="D246" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="E246" s="30">
+        <f>AVERAGE(B245:B246)</f>
+        <v>2214.2902980570798</v>
+      </c>
+      <c r="F246" s="30">
+        <f>_xlfn.STDEV.S(B245:B246)</f>
+        <v>75.362921178945882</v>
+      </c>
+      <c r="G246" s="30">
+        <f>2*F246</f>
+        <v>150.72584235789176</v>
+      </c>
+      <c r="H246" s="30">
+        <f>F246/E246</f>
+        <v>3.4034797174098075E-2</v>
+      </c>
+      <c r="I246" s="44">
+        <f>H246</f>
+        <v>3.4034797174098075E-2</v>
+      </c>
+      <c r="J246" s="30">
+        <f>MIN(B245:B246)</f>
+        <v>2161.0006654414201</v>
+      </c>
+      <c r="K246" s="30">
+        <f>MAX(B245:B246)</f>
+        <v>2267.5799306727399</v>
+      </c>
+      <c r="L246" s="30">
+        <f>K246-J246</f>
+        <v>106.57926523131982</v>
+      </c>
+    </row>
+    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A247" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="B247" s="19">
+        <v>2238.0430180316098</v>
+      </c>
+      <c r="D247" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A248" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="B248" s="19">
+        <v>2242.35802318177</v>
+      </c>
+      <c r="D248" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E248" s="21">
+        <f>AVERAGE(B247:B248)</f>
+        <v>2240.2005206066897</v>
+      </c>
+      <c r="F248" s="21">
+        <f>_xlfn.STDEV.S(B247:B248)</f>
+        <v>3.0511694025331768</v>
+      </c>
+      <c r="G248" s="21">
+        <f>2*F248</f>
+        <v>6.1023388050663536</v>
+      </c>
+      <c r="H248" s="21">
+        <f>F248/E248</f>
+        <v>1.3620072732180514E-3</v>
+      </c>
+      <c r="I248" s="42">
+        <f>H248</f>
+        <v>1.3620072732180514E-3</v>
+      </c>
+      <c r="J248" s="21">
+        <f>MIN(B247:B248)</f>
+        <v>2238.0430180316098</v>
+      </c>
+      <c r="K248" s="21">
+        <f>MAX(B247:B248)</f>
+        <v>2242.35802318177</v>
+      </c>
+      <c r="L248" s="21">
+        <f>K248-J248</f>
+        <v>4.315005150160232</v>
+      </c>
+    </row>
+    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A249" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="B249" s="19">
+        <v>1652.86862150455</v>
+      </c>
+      <c r="D249" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A250" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="B250" s="19">
+        <v>2240.12685831519</v>
+      </c>
+      <c r="D250" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A251" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="B251" s="19">
+        <v>2241.2328629815102</v>
+      </c>
+      <c r="D251" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E251" s="21">
+        <f>AVERAGE(B250:B251)</f>
+        <v>2240.6798606483499</v>
+      </c>
+      <c r="F251" s="21">
+        <f>_xlfn.STDEV.S(B250:B251)</f>
+        <v>0.78206339957893012</v>
+      </c>
+      <c r="G251" s="21">
+        <f>2*F251</f>
+        <v>1.5641267991578602</v>
+      </c>
+      <c r="H251" s="21">
+        <f>F251/E251</f>
+        <v>3.4902951256617125E-4</v>
+      </c>
+      <c r="I251" s="42">
+        <f>H251</f>
+        <v>3.4902951256617125E-4</v>
+      </c>
+      <c r="J251" s="21">
+        <f>MIN(B250:B251)</f>
+        <v>2240.12685831519</v>
+      </c>
+      <c r="K251" s="21">
+        <f>MAX(B250:B251)</f>
+        <v>2241.2328629815102</v>
+      </c>
+      <c r="L251" s="21">
+        <f>K251-J251</f>
+        <v>1.1060046663201319</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A252" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="B252" s="19">
+        <v>2233.7405171548899</v>
+      </c>
+      <c r="D252" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A253" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="B253" s="19">
+        <v>2237.4207480158998</v>
+      </c>
+      <c r="D253" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E253" s="21">
+        <f>AVERAGE(B252:B253)</f>
+        <v>2235.5806325853946</v>
+      </c>
+      <c r="F253" s="21">
+        <f>_xlfn.STDEV.S(B252:B253)</f>
+        <v>2.602316198152129</v>
+      </c>
+      <c r="G253" s="21">
+        <f>2*F253</f>
+        <v>5.204632396304258</v>
+      </c>
+      <c r="H253" s="21">
+        <f>F253/E253</f>
+        <v>1.1640448840096694E-3</v>
+      </c>
+      <c r="I253" s="42">
+        <f>H253</f>
+        <v>1.1640448840096694E-3</v>
+      </c>
+      <c r="J253" s="21">
+        <f>MIN(B252:B253)</f>
+        <v>2233.7405171548899</v>
+      </c>
+      <c r="K253" s="21">
+        <f>MAX(B252:B253)</f>
+        <v>2237.4207480158998</v>
+      </c>
+      <c r="L253" s="21">
+        <f>K253-J253</f>
+        <v>3.6802308610099317</v>
+      </c>
+    </row>
+    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A254" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="B254" s="19">
+        <v>1688.41855227112</v>
+      </c>
+      <c r="D254" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A255" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="B255" s="19">
+        <v>2257.6301656681999</v>
+      </c>
+      <c r="D255" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A256" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="B256" s="19">
+        <v>2234.1767862008201</v>
+      </c>
+      <c r="D256" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E256" s="21">
+        <f>AVERAGE(B255:B256)</f>
+        <v>2245.90347593451</v>
+      </c>
+      <c r="F256" s="21">
+        <f>_xlfn.STDEV.S(B255:B256)</f>
+        <v>16.584043663125609</v>
+      </c>
+      <c r="G256" s="21">
+        <f>2*F256</f>
+        <v>33.168087326251218</v>
+      </c>
+      <c r="H256" s="21">
+        <f>F256/E256</f>
+        <v>7.3841301911806633E-3</v>
+      </c>
+      <c r="I256" s="42">
+        <f>H256</f>
+        <v>7.3841301911806633E-3</v>
+      </c>
+      <c r="J256" s="21">
+        <f>MIN(B255:B256)</f>
+        <v>2234.1767862008201</v>
+      </c>
+      <c r="K256" s="21">
+        <f>MAX(B255:B256)</f>
+        <v>2257.6301656681999</v>
+      </c>
+      <c r="L256" s="21">
+        <f>K256-J256</f>
+        <v>23.453379467379818</v>
+      </c>
+    </row>
+    <row r="257" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A257" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="B257" s="19">
+        <v>1586.91235962838</v>
+      </c>
+      <c r="D257" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="258" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A258" s="30" t="s">
+        <v>287</v>
+      </c>
+      <c r="B258" s="30">
+        <v>2378.97423431274</v>
+      </c>
+      <c r="C258" s="30"/>
+      <c r="D258" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="E258" s="30"/>
+      <c r="F258" s="30"/>
+      <c r="G258" s="30"/>
+      <c r="H258" s="30"/>
+      <c r="I258" s="44"/>
+      <c r="J258" s="30"/>
+      <c r="K258" s="30"/>
+      <c r="L258" s="30"/>
+    </row>
+    <row r="259" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A259" s="30" t="s">
+        <v>288</v>
+      </c>
+      <c r="B259" s="30">
+        <v>2300.7800619793502</v>
+      </c>
+      <c r="C259" s="30"/>
+      <c r="D259" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="E259" s="30">
+        <f>AVERAGE(B258:B259)</f>
+        <v>2339.8771481460453</v>
+      </c>
+      <c r="F259" s="30">
+        <f>_xlfn.STDEV.S(B258:B259)</f>
+        <v>55.29162950620946</v>
+      </c>
+      <c r="G259" s="30">
+        <f>2*F259</f>
+        <v>110.58325901241892</v>
+      </c>
+      <c r="H259" s="30">
+        <f>F259/E259</f>
+        <v>2.3630142099562223E-2</v>
+      </c>
+      <c r="I259" s="44">
+        <f>H259</f>
+        <v>2.3630142099562223E-2</v>
+      </c>
+      <c r="J259" s="30">
+        <f>MIN(B258:B259)</f>
+        <v>2300.7800619793502</v>
+      </c>
+      <c r="K259" s="30">
+        <f>MAX(B258:B259)</f>
+        <v>2378.97423431274</v>
+      </c>
+      <c r="L259" s="30">
+        <f>K259-J259</f>
+        <v>78.194172333389815</v>
+      </c>
+    </row>
+    <row r="260" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A260" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="B260" s="19">
+        <v>2284.0635793065999</v>
+      </c>
+      <c r="D260" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="261" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A261" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="B261" s="19">
+        <v>2280.97836434992</v>
+      </c>
+      <c r="D261" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E261" s="21">
+        <f>AVERAGE(B260:B261)</f>
+        <v>2282.5209718282599</v>
+      </c>
+      <c r="F261" s="21">
+        <f>_xlfn.STDEV.S(B260:B261)</f>
+        <v>2.1815764172865317</v>
+      </c>
+      <c r="G261" s="21">
+        <f>2*F261</f>
+        <v>4.3631528345730635</v>
+      </c>
+      <c r="H261" s="21">
+        <f>F261/E261</f>
+        <v>9.5577497171433503E-4</v>
+      </c>
+      <c r="I261" s="42">
+        <f>H261</f>
+        <v>9.5577497171433503E-4</v>
+      </c>
+      <c r="J261" s="21">
+        <f>MIN(B260:B261)</f>
+        <v>2280.97836434992</v>
+      </c>
+      <c r="K261" s="21">
+        <f>MAX(B260:B261)</f>
+        <v>2284.0635793065999</v>
+      </c>
+      <c r="L261" s="21">
+        <f>K261-J261</f>
+        <v>3.0852149566799199</v>
+      </c>
+    </row>
+    <row r="262" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A262" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="B262" s="19">
+        <v>2271.1866011728898</v>
+      </c>
+      <c r="D262" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="263" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A263" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="B263" s="19">
+        <v>2270.2598723444298</v>
+      </c>
+      <c r="D263" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E263" s="21">
+        <f>AVERAGE(B262:B263)</f>
+        <v>2270.7232367586598</v>
+      </c>
+      <c r="F263" s="21">
+        <f>_xlfn.STDEV.S(B262:B263)</f>
+        <v>0.65529623892513067</v>
+      </c>
+      <c r="G263" s="21">
+        <f>2*F263</f>
+        <v>1.3105924778502613</v>
+      </c>
+      <c r="H263" s="21">
+        <f>F263/E263</f>
+        <v>2.8858481223829473E-4</v>
+      </c>
+      <c r="I263" s="42">
+        <f>H263</f>
+        <v>2.8858481223829473E-4</v>
+      </c>
+      <c r="J263" s="21">
+        <f>MIN(B262:B263)</f>
+        <v>2270.2598723444298</v>
+      </c>
+      <c r="K263" s="21">
+        <f>MAX(B262:B263)</f>
+        <v>2271.1866011728898</v>
+      </c>
+      <c r="L263" s="21">
+        <f>K263-J263</f>
+        <v>0.92672882845999993</v>
+      </c>
+    </row>
+    <row r="264" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A264" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="B264" s="19">
+        <v>1464.32775647991</v>
+      </c>
+      <c r="D264" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="265" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A265" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="B265" s="19">
+        <v>2230.36285522256</v>
+      </c>
+      <c r="D265" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="266" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A266" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B266" s="19">
+        <v>2233.7284028355798</v>
+      </c>
+      <c r="D266" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E266" s="21">
+        <f>AVERAGE(B265:B266)</f>
+        <v>2232.0456290290699</v>
+      </c>
+      <c r="F266" s="21">
+        <f>_xlfn.STDEV.S(B265:B266)</f>
+        <v>2.3798015395724788</v>
+      </c>
+      <c r="G266" s="21">
+        <f>2*F266</f>
+        <v>4.7596030791449575</v>
+      </c>
+      <c r="H266" s="21">
+        <f>F266/E266</f>
+        <v>1.0661975313684255E-3</v>
+      </c>
+      <c r="I266" s="42">
+        <f>H266</f>
+        <v>1.0661975313684255E-3</v>
+      </c>
+      <c r="J266" s="21">
+        <f>MIN(B265:B266)</f>
+        <v>2230.36285522256</v>
+      </c>
+      <c r="K266" s="21">
+        <f>MAX(B265:B266)</f>
+        <v>2233.7284028355798</v>
+      </c>
+      <c r="L266" s="21">
+        <f>K266-J266</f>
+        <v>3.3655476130197712</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Imported and updated data compilation for Christian. Most of the rerun alkalinity data look good. There are some that were rerun and didn't improve things, unless we take the third sample from each sample run. After an accilmation those third replicates do align fairly closely, so I suggest that we work with those values. Will depend on how it works in with the rest of the data.
</commit_message>
<xml_diff>
--- a/check sample work/TA QAQC/20201110 results summary both probes.xlsx
+++ b/check sample work/TA QAQC/20201110 results summary both probes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rye-Tech\Documents\R\rye-tech-home\2021-season-summary\check sample work\TA QAQC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B899AD-A7C8-4211-9C2D-49541F122BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E9ECC5-DA32-4166-B396-20FC4EF6AD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="example to follow" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="305">
   <si>
     <t>sample</t>
   </si>
@@ -921,6 +921,30 @@
   </si>
   <si>
     <t>BaySTD2-05192021-2</t>
+  </si>
+  <si>
+    <t>BaySTD2-1</t>
+  </si>
+  <si>
+    <t>BaySTD2-2</t>
+  </si>
+  <si>
+    <t>T16-719-3</t>
+  </si>
+  <si>
+    <t>T8-714-3</t>
+  </si>
+  <si>
+    <t>T21-714-1</t>
+  </si>
+  <si>
+    <t>T21-714-2</t>
+  </si>
+  <si>
+    <t>T21-714-3</t>
+  </si>
+  <si>
+    <t>T6-702-3</t>
   </si>
 </sst>
 </file>
@@ -1716,20 +1740,20 @@
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.28515625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
-    <col min="13" max="13" width="51.140625" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" customWidth="1"/>
+    <col min="13" max="13" width="51.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1767,7 +1791,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1781,7 +1805,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1792,7 +1816,7 @@
         <v>2247.5363699999998</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1836,7 +1860,7 @@
       </c>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1847,7 +1871,7 @@
         <v>2114.1481899999999</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1858,7 +1882,7 @@
         <v>2138.9193500000001</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1902,7 +1926,7 @@
       </c>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1913,7 +1937,7 @@
         <v>2135.2389699999999</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1924,7 +1948,7 @@
         <v>2133.48756</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1968,7 +1992,7 @@
       </c>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1979,7 +2003,7 @@
         <v>2124.9360900000001</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1990,7 +2014,7 @@
         <v>2132.3921700000001</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2034,7 +2058,7 @@
       </c>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -2045,7 +2069,7 @@
         <v>2249.3508299999999</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -2056,7 +2080,7 @@
         <v>2250.2915600000001</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2103,10 +2127,10 @@
       </c>
       <c r="M16" s="3"/>
     </row>
-    <row r="20" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:14" x14ac:dyDescent="0.3">
       <c r="N20" s="4"/>
     </row>
-    <row r="21" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
         <v>34</v>
       </c>
@@ -2117,7 +2141,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E22">
         <f>2238.04</f>
         <v>2238.04</v>
@@ -2131,7 +2155,7 @@
         <v>21.704231088401922</v>
       </c>
     </row>
-    <row r="23" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E23">
         <f t="shared" ref="E23:E26" si="0">2238.04</f>
         <v>2238.04</v>
@@ -2145,7 +2169,7 @@
         <v>90.181043176897006</v>
       </c>
     </row>
-    <row r="24" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E24">
         <f t="shared" si="0"/>
         <v>2238.04</v>
@@ -2159,7 +2183,7 @@
         <v>62.986127504401573</v>
       </c>
     </row>
-    <row r="25" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E25">
         <f>2238.04</f>
         <v>2238.04</v>
@@ -2173,7 +2197,7 @@
         <v>127.93487528889766</v>
       </c>
     </row>
-    <row r="26" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E26">
         <f t="shared" si="0"/>
         <v>2238.04</v>
@@ -2187,7 +2211,7 @@
         <v>150.10072243360378</v>
       </c>
     </row>
-    <row r="29" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:14" x14ac:dyDescent="0.3">
       <c r="G29">
         <f>SQRT(SUM(G22:G26)/5)</f>
         <v>9.5174261173092578</v>
@@ -2196,7 +2220,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:14" x14ac:dyDescent="0.3">
       <c r="F30" s="3"/>
       <c r="G30">
         <v>0.53</v>
@@ -2205,7 +2229,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:14" x14ac:dyDescent="0.3">
       <c r="G31">
         <f>SQRT(G29^2+G30^2)</f>
         <v>9.5321718353395397</v>
@@ -2217,7 +2241,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:14" x14ac:dyDescent="0.3">
       <c r="G32">
         <f>G31/E26</f>
         <v>4.2591606206053246E-3</v>
@@ -2229,12 +2253,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:13" x14ac:dyDescent="0.3">
       <c r="M36" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="4:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D37" s="1" t="s">
         <v>38</v>
       </c>
@@ -2247,29 +2271,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M266"/>
+  <dimension ref="A1:M285"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A253" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A202" sqref="A202"/>
+      <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D286" sqref="D286"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.28515625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" style="18" customWidth="1"/>
     <col min="5" max="5" width="10" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="19"/>
+    <col min="6" max="7" width="9.109375" style="19"/>
     <col min="8" max="8" width="13" style="19" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="41"/>
-    <col min="10" max="10" width="11.42578125" style="19" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" style="19"/>
-    <col min="13" max="13" width="51.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="41"/>
+    <col min="10" max="10" width="11.44140625" style="19" customWidth="1"/>
+    <col min="11" max="12" width="9.109375" style="19"/>
+    <col min="13" max="13" width="51.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -2307,7 +2331,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>40</v>
       </c>
@@ -2329,7 +2353,7 @@
       <c r="K2" s="21"/>
       <c r="L2" s="21"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>41</v>
       </c>
@@ -2349,7 +2373,7 @@
       <c r="K3" s="21"/>
       <c r="L3" s="21"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>42</v>
       </c>
@@ -2394,7 +2418,7 @@
       </c>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
         <v>6</v>
       </c>
@@ -2414,7 +2438,7 @@
       <c r="K5" s="21"/>
       <c r="L5" s="21"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
         <v>7</v>
       </c>
@@ -2434,7 +2458,7 @@
       <c r="K6" s="21"/>
       <c r="L6" s="21"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>8</v>
       </c>
@@ -2479,7 +2503,7 @@
       </c>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
         <v>9</v>
       </c>
@@ -2499,7 +2523,7 @@
       <c r="K8" s="21"/>
       <c r="L8" s="21"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
         <v>10</v>
       </c>
@@ -2519,7 +2543,7 @@
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
         <v>11</v>
       </c>
@@ -2564,7 +2588,7 @@
       </c>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
         <v>12</v>
       </c>
@@ -2584,7 +2608,7 @@
       <c r="K11" s="21"/>
       <c r="L11" s="21"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
         <v>13</v>
       </c>
@@ -2604,7 +2628,7 @@
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
         <v>14</v>
       </c>
@@ -2649,7 +2673,7 @@
       </c>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>43</v>
       </c>
@@ -2669,7 +2693,7 @@
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
         <v>44</v>
       </c>
@@ -2689,7 +2713,7 @@
       <c r="K15" s="21"/>
       <c r="L15" s="21"/>
     </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>45</v>
       </c>
@@ -2736,7 +2760,7 @@
       </c>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="30" t="s">
         <v>54</v>
       </c>
@@ -2754,7 +2778,7 @@
       <c r="I17" s="33"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
         <v>56</v>
       </c>
@@ -2798,7 +2822,7 @@
       </c>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
         <v>48</v>
       </c>
@@ -2812,7 +2836,7 @@
       <c r="I19" s="33"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
         <v>49</v>
       </c>
@@ -2826,7 +2850,7 @@
       <c r="I20" s="33"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
         <v>50</v>
       </c>
@@ -2867,7 +2891,7 @@
       </c>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="19" t="s">
         <v>51</v>
       </c>
@@ -2881,7 +2905,7 @@
       <c r="I22" s="33"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="19" t="s">
         <v>52</v>
       </c>
@@ -2895,7 +2919,7 @@
       <c r="I23" s="33"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="19" t="s">
         <v>53</v>
       </c>
@@ -2936,7 +2960,7 @@
       </c>
       <c r="M24" s="3"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
         <v>55</v>
       </c>
@@ -2944,7 +2968,7 @@
         <v>2278.2465769999999</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
         <v>57</v>
       </c>
@@ -2984,7 +3008,7 @@
         <v>4.9946979999999712</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="21" t="s">
         <v>65</v>
       </c>
@@ -3002,7 +3026,7 @@
       <c r="K27" s="21"/>
       <c r="L27" s="21"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
         <v>108</v>
       </c>
@@ -3020,7 +3044,7 @@
       <c r="K28" s="21"/>
       <c r="L28" s="21"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="21" t="s">
         <v>109</v>
       </c>
@@ -3062,7 +3086,7 @@
         <v>202.47002357553993</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="21" t="s">
         <v>66</v>
       </c>
@@ -3080,7 +3104,7 @@
       <c r="K30" s="21"/>
       <c r="L30" s="21"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="21" t="s">
         <v>67</v>
       </c>
@@ -3098,7 +3122,7 @@
       <c r="K31" s="21"/>
       <c r="L31" s="21"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="21" t="s">
         <v>68</v>
       </c>
@@ -3140,7 +3164,7 @@
         <v>8.0012203823998789</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="s">
         <v>69</v>
       </c>
@@ -3158,7 +3182,7 @@
       <c r="K33" s="21"/>
       <c r="L33" s="21"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="21" t="s">
         <v>70</v>
       </c>
@@ -3176,7 +3200,7 @@
       <c r="K34" s="21"/>
       <c r="L34" s="21"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
         <v>71</v>
       </c>
@@ -3218,7 +3242,7 @@
         <v>9.1970026297599361</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="21" t="s">
         <v>110</v>
       </c>
@@ -3236,7 +3260,7 @@
       <c r="K36" s="21"/>
       <c r="L36" s="21"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="21" t="s">
         <v>111</v>
       </c>
@@ -3278,7 +3302,7 @@
         <v>8.9153114503401412</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="19" t="s">
         <v>65</v>
       </c>
@@ -3286,7 +3310,7 @@
         <v>1624.2912168376199</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="19" t="s">
         <v>112</v>
       </c>
@@ -3294,7 +3318,7 @@
         <v>2241.6865483083102</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="19" t="s">
         <v>113</v>
       </c>
@@ -3334,7 +3358,7 @@
         <v>0.14446479651041955</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="19" t="s">
         <v>72</v>
       </c>
@@ -3342,7 +3366,7 @@
         <v>2125.89715188732</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="19" t="s">
         <v>73</v>
       </c>
@@ -3350,7 +3374,7 @@
         <v>2109.3231506451998</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="19" t="s">
         <v>74</v>
       </c>
@@ -3390,7 +3414,7 @@
         <v>16.574001242120175</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="19" t="s">
         <v>75</v>
       </c>
@@ -3398,7 +3422,7 @@
         <v>2122.2192108210402</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="19" t="s">
         <v>76</v>
       </c>
@@ -3406,7 +3430,7 @@
         <v>2123.5923451169101</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="19" t="s">
         <v>77</v>
       </c>
@@ -3446,7 +3470,7 @@
         <v>12.418599309430192</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="19" t="s">
         <v>114</v>
       </c>
@@ -3454,7 +3478,7 @@
         <v>2236.1095817401701</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="19" t="s">
         <v>115</v>
       </c>
@@ -3494,7 +3518,7 @@
         <v>0.92449238705012249</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="21" t="s">
         <v>65</v>
       </c>
@@ -3512,7 +3536,7 @@
       <c r="K49" s="21"/>
       <c r="L49" s="21"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="21" t="s">
         <v>116</v>
       </c>
@@ -3530,7 +3554,7 @@
       <c r="K50" s="21"/>
       <c r="L50" s="21"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="21" t="s">
         <v>117</v>
       </c>
@@ -3572,7 +3596,7 @@
         <v>0.62477194547000181</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="21" t="s">
         <v>78</v>
       </c>
@@ -3590,7 +3614,7 @@
       <c r="K52" s="21"/>
       <c r="L52" s="21"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="21" t="s">
         <v>79</v>
       </c>
@@ -3608,7 +3632,7 @@
       <c r="K53" s="21"/>
       <c r="L53" s="21"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="21" t="s">
         <v>80</v>
       </c>
@@ -3650,7 +3674,7 @@
         <v>3.6758375283698115</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="21" t="s">
         <v>81</v>
       </c>
@@ -3668,7 +3692,7 @@
       <c r="K55" s="21"/>
       <c r="L55" s="21"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="21" t="s">
         <v>82</v>
       </c>
@@ -3686,7 +3710,7 @@
       <c r="K56" s="21"/>
       <c r="L56" s="21"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="21" t="s">
         <v>83</v>
       </c>
@@ -3728,7 +3752,7 @@
         <v>4.6240391373403327</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="21" t="s">
         <v>84</v>
       </c>
@@ -3746,7 +3770,7 @@
       <c r="K58" s="21"/>
       <c r="L58" s="21"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="21" t="s">
         <v>85</v>
       </c>
@@ -3764,7 +3788,7 @@
       <c r="K59" s="21"/>
       <c r="L59" s="21"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="21" t="s">
         <v>86</v>
       </c>
@@ -3806,7 +3830,7 @@
         <v>0.46416779767014305</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="21" t="s">
         <v>118</v>
       </c>
@@ -3824,7 +3848,7 @@
       <c r="K61" s="21"/>
       <c r="L61" s="21"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="21" t="s">
         <v>119</v>
       </c>
@@ -3866,7 +3890,7 @@
         <v>0.88344358794984146</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="19" t="s">
         <v>65</v>
       </c>
@@ -3874,7 +3898,7 @@
         <v>1592.1393647914399</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="19" t="s">
         <v>120</v>
       </c>
@@ -3882,7 +3906,7 @@
         <v>2247.3720067191798</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="19" t="s">
         <v>121</v>
       </c>
@@ -3922,7 +3946,7 @@
         <v>2.4952530231798846</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="19" t="s">
         <v>87</v>
       </c>
@@ -3930,7 +3954,7 @@
         <v>2234.7435887859501</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="19" t="s">
         <v>88</v>
       </c>
@@ -3938,7 +3962,7 @@
         <v>2227.2541142131499</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="19" t="s">
         <v>89</v>
       </c>
@@ -3978,7 +4002,7 @@
         <v>10.515290785639991</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="19" t="s">
         <v>90</v>
       </c>
@@ -3986,7 +4010,7 @@
         <v>2233.5328075264601</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="19" t="s">
         <v>91</v>
       </c>
@@ -3994,7 +4018,7 @@
         <v>2235.2718356786399</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="19" t="s">
         <v>92</v>
       </c>
@@ -4034,7 +4058,7 @@
         <v>5.2933858786800556</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="19" t="s">
         <v>93</v>
       </c>
@@ -4042,7 +4066,7 @@
         <v>2231.41222642809</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="19" t="s">
         <v>94</v>
       </c>
@@ -4050,7 +4074,7 @@
         <v>2218.87534925306</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="19" t="s">
         <v>95</v>
       </c>
@@ -4090,7 +4114,7 @@
         <v>12.536877175029986</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="19" t="s">
         <v>122</v>
       </c>
@@ -4098,7 +4122,7 @@
         <v>2241.6593895374199</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="19" t="s">
         <v>123</v>
       </c>
@@ -4138,7 +4162,7 @@
         <v>2.5427539370703016</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="21" t="s">
         <v>65</v>
       </c>
@@ -4156,7 +4180,7 @@
       <c r="K77" s="21"/>
       <c r="L77" s="21"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="21" t="s">
         <v>124</v>
       </c>
@@ -4174,7 +4198,7 @@
       <c r="K78" s="21"/>
       <c r="L78" s="21"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="21" t="s">
         <v>125</v>
       </c>
@@ -4216,7 +4240,7 @@
         <v>19.982069738440259</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="34" t="s">
         <v>128</v>
       </c>
@@ -4236,7 +4260,7 @@
       <c r="K80" s="34"/>
       <c r="L80" s="34"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="34" t="s">
         <v>130</v>
       </c>
@@ -4256,7 +4280,7 @@
       <c r="K81" s="34"/>
       <c r="L81" s="34"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="34" t="s">
         <v>131</v>
       </c>
@@ -4300,7 +4324,7 @@
         <v>9.7230443598400598</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="21" t="s">
         <v>126</v>
       </c>
@@ -4318,7 +4342,7 @@
       <c r="K83" s="21"/>
       <c r="L83" s="21"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="21" t="s">
         <v>127</v>
       </c>
@@ -4360,7 +4384,7 @@
         <v>3.114767579850195</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="19" t="s">
         <v>65</v>
       </c>
@@ -4368,7 +4392,7 @@
         <v>1767.4127862110699</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="30" t="s">
         <v>132</v>
       </c>
@@ -4378,7 +4402,7 @@
       <c r="C86" s="30"/>
       <c r="D86" s="31"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="19" t="s">
         <v>133</v>
       </c>
@@ -4418,7 +4442,7 @@
         <v>200.93180595105991</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="19" t="s">
         <v>136</v>
       </c>
@@ -4426,7 +4450,7 @@
         <v>2223.7491846081298</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" s="19" t="s">
         <v>137</v>
       </c>
@@ -4466,7 +4490,7 @@
         <v>4.2857932929500748</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="19" t="s">
         <v>96</v>
       </c>
@@ -4474,7 +4498,7 @@
         <v>2176.50294375658</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" s="19" t="s">
         <v>97</v>
       </c>
@@ -4482,7 +4506,7 @@
         <v>2186.08511792934</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" s="19" t="s">
         <v>98</v>
       </c>
@@ -4522,7 +4546,7 @@
         <v>35.996994867829926</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="19" t="s">
         <v>99</v>
       </c>
@@ -4530,7 +4554,7 @@
         <v>2103.7936989664699</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" s="19" t="s">
         <v>100</v>
       </c>
@@ -4538,7 +4562,7 @@
         <v>2076.5450829193901</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" s="19" t="s">
         <v>101</v>
       </c>
@@ -4578,7 +4602,7 @@
         <v>27.24861604707985</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" s="19" t="s">
         <v>134</v>
       </c>
@@ -4586,7 +4610,7 @@
         <v>2157.74591479522</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="19" t="s">
         <v>135</v>
       </c>
@@ -4626,7 +4650,7 @@
         <v>16.870894775150191</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" s="21" t="s">
         <v>65</v>
       </c>
@@ -4644,7 +4668,7 @@
       <c r="K98" s="21"/>
       <c r="L98" s="21"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" s="21" t="s">
         <v>139</v>
       </c>
@@ -4662,7 +4686,7 @@
       <c r="K99" s="21"/>
       <c r="L99" s="21"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" s="21" t="s">
         <v>140</v>
       </c>
@@ -4704,7 +4728,7 @@
         <v>7.5272198213497177</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" s="21" t="s">
         <v>138</v>
       </c>
@@ -4722,7 +4746,7 @@
       <c r="K101" s="21"/>
       <c r="L101" s="21"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" s="21" t="s">
         <v>102</v>
       </c>
@@ -4740,7 +4764,7 @@
       <c r="K102" s="21"/>
       <c r="L102" s="21"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" s="21" t="s">
         <v>103</v>
       </c>
@@ -4758,7 +4782,7 @@
       <c r="K103" s="21"/>
       <c r="L103" s="21"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" s="21" t="s">
         <v>104</v>
       </c>
@@ -4800,7 +4824,7 @@
         <v>7.1066143973698672</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="21" t="s">
         <v>105</v>
       </c>
@@ -4818,7 +4842,7 @@
       <c r="K105" s="21"/>
       <c r="L105" s="21"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" s="21" t="s">
         <v>106</v>
       </c>
@@ -4836,7 +4860,7 @@
       <c r="K106" s="21"/>
       <c r="L106" s="21"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" s="21" t="s">
         <v>107</v>
       </c>
@@ -4878,7 +4902,7 @@
         <v>12.227740629090022</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" s="21" t="s">
         <v>141</v>
       </c>
@@ -4896,7 +4920,7 @@
       <c r="K108" s="21"/>
       <c r="L108" s="21"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" s="21" t="s">
         <v>142</v>
       </c>
@@ -4938,7 +4962,7 @@
         <v>104.21104304512983</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" s="19" t="s">
         <v>65</v>
       </c>
@@ -4946,7 +4970,7 @@
         <v>1712.82598863931</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" s="19" t="s">
         <v>162</v>
       </c>
@@ -4954,7 +4978,7 @@
         <v>2156.3511491220902</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" s="19" t="s">
         <v>163</v>
       </c>
@@ -4962,7 +4986,7 @@
         <v>2167.2565757031798</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" s="19" t="s">
         <v>164</v>
       </c>
@@ -5002,7 +5026,7 @@
         <v>10.905426581089614</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" s="19" t="s">
         <v>153</v>
       </c>
@@ -5010,7 +5034,7 @@
         <v>2095.24484288339</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" s="19" t="s">
         <v>154</v>
       </c>
@@ -5018,7 +5042,7 @@
         <v>2100.3120996130501</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" s="19" t="s">
         <v>155</v>
       </c>
@@ -5058,7 +5082,7 @@
         <v>10.806316414660159</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" s="19" t="s">
         <v>156</v>
       </c>
@@ -5066,7 +5090,7 @@
         <v>2218.8993800551598</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" s="19" t="s">
         <v>157</v>
       </c>
@@ -5074,7 +5098,7 @@
         <v>2186.6045565018098</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" s="19" t="s">
         <v>158</v>
       </c>
@@ -5114,7 +5138,7 @@
         <v>32.294823553349943</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" s="19" t="s">
         <v>159</v>
       </c>
@@ -5122,7 +5146,7 @@
         <v>2186.45070089</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" s="19" t="s">
         <v>160</v>
       </c>
@@ -5130,7 +5154,7 @@
         <v>2194.8913127686101</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122" s="19" t="s">
         <v>161</v>
       </c>
@@ -5170,7 +5194,7 @@
         <v>8.4406118786100706</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123" s="19" t="s">
         <v>165</v>
       </c>
@@ -5178,7 +5202,7 @@
         <v>2173.0418402661999</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" s="19" t="s">
         <v>166</v>
       </c>
@@ -5186,7 +5210,7 @@
         <v>2182.96053312513</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" s="19" t="s">
         <v>167</v>
       </c>
@@ -5226,7 +5250,7 @@
         <v>9.9186928589301715</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126" s="19" t="s">
         <v>168</v>
       </c>
@@ -5234,7 +5258,7 @@
         <v>2232.7275708530301</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127" s="19" t="s">
         <v>169</v>
       </c>
@@ -5242,7 +5266,7 @@
         <v>2225.3939498013601</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" s="19" t="s">
         <v>170</v>
       </c>
@@ -5282,7 +5306,7 @@
         <v>8.6111939932702626</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129" s="21" t="s">
         <v>65</v>
       </c>
@@ -5300,7 +5324,7 @@
       <c r="K129" s="21"/>
       <c r="L129" s="21"/>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130" s="21" t="s">
         <v>171</v>
       </c>
@@ -5318,7 +5342,7 @@
       <c r="K130" s="21"/>
       <c r="L130" s="21"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131" s="21" t="s">
         <v>172</v>
       </c>
@@ -5336,7 +5360,7 @@
       <c r="K131" s="21"/>
       <c r="L131" s="21"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132" s="21" t="s">
         <v>173</v>
       </c>
@@ -5378,7 +5402,7 @@
         <v>6.1719923844798359</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A133" s="21" t="s">
         <v>174</v>
       </c>
@@ -5396,7 +5420,7 @@
       <c r="K133" s="21"/>
       <c r="L133" s="21"/>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134" s="21" t="s">
         <v>175</v>
       </c>
@@ -5414,7 +5438,7 @@
       <c r="K134" s="21"/>
       <c r="L134" s="21"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A135" s="21" t="s">
         <v>176</v>
       </c>
@@ -5456,7 +5480,7 @@
         <v>3.7418551294699682</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A136" s="21" t="s">
         <v>177</v>
       </c>
@@ -5474,7 +5498,7 @@
       <c r="K136" s="21"/>
       <c r="L136" s="21"/>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137" s="21" t="s">
         <v>178</v>
       </c>
@@ -5492,7 +5516,7 @@
       <c r="K137" s="21"/>
       <c r="L137" s="21"/>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138" s="21" t="s">
         <v>179</v>
       </c>
@@ -5534,7 +5558,7 @@
         <v>99.351645211729647</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A139" s="21" t="s">
         <v>180</v>
       </c>
@@ -5552,7 +5576,7 @@
       <c r="K139" s="21"/>
       <c r="L139" s="21"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A140" s="21" t="s">
         <v>181</v>
       </c>
@@ -5570,7 +5594,7 @@
       <c r="K140" s="21"/>
       <c r="L140" s="21"/>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A141" s="21" t="s">
         <v>182</v>
       </c>
@@ -5612,7 +5636,7 @@
         <v>7.6350153611201677</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A142" s="21" t="s">
         <v>183</v>
       </c>
@@ -5630,7 +5654,7 @@
       <c r="K142" s="21"/>
       <c r="L142" s="21"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143" s="21" t="s">
         <v>184</v>
       </c>
@@ -5648,7 +5672,7 @@
       <c r="K143" s="21"/>
       <c r="L143" s="21"/>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A144" s="21" t="s">
         <v>185</v>
       </c>
@@ -5690,7 +5714,7 @@
         <v>5.9110954046300321</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145" s="19" t="s">
         <v>65</v>
       </c>
@@ -5698,7 +5722,7 @@
         <v>1732.26717091612</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A146" s="19" t="s">
         <v>186</v>
       </c>
@@ -5706,7 +5730,7 @@
         <v>2171.6037363503101</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A147" s="19" t="s">
         <v>187</v>
       </c>
@@ -5714,7 +5738,7 @@
         <v>2168.3325368241499</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A148" s="19" t="s">
         <v>188</v>
       </c>
@@ -5754,7 +5778,7 @@
         <v>3.2711995261602169</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A149" s="19" t="s">
         <v>189</v>
       </c>
@@ -5762,7 +5786,7 @@
         <v>2205.29339655284</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A150" s="19" t="s">
         <v>190</v>
       </c>
@@ -5770,7 +5794,7 @@
         <v>2203.5715719336199</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A151" s="19" t="s">
         <v>191</v>
       </c>
@@ -5810,7 +5834,7 @@
         <v>1.721824619220115</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A152" s="19" t="s">
         <v>192</v>
       </c>
@@ -5818,7 +5842,7 @@
         <v>2209.2654099239599</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A153" s="19" t="s">
         <v>193</v>
       </c>
@@ -5826,7 +5850,7 @@
         <v>2205.6468945710899</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A154" s="19" t="s">
         <v>194</v>
       </c>
@@ -5866,7 +5890,7 @@
         <v>3.618515352869963</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A155" s="19" t="s">
         <v>195</v>
       </c>
@@ -5874,7 +5898,7 @@
         <v>2201.95312729751</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A156" s="19" t="s">
         <v>196</v>
       </c>
@@ -5882,7 +5906,7 @@
         <v>2201.7544015737499</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A157" s="19" t="s">
         <v>197</v>
       </c>
@@ -5922,7 +5946,7 @@
         <v>5.0274952043100711</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A158" s="19" t="s">
         <v>198</v>
       </c>
@@ -5930,7 +5954,7 @@
         <v>2172.39686499658</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A159" s="19" t="s">
         <v>199</v>
       </c>
@@ -5938,7 +5962,7 @@
         <v>2167.4396622854201</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A160" s="19" t="s">
         <v>200</v>
       </c>
@@ -5978,7 +6002,7 @@
         <v>4.95720271115988</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A161" s="19" t="s">
         <v>201</v>
       </c>
@@ -5986,7 +6010,7 @@
         <v>2234.9084845810298</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A162" s="19" t="s">
         <v>202</v>
       </c>
@@ -5994,7 +6018,7 @@
         <v>2233.8319039288199</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A163" s="19" t="s">
         <v>203</v>
       </c>
@@ -6034,7 +6058,7 @@
         <v>2.9707386936402145</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A164" s="19" t="s">
         <v>215</v>
       </c>
@@ -6042,7 +6066,7 @@
         <v>2791.47452987631</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A165" s="19" t="s">
         <v>207</v>
       </c>
@@ -6050,7 +6074,7 @@
         <v>2253.5400879193598</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A166" s="19" t="s">
         <v>208</v>
       </c>
@@ -6058,7 +6082,7 @@
         <v>2250.3490168078902</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A167" s="19" t="s">
         <v>209</v>
       </c>
@@ -6066,7 +6090,7 @@
         <v>2261.73917919109</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A168" s="19" t="s">
         <v>210</v>
       </c>
@@ -6074,7 +6098,7 @@
         <v>2241.4624109891101</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A169" s="19" t="s">
         <v>211</v>
       </c>
@@ -6082,7 +6106,7 @@
         <v>2258.1304930768201</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A170" s="19" t="s">
         <v>212</v>
       </c>
@@ -6090,7 +6114,7 @@
         <v>2251.4238491137899</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A171" s="19" t="s">
         <v>213</v>
       </c>
@@ -6130,7 +6154,7 @@
         <v>20.276768201979849</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A172" s="19" t="s">
         <v>214</v>
       </c>
@@ -6138,7 +6162,7 @@
         <v>2424.3536009301201</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A173" s="19" t="s">
         <v>204</v>
       </c>
@@ -6146,7 +6170,7 @@
         <v>2220.1114998255798</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A174" s="19" t="s">
         <v>205</v>
       </c>
@@ -6154,7 +6178,7 @@
         <v>2223.29862647973</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A175" s="19" t="s">
         <v>206</v>
       </c>
@@ -6194,7 +6218,7 @@
         <v>5.3446747965799659</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A176" s="19" t="s">
         <v>215</v>
       </c>
@@ -6202,7 +6226,7 @@
         <v>2053.3155707137898</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A177" s="19" t="s">
         <v>217</v>
       </c>
@@ -6210,7 +6234,7 @@
         <v>2121.1126006919999</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A178" s="19" t="s">
         <v>218</v>
       </c>
@@ -6218,7 +6242,7 @@
         <v>2114.3140912812701</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A179" s="19" t="s">
         <v>219</v>
       </c>
@@ -6258,7 +6282,7 @@
         <v>16.851486293259768</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A180" s="19" t="s">
         <v>220</v>
       </c>
@@ -6266,7 +6290,7 @@
         <v>2136.7025174391802</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A181" s="19" t="s">
         <v>221</v>
       </c>
@@ -6274,7 +6298,7 @@
         <v>2137.4028738178399</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A182" s="19" t="s">
         <v>222</v>
       </c>
@@ -6314,7 +6338,7 @@
         <v>1.0440521757400347</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A183" s="19" t="s">
         <v>223</v>
       </c>
@@ -6322,7 +6346,7 @@
         <v>2112.5960733162501</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A184" s="19" t="s">
         <v>224</v>
       </c>
@@ -6330,7 +6354,7 @@
         <v>2105.44065001114</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A185" s="19" t="s">
         <v>225</v>
       </c>
@@ -6370,7 +6394,7 @@
         <v>10.104269404670049</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A186" s="19" t="s">
         <v>214</v>
       </c>
@@ -6378,7 +6402,7 @@
         <v>1798.38269926629</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A187" s="19" t="s">
         <v>226</v>
       </c>
@@ -6386,7 +6410,7 @@
         <v>2167.3314732691902</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A188" s="19" t="s">
         <v>227</v>
       </c>
@@ -6394,7 +6418,7 @@
         <v>2162.0931306789098</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A189" s="19" t="s">
         <v>228</v>
       </c>
@@ -6434,7 +6458,7 @@
         <v>5.2383425902803538</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A190" s="19" t="s">
         <v>215</v>
       </c>
@@ -6442,7 +6466,7 @@
         <v>2290.3416417366602</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A191" s="19" t="s">
         <v>232</v>
       </c>
@@ -6450,7 +6474,7 @@
         <v>2185.6742415221702</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A192" s="19" t="s">
         <v>214</v>
       </c>
@@ -6458,7 +6482,7 @@
         <v>2450.9836064696501</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A193" s="19" t="s">
         <v>230</v>
       </c>
@@ -6466,7 +6490,7 @@
         <v>2203.76908601887</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A194" s="19" t="s">
         <v>231</v>
       </c>
@@ -6506,7 +6530,7 @@
         <v>135.39340726519004</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A195" s="19" t="s">
         <v>215</v>
       </c>
@@ -6517,7 +6541,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A196" s="19" t="s">
         <v>254</v>
       </c>
@@ -6528,7 +6552,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A197" s="30" t="s">
         <v>246</v>
       </c>
@@ -6548,7 +6572,7 @@
       <c r="K197" s="30"/>
       <c r="L197" s="30"/>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A198" s="30" t="s">
         <v>247</v>
       </c>
@@ -6568,7 +6592,7 @@
       <c r="K198" s="30"/>
       <c r="L198" s="30"/>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A199" s="30" t="s">
         <v>248</v>
       </c>
@@ -6612,7 +6636,7 @@
         <v>80.530173698789895</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A200" s="19" t="s">
         <v>249</v>
       </c>
@@ -6623,7 +6647,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A201" s="19" t="s">
         <v>250</v>
       </c>
@@ -6634,7 +6658,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A202" s="19" t="s">
         <v>251</v>
       </c>
@@ -6677,7 +6701,7 @@
         <v>22.106909910789909</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A203" s="19" t="s">
         <v>252</v>
       </c>
@@ -6688,7 +6712,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A204" s="19" t="s">
         <v>253</v>
       </c>
@@ -6731,7 +6755,7 @@
         <v>6.3773501485898123</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A205" s="19" t="s">
         <v>215</v>
       </c>
@@ -6739,7 +6763,7 @@
         <v>2380.6235945409098</v>
       </c>
     </row>
-    <row r="206" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A206" s="30" t="s">
         <v>234</v>
       </c>
@@ -6750,7 +6774,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A207" s="19" t="s">
         <v>235</v>
       </c>
@@ -6758,7 +6782,7 @@
         <v>2203.22618654695</v>
       </c>
     </row>
-    <row r="208" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A208" s="19" t="s">
         <v>236</v>
       </c>
@@ -6801,7 +6825,7 @@
         <v>2.9465776584497689</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A209" s="19" t="s">
         <v>214</v>
       </c>
@@ -6809,7 +6833,7 @@
         <v>2398.0314183502901</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A210" s="19" t="s">
         <v>237</v>
       </c>
@@ -6817,7 +6841,7 @@
         <v>2188.0548117417202</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A211" s="19" t="s">
         <v>238</v>
       </c>
@@ -6825,7 +6849,7 @@
         <v>2182.1633268279402</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A212" s="19" t="s">
         <v>239</v>
       </c>
@@ -6865,7 +6889,7 @@
         <v>8.1509765235000486</v>
       </c>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A213" s="19" t="s">
         <v>233</v>
       </c>
@@ -6873,7 +6897,7 @@
         <v>2110.5869142463098</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A214" s="19" t="s">
         <v>240</v>
       </c>
@@ -6884,7 +6908,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A215" s="19" t="s">
         <v>241</v>
       </c>
@@ -6895,7 +6919,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A216" s="19" t="s">
         <v>242</v>
       </c>
@@ -6938,7 +6962,7 @@
         <v>3.904750337889709</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A217" s="19" t="s">
         <v>215</v>
       </c>
@@ -6949,7 +6973,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A218" s="19" t="s">
         <v>264</v>
       </c>
@@ -6960,7 +6984,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A219" s="19" t="s">
         <v>265</v>
       </c>
@@ -7003,7 +7027,7 @@
         <v>8.68463262503019</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A220" s="19" t="s">
         <v>214</v>
       </c>
@@ -7014,7 +7038,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A221" s="19" t="s">
         <v>256</v>
       </c>
@@ -7025,7 +7049,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A222" s="19" t="s">
         <v>257</v>
       </c>
@@ -7068,7 +7092,7 @@
         <v>5.8165934254902822</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A223" s="30" t="s">
         <v>258</v>
       </c>
@@ -7088,7 +7112,7 @@
       <c r="K223" s="30"/>
       <c r="L223" s="30"/>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A224" s="30" t="s">
         <v>259</v>
       </c>
@@ -7132,7 +7156,7 @@
         <v>32.954345410279984</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A225" s="19" t="s">
         <v>260</v>
       </c>
@@ -7143,7 +7167,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A226" s="19" t="s">
         <v>261</v>
       </c>
@@ -7186,7 +7210,7 @@
         <v>5.2026737861701804</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A227" s="19" t="s">
         <v>262</v>
       </c>
@@ -7197,7 +7221,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A228" s="19" t="s">
         <v>263</v>
       </c>
@@ -7240,7 +7264,7 @@
         <v>4.3245947201799027</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A229" s="19" t="s">
         <v>215</v>
       </c>
@@ -7251,7 +7275,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A230" s="19" t="s">
         <v>266</v>
       </c>
@@ -7262,7 +7286,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A231" s="19" t="s">
         <v>267</v>
       </c>
@@ -7305,7 +7329,7 @@
         <v>29.590618718740188</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A232" s="19" t="s">
         <v>214</v>
       </c>
@@ -7316,7 +7340,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A233" s="30" t="s">
         <v>268</v>
       </c>
@@ -7336,7 +7360,7 @@
       <c r="K233" s="30"/>
       <c r="L233" s="30"/>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A234" s="30" t="s">
         <v>269</v>
       </c>
@@ -7380,7 +7404,7 @@
         <v>98.563241012080198</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A235" s="30" t="s">
         <v>270</v>
       </c>
@@ -7400,7 +7424,7 @@
       <c r="K235" s="30"/>
       <c r="L235" s="30"/>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A236" s="30" t="s">
         <v>271</v>
       </c>
@@ -7444,7 +7468,7 @@
         <v>50.702122795780269</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A237" s="19" t="s">
         <v>272</v>
       </c>
@@ -7455,7 +7479,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A238" s="19" t="s">
         <v>273</v>
       </c>
@@ -7498,7 +7522,7 @@
         <v>2.8650123670299763</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A239" s="19" t="s">
         <v>274</v>
       </c>
@@ -7509,7 +7533,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A240" s="19" t="s">
         <v>275</v>
       </c>
@@ -7552,7 +7576,7 @@
         <v>0.59521187339987591</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A241" s="19" t="s">
         <v>215</v>
       </c>
@@ -7563,7 +7587,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A242" s="19" t="s">
         <v>284</v>
       </c>
@@ -7574,7 +7598,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A243" s="19" t="s">
         <v>285</v>
       </c>
@@ -7617,7 +7641,7 @@
         <v>27.431380469030046</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A244" s="19" t="s">
         <v>214</v>
       </c>
@@ -7628,7 +7652,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A245" s="30" t="s">
         <v>276</v>
       </c>
@@ -7648,7 +7672,7 @@
       <c r="K245" s="30"/>
       <c r="L245" s="30"/>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A246" s="30" t="s">
         <v>277</v>
       </c>
@@ -7692,7 +7716,7 @@
         <v>106.57926523131982</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A247" s="19" t="s">
         <v>278</v>
       </c>
@@ -7703,7 +7727,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A248" s="19" t="s">
         <v>279</v>
       </c>
@@ -7746,7 +7770,7 @@
         <v>4.315005150160232</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A249" s="19" t="s">
         <v>233</v>
       </c>
@@ -7757,7 +7781,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A250" s="19" t="s">
         <v>280</v>
       </c>
@@ -7768,7 +7792,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A251" s="19" t="s">
         <v>281</v>
       </c>
@@ -7811,7 +7835,7 @@
         <v>1.1060046663201319</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A252" s="19" t="s">
         <v>282</v>
       </c>
@@ -7822,7 +7846,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A253" s="19" t="s">
         <v>283</v>
       </c>
@@ -7865,7 +7889,7 @@
         <v>3.6802308610099317</v>
       </c>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A254" s="19" t="s">
         <v>215</v>
       </c>
@@ -7876,7 +7900,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A255" s="19" t="s">
         <v>295</v>
       </c>
@@ -7887,7 +7911,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A256" s="19" t="s">
         <v>296</v>
       </c>
@@ -7930,7 +7954,7 @@
         <v>23.453379467379818</v>
       </c>
     </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A257" s="19" t="s">
         <v>214</v>
       </c>
@@ -7941,7 +7965,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A258" s="30" t="s">
         <v>287</v>
       </c>
@@ -7961,7 +7985,7 @@
       <c r="K258" s="30"/>
       <c r="L258" s="30"/>
     </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A259" s="30" t="s">
         <v>288</v>
       </c>
@@ -8005,7 +8029,7 @@
         <v>78.194172333389815</v>
       </c>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A260" s="19" t="s">
         <v>289</v>
       </c>
@@ -8016,7 +8040,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A261" s="19" t="s">
         <v>290</v>
       </c>
@@ -8059,7 +8083,7 @@
         <v>3.0852149566799199</v>
       </c>
     </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A262" s="19" t="s">
         <v>291</v>
       </c>
@@ -8070,7 +8094,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A263" s="19" t="s">
         <v>292</v>
       </c>
@@ -8113,7 +8137,7 @@
         <v>0.92672882845999993</v>
       </c>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A264" s="19" t="s">
         <v>233</v>
       </c>
@@ -8124,7 +8148,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A265" s="19" t="s">
         <v>293</v>
       </c>
@@ -8135,7 +8159,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A266" s="19" t="s">
         <v>294</v>
       </c>
@@ -8176,6 +8200,363 @@
       <c r="L266" s="21">
         <f>K266-J266</f>
         <v>3.3655476130197712</v>
+      </c>
+    </row>
+    <row r="267" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A267" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="B267" s="19">
+        <v>1282.0911771297899</v>
+      </c>
+    </row>
+    <row r="268" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A268" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="B268" s="19">
+        <v>2260.8897208861899</v>
+      </c>
+    </row>
+    <row r="269" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A269" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="B269" s="19">
+        <v>2231.0035244408</v>
+      </c>
+    </row>
+    <row r="270" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A270" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="B270" s="19">
+        <v>1253.12244399984</v>
+      </c>
+    </row>
+    <row r="271" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A271" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="B271" s="19">
+        <v>2326.79680136756</v>
+      </c>
+      <c r="D271" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="272" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A272" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="B272" s="19">
+        <v>2329.0032371468801</v>
+      </c>
+      <c r="D272" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="273" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A273" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="B273" s="19">
+        <v>2269.2716409028999</v>
+      </c>
+      <c r="D273" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E273" s="19">
+        <f>AVERAGE(B271:B273)</f>
+        <v>2308.3572264724467</v>
+      </c>
+      <c r="F273" s="19">
+        <f>_xlfn.STDEV.S(B271:B273)</f>
+        <v>33.867083417351395</v>
+      </c>
+      <c r="G273" s="19">
+        <f>2*F273</f>
+        <v>67.734166834702791</v>
+      </c>
+      <c r="H273" s="19">
+        <f>F273/E273</f>
+        <v>1.4671508824093888E-2</v>
+      </c>
+      <c r="I273" s="41">
+        <f>H273</f>
+        <v>1.4671508824093888E-2</v>
+      </c>
+      <c r="J273" s="19">
+        <f>MIN(B271:B273)</f>
+        <v>2269.2716409028999</v>
+      </c>
+      <c r="K273" s="19">
+        <f>MAX(B271:B273)</f>
+        <v>2329.0032371468801</v>
+      </c>
+      <c r="L273" s="19">
+        <f>K273-J273</f>
+        <v>59.731596243980221</v>
+      </c>
+    </row>
+    <row r="274" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A274" s="19" t="s">
+        <v>287</v>
+      </c>
+      <c r="B274" s="19">
+        <v>2299.5908509404499</v>
+      </c>
+      <c r="D274" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="275" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A275" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="B275" s="19">
+        <v>2300.80332507719</v>
+      </c>
+      <c r="D275" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="276" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A276" s="19" t="s">
+        <v>300</v>
+      </c>
+      <c r="B276" s="19">
+        <v>2299.0965355468402</v>
+      </c>
+      <c r="D276" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E276" s="19">
+        <f>AVERAGE(B274:B276)</f>
+        <v>2299.83023718816</v>
+      </c>
+      <c r="F276" s="19">
+        <f>_xlfn.STDEV.S(B274:B276)</f>
+        <v>0.87821521105167244</v>
+      </c>
+      <c r="G276" s="19">
+        <f>2*F276</f>
+        <v>1.7564304221033449</v>
+      </c>
+      <c r="H276" s="19">
+        <f>F276/E276</f>
+        <v>3.8186088557797383E-4</v>
+      </c>
+      <c r="I276" s="41">
+        <f>H276</f>
+        <v>3.8186088557797383E-4</v>
+      </c>
+      <c r="J276" s="19">
+        <f>MIN(B274:B276)</f>
+        <v>2299.0965355468402</v>
+      </c>
+      <c r="K276" s="19">
+        <f>MAX(B274:B276)</f>
+        <v>2300.80332507719</v>
+      </c>
+      <c r="L276" s="19">
+        <f>K276-J276</f>
+        <v>1.7067895303498517</v>
+      </c>
+    </row>
+    <row r="277" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A277" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="B277" s="19">
+        <v>2282.5460830258598</v>
+      </c>
+      <c r="D277" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="278" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A278" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="B278" s="19">
+        <v>2281.12861430166</v>
+      </c>
+      <c r="D278" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="279" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A279" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="B279" s="19">
+        <v>2284.77788569108</v>
+      </c>
+      <c r="D279" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E279" s="19">
+        <f>AVERAGE(B277:B279)</f>
+        <v>2282.8175276728666</v>
+      </c>
+      <c r="F279" s="19">
+        <f>_xlfn.STDEV.S(B277:B279)</f>
+        <v>1.8397165721113684</v>
+      </c>
+      <c r="G279" s="19">
+        <f>2*F279</f>
+        <v>3.6794331442227368</v>
+      </c>
+      <c r="H279" s="19">
+        <f>F279/E279</f>
+        <v>8.0589733949817661E-4</v>
+      </c>
+      <c r="I279" s="41">
+        <f>H279</f>
+        <v>8.0589733949817661E-4</v>
+      </c>
+      <c r="J279" s="19">
+        <f>MIN(B277:B279)</f>
+        <v>2281.12861430166</v>
+      </c>
+      <c r="K279" s="19">
+        <f>MAX(B277:B279)</f>
+        <v>2284.77788569108</v>
+      </c>
+      <c r="L279" s="19">
+        <f>K279-J279</f>
+        <v>3.6492713894199369</v>
+      </c>
+    </row>
+    <row r="280" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A280" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="B280" s="19">
+        <v>2294.3269056540098</v>
+      </c>
+      <c r="D280" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="281" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A281" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="B281" s="19">
+        <v>2300.3023019523998</v>
+      </c>
+      <c r="D281" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="282" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A282" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="B282" s="19">
+        <v>2292.3116146153802</v>
+      </c>
+      <c r="D282" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E282" s="19">
+        <f>AVERAGE(B280:B282)</f>
+        <v>2295.6469407405966</v>
+      </c>
+      <c r="F282" s="19">
+        <f>_xlfn.STDEV.S(B280:B282)</f>
+        <v>4.1556756973886415</v>
+      </c>
+      <c r="G282" s="19">
+        <f>2*F282</f>
+        <v>8.311351394777283</v>
+      </c>
+      <c r="H282" s="19">
+        <f>F282/E282</f>
+        <v>1.8102416463256247E-3</v>
+      </c>
+      <c r="I282" s="41">
+        <f>H282</f>
+        <v>1.8102416463256247E-3</v>
+      </c>
+      <c r="J282" s="19">
+        <f>MIN(B280:B282)</f>
+        <v>2292.3116146153802</v>
+      </c>
+      <c r="K282" s="19">
+        <f>MAX(B280:B282)</f>
+        <v>2300.3023019523998</v>
+      </c>
+      <c r="L282" s="19">
+        <f>K282-J282</f>
+        <v>7.9906873370196081</v>
+      </c>
+    </row>
+    <row r="283" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A283" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="B283" s="19">
+        <v>2321.2838337913399</v>
+      </c>
+      <c r="D283" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="284" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A284" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="B284" s="19">
+        <v>2320.25500233517</v>
+      </c>
+      <c r="D284" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="285" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A285" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="B285" s="19">
+        <v>2312.12020282716</v>
+      </c>
+      <c r="D285" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="E285" s="19">
+        <f>AVERAGE(B283:B285)</f>
+        <v>2317.88634631789</v>
+      </c>
+      <c r="F285" s="19">
+        <f>_xlfn.STDEV.S(B283:B285)</f>
+        <v>5.0200529487314069</v>
+      </c>
+      <c r="G285" s="19">
+        <f>2*F285</f>
+        <v>10.040105897462814</v>
+      </c>
+      <c r="H285" s="19">
+        <f>F285/E285</f>
+        <v>2.1657890848298411E-3</v>
+      </c>
+      <c r="I285" s="41">
+        <f>H285</f>
+        <v>2.1657890848298411E-3</v>
+      </c>
+      <c r="J285" s="19">
+        <f>MIN(B283:B285)</f>
+        <v>2312.12020282716</v>
+      </c>
+      <c r="K285" s="19">
+        <f>MAX(B283:B285)</f>
+        <v>2321.2838337913399</v>
+      </c>
+      <c r="L285" s="19">
+        <f>K285-J285</f>
+        <v>9.1636309641799016</v>
       </c>
     </row>
   </sheetData>
@@ -8192,25 +8573,25 @@
       <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="103" style="6" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" style="11" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="12" customWidth="1"/>
-    <col min="14" max="14" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" style="11" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="12" customWidth="1"/>
+    <col min="14" max="14" width="59.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -8241,7 +8622,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>40</v>
       </c>
@@ -8272,7 +8653,7 @@
         <v>33.311999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>41</v>
       </c>
@@ -8308,7 +8689,7 @@
         <v>33.661000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>42</v>
       </c>
@@ -8343,7 +8724,7 @@
         <v>33.524999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>43</v>
       </c>
@@ -8382,7 +8763,7 @@
         <v>27.53</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>44</v>
       </c>
@@ -8411,7 +8792,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -8431,7 +8812,7 @@
         <v>4.9540482249982379E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -8451,7 +8832,7 @@
         <v>1616.5688340569229</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -8471,7 +8852,7 @@
         <v>2043.1552616256156</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>108</v>
       </c>
@@ -8491,7 +8872,7 @@
         <v>1194.6338725265152</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>110</v>
       </c>
@@ -8511,7 +8892,7 @@
         <v>460.54747632980491</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>111</v>
       </c>
@@ -8531,7 +8912,7 @@
         <v>922.68201761768364</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>112</v>
       </c>
@@ -8551,7 +8932,7 @@
         <v>881.29115046163486</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>113</v>
       </c>
@@ -8571,7 +8952,7 @@
         <v>872.73469821815206</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>114</v>
       </c>
@@ -8591,7 +8972,7 @@
         <v>581.27193168594556</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>115</v>
       </c>
@@ -8611,7 +8992,7 @@
         <v>537.54836831215925</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>116</v>
       </c>
@@ -8631,7 +9012,7 @@
         <v>1296.1908027475388</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>117</v>
       </c>
@@ -8651,7 +9032,7 @@
         <v>1251.5942514404196</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>118</v>
       </c>
@@ -8677,7 +9058,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>119</v>
       </c>
@@ -8703,7 +9084,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>120</v>
       </c>
@@ -8723,7 +9104,7 @@
         <v>1251.1788593417016</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>121</v>
       </c>
@@ -8743,7 +9124,7 @@
         <v>1080.8809335874446</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>122</v>
       </c>
@@ -8763,7 +9144,7 @@
         <v>879.67938773241201</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>123</v>
       </c>
@@ -8783,7 +9164,7 @@
         <v>1036.9780443516509</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>124</v>
       </c>
@@ -8803,7 +9184,7 @@
         <v>1778.9155994712464</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>125</v>
       </c>
@@ -8823,7 +9204,7 @@
         <v>492.6234913924153</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>126</v>
       </c>
@@ -8843,7 +9224,7 @@
         <v>24.072827949184788</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>127</v>
       </c>
@@ -8863,7 +9244,7 @@
         <v>64.339238860453506</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>133</v>
       </c>
@@ -8883,7 +9264,7 @@
         <v>207.8719331919755</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>136</v>
       </c>
@@ -8903,7 +9284,7 @@
         <v>138.04333895591375</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>137</v>
       </c>
@@ -8924,7 +9305,7 @@
       </c>
       <c r="F31" s="7"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>134</v>
       </c>
@@ -8944,7 +9325,7 @@
         <v>184.24908079822336</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>135</v>
       </c>
@@ -8964,7 +9345,7 @@
         <v>926.88175991374135</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>139</v>
       </c>
@@ -8984,7 +9365,7 @@
         <v>486.91166620058681</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
         <v>140</v>
       </c>
@@ -9004,7 +9385,7 @@
         <v>875.76309877890378</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
         <v>138</v>
       </c>
@@ -9024,7 +9405,7 @@
         <v>303.23018266722977</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
         <v>141</v>
       </c>
@@ -9044,7 +9425,7 @@
         <v>2294.9404868978409</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>162</v>
       </c>
@@ -9064,7 +9445,7 @@
         <v>148.32980520874986</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>163</v>
       </c>
@@ -9084,7 +9465,7 @@
         <v>532.89409450498101</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>164</v>
       </c>
@@ -9104,7 +9485,7 @@
         <v>283.20100953040998</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>165</v>
       </c>
@@ -9124,7 +9505,7 @@
         <v>833.46324871491561</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>166</v>
       </c>
@@ -9144,7 +9525,7 @@
         <v>1504.5443523099382</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>167</v>
       </c>
@@ -9164,7 +9545,7 @@
         <v>1359.7250044629604</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>168</v>
       </c>
@@ -9184,7 +9565,7 @@
         <v>429.63219346738299</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>169</v>
       </c>
@@ -9204,7 +9585,7 @@
         <v>179.39789128135487</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>170</v>
       </c>
@@ -9224,7 +9605,7 @@
         <v>146.80658820772371</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>171</v>
       </c>
@@ -9244,7 +9625,7 @@
         <v>804.34807109832093</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
         <v>172</v>
       </c>
@@ -9264,7 +9645,7 @@
         <v>625.20915402841661</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
         <v>173</v>
       </c>
@@ -9284,7 +9665,7 @@
         <v>492.3534281993272</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
         <v>180</v>
       </c>
@@ -9304,7 +9685,7 @@
         <v>695.82572169514754</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
         <v>181</v>
       </c>
@@ -9324,7 +9705,7 @@
         <v>611.69319324915011</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
         <v>182</v>
       </c>
@@ -9344,7 +9725,7 @@
         <v>351.31854287090141</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="s">
         <v>183</v>
       </c>
@@ -9364,7 +9745,7 @@
         <v>380.30484808213612</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
         <v>184</v>
       </c>
@@ -9384,7 +9765,7 @@
         <v>636.11390476472218</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -9404,7 +9785,7 @@
         <v>372.88394874373085</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>186</v>
       </c>
@@ -9424,7 +9805,7 @@
         <v>752.49595149981849</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>187</v>
       </c>
@@ -9444,7 +9825,7 @@
         <v>583.72783370072705</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>188</v>
       </c>
@@ -9464,7 +9845,7 @@
         <v>650.68824789365851</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>198</v>
       </c>
@@ -9484,7 +9865,7 @@
         <v>796.63867472564982</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>199</v>
       </c>
@@ -9504,7 +9885,7 @@
         <v>541.38053925422037</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>200</v>
       </c>
@@ -9524,7 +9905,7 @@
         <v>764.16382344027829</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>201</v>
       </c>
@@ -9544,7 +9925,7 @@
         <v>524.79866579928125</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>202</v>
       </c>
@@ -9564,7 +9945,7 @@
         <v>476.6320291572211</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>203</v>
       </c>
@@ -9584,7 +9965,7 @@
         <v>615.17108105747434</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>204</v>
       </c>
@@ -9604,7 +9985,7 @@
         <v>65.79642942038133</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>205</v>
       </c>
@@ -9624,7 +10005,7 @@
         <v>127.65896032845698</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>206</v>
       </c>
@@ -9644,7 +10025,7 @@
         <v>35.44954064528568</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>226</v>
       </c>
@@ -9664,7 +10045,7 @@
         <v>536.35764972708762</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>227</v>
       </c>
@@ -9684,7 +10065,7 @@
         <v>321.16417593017383</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>228</v>
       </c>
@@ -9723,26 +10104,26 @@
       <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" customWidth="1"/>
     <col min="11" max="11" width="103" style="6" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" style="11" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" style="12" customWidth="1"/>
-    <col min="15" max="15" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" style="11" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" style="12" customWidth="1"/>
+    <col min="15" max="15" width="59.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
@@ -9773,7 +10154,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>56</v>
       </c>
@@ -9811,7 +10192,7 @@
         <v>33.311999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>40</v>
       </c>
@@ -9846,7 +10227,7 @@
         <v>33.661000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>41</v>
       </c>
@@ -9885,7 +10266,7 @@
         <v>33.524999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
         <v>42</v>
       </c>
@@ -9923,7 +10304,7 @@
         <v>27.53</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
         <v>43</v>
       </c>
@@ -9943,7 +10324,7 @@
         <v>127.93487528889766</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>44</v>
       </c>
@@ -9966,7 +10347,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
@@ -9986,7 +10367,7 @@
         <v>1616.5688340569229</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
         <v>57</v>
       </c>
@@ -10013,7 +10394,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
         <v>108</v>
       </c>
@@ -10039,7 +10420,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
         <v>110</v>
       </c>
@@ -10069,7 +10450,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
         <v>111</v>
       </c>
@@ -10099,7 +10480,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>112</v>
       </c>
@@ -10119,7 +10500,7 @@
         <v>881.29115046163486</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>113</v>
       </c>
@@ -10139,7 +10520,7 @@
         <v>872.73469821815206</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>114</v>
       </c>
@@ -10162,7 +10543,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>115</v>
       </c>
@@ -10182,7 +10563,7 @@
         <v>537.54836831215925</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="23" t="s">
         <v>116</v>
       </c>
@@ -10209,7 +10590,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="23" t="s">
         <v>117</v>
       </c>
@@ -10235,7 +10616,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="23" t="s">
         <v>118</v>
       </c>
@@ -10271,7 +10652,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="23" t="s">
         <v>119</v>
       </c>
@@ -10307,7 +10688,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
         <v>120</v>
       </c>
@@ -10327,7 +10708,7 @@
         <v>1251.1788593417016</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
         <v>121</v>
       </c>
@@ -10350,7 +10731,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
         <v>122</v>
       </c>
@@ -10370,7 +10751,7 @@
         <v>879.67938773241201</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
         <v>123</v>
       </c>
@@ -10397,7 +10778,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="23" t="s">
         <v>124</v>
       </c>
@@ -10423,7 +10804,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
         <v>125</v>
       </c>
@@ -10453,7 +10834,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="21" t="s">
         <v>126</v>
       </c>
@@ -10483,7 +10864,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
         <v>127</v>
       </c>
@@ -10503,7 +10884,7 @@
         <v>64.339238860453506</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="19" t="s">
         <v>136</v>
       </c>
@@ -10523,7 +10904,7 @@
         <v>138.04333895591375</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="19" t="s">
         <v>137</v>
       </c>
@@ -10543,7 +10924,7 @@
         <v>257.12051628811935</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="21" t="s">
         <v>138</v>
       </c>
@@ -10564,7 +10945,7 @@
       </c>
       <c r="F31" s="7"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="19" t="s">
         <v>168</v>
       </c>
@@ -10590,7 +10971,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="19" t="s">
         <v>169</v>
       </c>
@@ -10610,7 +10991,7 @@
         <v>179.39789128135487</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
         <v>170</v>
       </c>
@@ -10637,7 +11018,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
         <v>183</v>
       </c>
@@ -10663,7 +11044,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="21" t="s">
         <v>184</v>
       </c>
@@ -10693,7 +11074,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="21" t="s">
         <v>185</v>
       </c>
@@ -10723,7 +11104,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="19" t="s">
         <v>201</v>
       </c>
@@ -10743,7 +11124,7 @@
         <v>524.79866579928125</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="19" t="s">
         <v>202</v>
       </c>
@@ -10763,7 +11144,7 @@
         <v>476.6320291572211</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="19" t="s">
         <v>203</v>
       </c>
@@ -10783,7 +11164,7 @@
         <v>615.17108105747434</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="39" t="s">
         <v>204</v>
       </c>
@@ -10803,7 +11184,7 @@
         <v>65.79642942038133</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="39" t="s">
         <v>205</v>
       </c>
@@ -10823,7 +11204,7 @@
         <v>127.65896032845698</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="39" t="s">
         <v>206</v>
       </c>
@@ -10858,25 +11239,25 @@
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="103" style="6" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" style="11" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="12" customWidth="1"/>
-    <col min="14" max="14" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" style="11" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="12" customWidth="1"/>
+    <col min="14" max="14" width="59.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -10904,7 +11285,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>133</v>
       </c>
@@ -10942,7 +11323,7 @@
         <v>33.311999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>134</v>
       </c>
@@ -10977,7 +11358,7 @@
         <v>33.661000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -11016,7 +11397,7 @@
         <v>33.524999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>139</v>
       </c>
@@ -11055,7 +11436,7 @@
         <v>27.53</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>140</v>
       </c>
@@ -11084,7 +11465,7 @@
         <v>30.34</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>141</v>
       </c>
@@ -11104,7 +11485,7 @@
         <v>2294.9404868978409</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>162</v>
       </c>
@@ -11124,7 +11505,7 @@
         <v>148.32980520874986</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>163</v>
       </c>
@@ -11144,7 +11525,7 @@
         <v>532.89409450498101</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>164</v>
       </c>
@@ -11164,7 +11545,7 @@
         <v>283.20100953040998</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>165</v>
       </c>
@@ -11184,7 +11565,7 @@
         <v>833.46324871491561</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>166</v>
       </c>
@@ -11204,7 +11585,7 @@
         <v>1504.5443523099382</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>167</v>
       </c>
@@ -11224,7 +11605,7 @@
         <v>1359.7250044629604</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>171</v>
       </c>
@@ -11244,7 +11625,7 @@
         <v>804.34807109832093</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>172</v>
       </c>
@@ -11264,7 +11645,7 @@
         <v>625.20915402841661</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>173</v>
       </c>
@@ -11284,7 +11665,7 @@
         <v>492.3534281993272</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>180</v>
       </c>
@@ -11304,7 +11685,7 @@
         <v>695.82572169514754</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>181</v>
       </c>
@@ -11324,7 +11705,7 @@
         <v>611.69319324915011</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>182</v>
       </c>
@@ -11350,7 +11731,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>186</v>
       </c>
@@ -11376,7 +11757,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>187</v>
       </c>
@@ -11396,7 +11777,7 @@
         <v>583.72783370072705</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>188</v>
       </c>
@@ -11416,7 +11797,7 @@
         <v>650.68824789365851</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>198</v>
       </c>
@@ -11436,7 +11817,7 @@
         <v>796.63867472564982</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>199</v>
       </c>
@@ -11462,7 +11843,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>200</v>
       </c>
@@ -11482,7 +11863,7 @@
         <v>764.16382344027829</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>226</v>
       </c>
@@ -11509,7 +11890,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>227</v>
       </c>
@@ -11535,7 +11916,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>228</v>
       </c>
@@ -11565,7 +11946,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>232</v>
       </c>
@@ -11595,7 +11976,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F31" s="7"/>
     </row>
   </sheetData>
@@ -11613,22 +11994,22 @@
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="37" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" style="11" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="12" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" style="11" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -11654,7 +12035,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>133</v>
       </c>
@@ -11690,7 +12071,7 @@
         <v>33.311999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>134</v>
       </c>
@@ -11725,7 +12106,7 @@
         <v>33.661000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -11764,7 +12145,7 @@
         <v>33.524999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>139</v>
       </c>
@@ -11804,7 +12185,7 @@
         <v>27.53</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>140</v>
       </c>
@@ -11824,7 +12205,7 @@
         <v>102.30344069771941</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>141</v>
       </c>
@@ -11844,7 +12225,7 @@
         <v>808.08060613910686</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>162</v>
       </c>
@@ -11864,7 +12245,7 @@
         <v>53.285708629655147</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>163</v>
       </c>
@@ -11884,7 +12265,7 @@
         <v>13.001220442986153</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>164</v>
       </c>
@@ -11904,7 +12285,7 @@
         <v>7.023567056548595</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>165</v>
       </c>
@@ -11924,7 +12305,7 @@
         <v>88.190600763448444</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>166</v>
       </c>
@@ -11944,7 +12325,7 @@
         <v>372.86366208601373</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>167</v>
       </c>
@@ -11964,7 +12345,7 @@
         <v>302.60935966796575</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>171</v>
       </c>
@@ -11984,7 +12365,7 @@
         <v>78.894407008806681</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>172</v>
       </c>
@@ -12004,7 +12385,7 @@
         <v>30.530091992903429</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>173</v>
       </c>
@@ -12024,7 +12405,7 @@
         <v>7.3455091416442153</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>180</v>
       </c>
@@ -12044,7 +12425,7 @@
         <v>47.606277053628439</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>181</v>
       </c>
@@ -12064,7 +12445,7 @@
         <v>27.600875305300281</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>182</v>
       </c>
@@ -12084,7 +12465,7 @@
         <v>0.54064424462958727</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>186</v>
       </c>
@@ -12104,7 +12485,7 @@
         <v>63.248318802554536</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>187</v>
       </c>
@@ -12124,7 +12505,7 @@
         <v>21.918142954464969</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>188</v>
       </c>
@@ -12144,7 +12525,7 @@
         <v>36.358646694738432</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>198</v>
       </c>
@@ -12164,7 +12545,7 @@
         <v>76.492687594572502</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>199</v>
       </c>
@@ -12190,7 +12571,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>200</v>
       </c>
@@ -12210,7 +12591,7 @@
         <v>66.662893254589605</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>226</v>
       </c>
@@ -12237,7 +12618,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>227</v>
       </c>
@@ -12263,7 +12644,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>228</v>
       </c>
@@ -12293,7 +12674,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G29">
         <f>G28/L5</f>
         <v>1.0996962711927174E-3</v>

</xml_diff>